<commit_message>
reorganized the code in functions and cleaned the main file for future development. Before trying to automize email sent, if it breaks later, return to this commit.
</commit_message>
<xml_diff>
--- a/stocksPercentage.xlsx
+++ b/stocksPercentage.xlsx
@@ -497,31 +497,31 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.52</v>
+        <v>0.7</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.34</v>
+        <v>0.38</v>
       </c>
       <c r="D2" t="n">
-        <v>2.2</v>
+        <v>2.07</v>
       </c>
       <c r="E2" t="n">
-        <v>-7.84</v>
+        <v>-6.71</v>
       </c>
       <c r="F2" t="n">
-        <v>-2.35</v>
+        <v>-1.99</v>
       </c>
       <c r="G2" t="n">
-        <v>1.6</v>
+        <v>1.66</v>
       </c>
       <c r="H2" t="n">
-        <v>7.31</v>
+        <v>8.5</v>
       </c>
       <c r="I2" t="n">
-        <v>9.039999999999999</v>
+        <v>9.82</v>
       </c>
       <c r="J2" t="n">
-        <v>26.82</v>
+        <v>28.14</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
@@ -536,31 +536,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
         <v>0.5</v>
       </c>
       <c r="D3" t="n">
-        <v>-1.47</v>
+        <v>-0.71</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.82</v>
+        <v>-1.41</v>
       </c>
       <c r="F3" t="n">
-        <v>-4.37</v>
+        <v>-4.12</v>
       </c>
       <c r="G3" t="n">
-        <v>-4.32</v>
+        <v>-3.66</v>
       </c>
       <c r="H3" t="n">
-        <v>-9.65</v>
+        <v>-9.970000000000001</v>
       </c>
       <c r="I3" t="n">
         <v>-13.97</v>
       </c>
       <c r="J3" t="n">
-        <v>-31.88</v>
+        <v>-32.06</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
@@ -578,28 +578,28 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>0.91</v>
       </c>
       <c r="D4" t="n">
-        <v>-1.83</v>
+        <v>-0.45</v>
       </c>
       <c r="E4" t="n">
-        <v>0.97</v>
+        <v>0.91</v>
       </c>
       <c r="F4" t="n">
-        <v>-1.01</v>
+        <v>0.28</v>
       </c>
       <c r="G4" t="n">
-        <v>0.45</v>
+        <v>1.19</v>
       </c>
       <c r="H4" t="n">
-        <v>1.09</v>
+        <v>1.83</v>
       </c>
       <c r="I4" t="n">
-        <v>-5.1</v>
+        <v>-4.46</v>
       </c>
       <c r="J4" t="n">
-        <v>-9.289999999999999</v>
+        <v>-8.199999999999999</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
@@ -614,31 +614,31 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>1.93</v>
+        <v>0.7</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.64</v>
+        <v>-0.71</v>
       </c>
       <c r="E5" t="n">
-        <v>-1.61</v>
+        <v>-2.13</v>
       </c>
       <c r="F5" t="n">
-        <v>-1.61</v>
+        <v>-1.07</v>
       </c>
       <c r="G5" t="n">
-        <v>-2.13</v>
+        <v>-0.37</v>
       </c>
       <c r="H5" t="n">
-        <v>3.44</v>
+        <v>2.84</v>
       </c>
       <c r="I5" t="n">
-        <v>33.16</v>
+        <v>32.78</v>
       </c>
       <c r="J5" t="n">
-        <v>23.73</v>
+        <v>21.98</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
@@ -653,31 +653,31 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9399999999999999</v>
+        <v>-1.23</v>
       </c>
       <c r="C6" t="n">
-        <v>1.72</v>
+        <v>-0.14</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.49</v>
+        <v>-1.39</v>
       </c>
       <c r="E6" t="n">
-        <v>3.66</v>
+        <v>2.14</v>
       </c>
       <c r="F6" t="n">
-        <v>5.41</v>
+        <v>4.71</v>
       </c>
       <c r="G6" t="n">
-        <v>4.71</v>
+        <v>5.71</v>
       </c>
       <c r="H6" t="n">
-        <v>13.08</v>
+        <v>11.38</v>
       </c>
       <c r="I6" t="n">
-        <v>52.79</v>
+        <v>51.05</v>
       </c>
       <c r="J6" t="n">
-        <v>58.41</v>
+        <v>55.01</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
@@ -692,31 +692,31 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>-2.92</v>
       </c>
       <c r="C7" t="n">
-        <v>1.25</v>
+        <v>-2.92</v>
       </c>
       <c r="D7" t="n">
-        <v>-3.03</v>
+        <v>-4.9</v>
       </c>
       <c r="E7" t="n">
-        <v>0.71</v>
+        <v>-1.34</v>
       </c>
       <c r="F7" t="n">
-        <v>-5.25</v>
+        <v>-5.33</v>
       </c>
       <c r="G7" t="n">
-        <v>-4.35</v>
+        <v>-4.54</v>
       </c>
       <c r="H7" t="n">
-        <v>0.86</v>
+        <v>-1.62</v>
       </c>
       <c r="I7" t="n">
-        <v>41.55</v>
+        <v>38</v>
       </c>
       <c r="J7" t="n">
-        <v>14.47</v>
+        <v>10.64</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
@@ -731,31 +731,31 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.43</v>
+        <v>-1.44</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.25</v>
+        <v>-3.18</v>
       </c>
       <c r="D8" t="n">
-        <v>-7.82</v>
+        <v>-8.130000000000001</v>
       </c>
       <c r="E8" t="n">
-        <v>-1.26</v>
+        <v>-2.44</v>
       </c>
       <c r="F8" t="n">
-        <v>-2.36</v>
+        <v>-2.61</v>
       </c>
       <c r="G8" t="n">
-        <v>-9.9</v>
+        <v>-12.23</v>
       </c>
       <c r="H8" t="n">
-        <v>-12.12</v>
+        <v>-13.8</v>
       </c>
       <c r="I8" t="n">
-        <v>7.35</v>
+        <v>6.12</v>
       </c>
       <c r="J8" t="n">
-        <v>-37.42</v>
+        <v>-38.5</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
@@ -770,31 +770,31 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-1.75</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>-4.06</v>
+        <v>-2.99</v>
       </c>
       <c r="D9" t="n">
-        <v>2.24</v>
+        <v>2.5</v>
       </c>
       <c r="E9" t="n">
-        <v>-12.1</v>
+        <v>-14.14</v>
       </c>
       <c r="F9" t="n">
-        <v>-12.1</v>
+        <v>-10.98</v>
       </c>
       <c r="G9" t="n">
-        <v>-7.8</v>
+        <v>-7.04</v>
       </c>
       <c r="H9" t="n">
-        <v>0.62</v>
+        <v>-0.67</v>
       </c>
       <c r="I9" t="n">
-        <v>40.44</v>
+        <v>40.07</v>
       </c>
       <c r="J9" t="n">
-        <v>-30.77</v>
+        <v>-30.81</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
@@ -809,31 +809,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-1.59</v>
+        <v>-1.15</v>
       </c>
       <c r="C10" t="n">
-        <v>-3.84</v>
+        <v>-4.51</v>
       </c>
       <c r="D10" t="n">
-        <v>2.52</v>
+        <v>1.57</v>
       </c>
       <c r="E10" t="n">
-        <v>-13.52</v>
+        <v>-16.45</v>
       </c>
       <c r="F10" t="n">
-        <v>-11.54</v>
+        <v>-11.16</v>
       </c>
       <c r="G10" t="n">
-        <v>-3.39</v>
+        <v>-4.05</v>
       </c>
       <c r="H10" t="n">
-        <v>-5.81</v>
+        <v>-7.41</v>
       </c>
       <c r="I10" t="n">
-        <v>40.35</v>
+        <v>38.16</v>
       </c>
       <c r="J10" t="n">
-        <v>-46.95</v>
+        <v>-47.45</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
@@ -848,31 +848,31 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-3.9</v>
+        <v>0.9</v>
       </c>
       <c r="C11" t="n">
-        <v>-6.33</v>
+        <v>-0.26</v>
       </c>
       <c r="D11" t="n">
-        <v>-6.98</v>
+        <v>-8.09</v>
       </c>
       <c r="E11" t="n">
-        <v>-35.13</v>
+        <v>-34.57</v>
       </c>
       <c r="F11" t="n">
-        <v>-31.85</v>
+        <v>-28.49</v>
       </c>
       <c r="G11" t="n">
-        <v>-44.51</v>
+        <v>-43.08</v>
       </c>
       <c r="H11" t="n">
-        <v>-72.42</v>
+        <v>-74.87</v>
       </c>
       <c r="I11" t="n">
-        <v>-80.69</v>
+        <v>-80.47</v>
       </c>
       <c r="J11" t="n">
-        <v>-95.12</v>
+        <v>-95.09</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
@@ -887,31 +887,31 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-1.4</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>-1.56</v>
+        <v>-1.58</v>
       </c>
       <c r="D12" t="n">
-        <v>-4.36</v>
+        <v>-2.84</v>
       </c>
       <c r="E12" t="n">
-        <v>-5.29</v>
+        <v>-5.41</v>
       </c>
       <c r="F12" t="n">
-        <v>-7.59</v>
+        <v>-6.13</v>
       </c>
       <c r="G12" t="n">
-        <v>-19.75</v>
+        <v>-18.71</v>
       </c>
       <c r="H12" t="n">
-        <v>-24.36</v>
+        <v>-24.37</v>
       </c>
       <c r="I12" t="n">
-        <v>7.31</v>
+        <v>7.11</v>
       </c>
       <c r="J12" t="n">
-        <v>10.08</v>
+        <v>10.92</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
@@ -926,31 +926,31 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0.83</v>
+        <v>-0.51</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.12</v>
+        <v>-1.3</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.62</v>
+        <v>-0.51</v>
       </c>
       <c r="E13" t="n">
-        <v>5.22</v>
+        <v>3.82</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.87</v>
+        <v>0.28</v>
       </c>
       <c r="G13" t="n">
-        <v>-5.7</v>
+        <v>-4</v>
       </c>
       <c r="H13" t="n">
-        <v>-11.28</v>
+        <v>-12.79</v>
       </c>
       <c r="I13" t="n">
-        <v>38.51</v>
+        <v>37.57</v>
       </c>
       <c r="J13" t="n">
-        <v>11.79</v>
+        <v>11.55</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
@@ -965,31 +965,31 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.74</v>
+        <v>-1.97</v>
       </c>
       <c r="C14" t="n">
-        <v>1.35</v>
+        <v>-4.24</v>
       </c>
       <c r="D14" t="n">
-        <v>-11.36</v>
+        <v>-12.82</v>
       </c>
       <c r="E14" t="n">
-        <v>-12.28</v>
+        <v>-15.25</v>
       </c>
       <c r="F14" t="n">
-        <v>-21.64</v>
+        <v>-24.33</v>
       </c>
       <c r="G14" t="n">
-        <v>-42.46</v>
+        <v>-43.28</v>
       </c>
       <c r="H14" t="n">
-        <v>-59.12</v>
+        <v>-60.53</v>
       </c>
       <c r="I14" t="n">
-        <v>-29.8</v>
+        <v>-31.84</v>
       </c>
       <c r="J14" t="n">
-        <v>30.44</v>
+        <v>27.19</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
@@ -1004,31 +1004,31 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.21</v>
+        <v>0.18</v>
       </c>
       <c r="C15" t="n">
-        <v>1.05</v>
+        <v>1.78</v>
       </c>
       <c r="D15" t="n">
-        <v>4.51</v>
+        <v>5.03</v>
       </c>
       <c r="E15" t="n">
-        <v>-1.39</v>
+        <v>-2.29</v>
       </c>
       <c r="F15" t="n">
-        <v>-1.3</v>
+        <v>-0.28</v>
       </c>
       <c r="G15" t="n">
-        <v>7.89</v>
+        <v>7.73</v>
       </c>
       <c r="H15" t="n">
-        <v>5.89</v>
+        <v>6.42</v>
       </c>
       <c r="I15" t="n">
-        <v>28.03</v>
+        <v>28.35</v>
       </c>
       <c r="J15" t="n">
-        <v>-12.07</v>
+        <v>-12.94</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
@@ -1058,16 +1058,16 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>29.79</v>
+        <v>29.01</v>
       </c>
       <c r="H16" t="n">
-        <v>20.64</v>
+        <v>20.35</v>
       </c>
       <c r="I16" t="n">
         <v>45.92</v>
       </c>
       <c r="J16" t="n">
-        <v>-5.52</v>
+        <v>-6.18</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
@@ -1082,31 +1082,31 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.18</v>
+        <v>1.23</v>
       </c>
       <c r="C17" t="n">
-        <v>-1.05</v>
+        <v>1.59</v>
       </c>
       <c r="D17" t="n">
-        <v>-5.03</v>
+        <v>-0.86</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.18</v>
+        <v>0.88</v>
       </c>
       <c r="F17" t="n">
-        <v>-14.48</v>
+        <v>-11.52</v>
       </c>
       <c r="G17" t="n">
-        <v>-26.55</v>
+        <v>-25.29</v>
       </c>
       <c r="H17" t="n">
-        <v>-23.27</v>
+        <v>-20.77</v>
       </c>
       <c r="I17" t="n">
-        <v>-6.9</v>
+        <v>-5.42</v>
       </c>
       <c r="J17" t="n">
-        <v>-58</v>
+        <v>-57.46</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
@@ -1121,31 +1121,31 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.79</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.43</v>
+        <v>0.14</v>
       </c>
       <c r="D18" t="n">
-        <v>11.21</v>
+        <v>9.84</v>
       </c>
       <c r="E18" t="n">
-        <v>-9.4</v>
+        <v>-9.800000000000001</v>
       </c>
       <c r="F18" t="n">
-        <v>2.3</v>
+        <v>2.38</v>
       </c>
       <c r="G18" t="n">
-        <v>34.93</v>
+        <v>32.17</v>
       </c>
       <c r="H18" t="n">
-        <v>53.73</v>
+        <v>56.61</v>
       </c>
       <c r="I18" t="n">
-        <v>85.09999999999999</v>
+        <v>84.15000000000001</v>
       </c>
       <c r="J18" t="n">
-        <v>2.45</v>
+        <v>1.1</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
@@ -1175,10 +1175,10 @@
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>5.68</v>
+        <v>5.63</v>
       </c>
       <c r="H19" t="n">
-        <v>-16.67</v>
+        <v>-16.73</v>
       </c>
       <c r="I19" t="n">
         <v>41.14</v>
@@ -1197,31 +1197,31 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-0.51</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>0.12</v>
+        <v>1.29</v>
       </c>
       <c r="D20" t="n">
-        <v>-5.31</v>
+        <v>-4.08</v>
       </c>
       <c r="E20" t="n">
-        <v>-7.7</v>
+        <v>-6.79</v>
       </c>
       <c r="F20" t="n">
-        <v>-10.92</v>
+        <v>-9.75</v>
       </c>
       <c r="G20" t="n">
-        <v>-23.47</v>
+        <v>-22.76</v>
       </c>
       <c r="H20" t="n">
-        <v>-10.77</v>
+        <v>-9.23</v>
       </c>
       <c r="I20" t="n">
-        <v>25.77</v>
+        <v>25.99</v>
       </c>
       <c r="J20" t="n">
-        <v>-33.9</v>
+        <v>-34.06</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
@@ -1236,31 +1236,31 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-1.63</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.24</v>
+        <v>0.59</v>
       </c>
       <c r="D21" t="n">
-        <v>-6.29</v>
+        <v>-4.37</v>
       </c>
       <c r="E21" t="n">
-        <v>-7.93</v>
+        <v>-8.6</v>
       </c>
       <c r="F21" t="n">
-        <v>-9.15</v>
+        <v>-7.34</v>
       </c>
       <c r="G21" t="n">
-        <v>-9.74</v>
+        <v>-9.93</v>
       </c>
       <c r="H21" t="n">
-        <v>-0.51</v>
+        <v>-0.98</v>
       </c>
       <c r="I21" t="n">
-        <v>52.47</v>
+        <v>52.95</v>
       </c>
       <c r="J21" t="n">
-        <v>12.49</v>
+        <v>11.95</v>
       </c>
       <c r="K21" t="inlineStr">
         <is>
@@ -1290,10 +1290,10 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.15</v>
+        <v>-0.92</v>
       </c>
       <c r="H22" t="n">
-        <v>-15.75</v>
+        <v>-14.63</v>
       </c>
       <c r="I22" t="n">
         <v>35.18</v>
@@ -1327,10 +1327,10 @@
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>2.92</v>
+        <v>1.46</v>
       </c>
       <c r="H23" t="n">
-        <v>1.14</v>
+        <v>0.05</v>
       </c>
       <c r="I23" t="n">
         <v>-17.25</v>
@@ -1349,31 +1349,31 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.85</v>
+        <v>0.11</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.09</v>
+        <v>-0.32</v>
       </c>
       <c r="D24" t="n">
-        <v>2.46</v>
+        <v>3.61</v>
       </c>
       <c r="E24" t="n">
-        <v>15.22</v>
+        <v>13.69</v>
       </c>
       <c r="F24" t="n">
-        <v>6.68</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="G24" t="n">
-        <v>18.55</v>
+        <v>17.5</v>
       </c>
       <c r="H24" t="n">
-        <v>7.52</v>
+        <v>7.08</v>
       </c>
       <c r="I24" t="n">
-        <v>80.33</v>
+        <v>81.34</v>
       </c>
       <c r="J24" t="n">
-        <v>173.31</v>
+        <v>181.17</v>
       </c>
       <c r="K24" t="inlineStr">
         <is>
@@ -1388,31 +1388,31 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.41</v>
+        <v>-0.7</v>
       </c>
       <c r="C25" t="n">
-        <v>0.08</v>
+        <v>-0.97</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.49</v>
+        <v>0.12</v>
       </c>
       <c r="E25" t="n">
-        <v>13.81</v>
+        <v>9.050000000000001</v>
       </c>
       <c r="F25" t="n">
-        <v>2.47</v>
+        <v>4.11</v>
       </c>
       <c r="G25" t="n">
-        <v>1.87</v>
+        <v>1.72</v>
       </c>
       <c r="H25" t="n">
-        <v>-5.64</v>
+        <v>-6.42</v>
       </c>
       <c r="I25" t="n">
-        <v>34.54</v>
+        <v>33.97</v>
       </c>
       <c r="J25" t="n">
-        <v>30.68</v>
+        <v>31.83</v>
       </c>
       <c r="K25" t="inlineStr">
         <is>
@@ -1427,31 +1427,31 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.85</v>
+        <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>0.05</v>
+        <v>0.33</v>
       </c>
       <c r="D26" t="n">
-        <v>-1.16</v>
+        <v>0.37</v>
       </c>
       <c r="E26" t="n">
-        <v>10.56</v>
+        <v>8.09</v>
       </c>
       <c r="F26" t="n">
-        <v>2.15</v>
+        <v>3.99</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.28</v>
+        <v>0.47</v>
       </c>
       <c r="H26" t="n">
-        <v>-16.79</v>
+        <v>-17.62</v>
       </c>
       <c r="I26" t="n">
-        <v>6.69</v>
+        <v>6.74</v>
       </c>
       <c r="J26" t="n">
-        <v>9.539999999999999</v>
+        <v>10.72</v>
       </c>
       <c r="K26" t="inlineStr">
         <is>
@@ -1466,31 +1466,31 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0</v>
+        <v>-0.38</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.77</v>
+        <v>-0.55</v>
       </c>
       <c r="D27" t="n">
-        <v>-3.77</v>
+        <v>-2.58</v>
       </c>
       <c r="E27" t="n">
-        <v>7.47</v>
+        <v>4.85</v>
       </c>
       <c r="F27" t="n">
-        <v>-3.1</v>
+        <v>-2.05</v>
       </c>
       <c r="G27" t="n">
-        <v>-4.48</v>
+        <v>-4.77</v>
       </c>
       <c r="H27" t="n">
-        <v>-12.67</v>
+        <v>-13.12</v>
       </c>
       <c r="I27" t="n">
-        <v>2.2</v>
+        <v>2.31</v>
       </c>
       <c r="J27" t="n">
-        <v>14.89</v>
+        <v>17.7</v>
       </c>
       <c r="K27" t="inlineStr">
         <is>
@@ -1505,31 +1505,31 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1.27</v>
+        <v>0</v>
       </c>
       <c r="C28" t="n">
-        <v>2.21</v>
+        <v>2.14</v>
       </c>
       <c r="D28" t="n">
-        <v>3.51</v>
+        <v>4.46</v>
       </c>
       <c r="E28" t="n">
-        <v>18.92</v>
+        <v>16.38</v>
       </c>
       <c r="F28" t="n">
-        <v>9.220000000000001</v>
+        <v>11.5</v>
       </c>
       <c r="G28" t="n">
-        <v>14.44</v>
+        <v>14.74</v>
       </c>
       <c r="H28" t="n">
-        <v>14.23</v>
+        <v>12.1</v>
       </c>
       <c r="I28" t="n">
-        <v>93.45</v>
+        <v>93.88</v>
       </c>
       <c r="J28" t="n">
-        <v>154.14</v>
+        <v>157.75</v>
       </c>
       <c r="K28" t="inlineStr">
         <is>
@@ -1544,31 +1544,31 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-0.26</v>
+        <v>0</v>
       </c>
       <c r="C29" t="n">
-        <v>-1.55</v>
+        <v>-1.4</v>
       </c>
       <c r="D29" t="n">
-        <v>-2.18</v>
+        <v>-1.38</v>
       </c>
       <c r="E29" t="n">
-        <v>10.68</v>
+        <v>8</v>
       </c>
       <c r="F29" t="n">
-        <v>0.09</v>
+        <v>2.51</v>
       </c>
       <c r="G29" t="n">
-        <v>-11.97</v>
+        <v>-11.86</v>
       </c>
       <c r="H29" t="n">
-        <v>-23.8</v>
+        <v>-23.67</v>
       </c>
       <c r="I29" t="n">
-        <v>-7.87</v>
+        <v>-7.68</v>
       </c>
       <c r="J29" t="n">
-        <v>5.67</v>
+        <v>10.59</v>
       </c>
       <c r="K29" t="inlineStr">
         <is>
@@ -1583,31 +1583,31 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.28</v>
+        <v>-0.85</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.33</v>
+        <v>-1.23</v>
       </c>
       <c r="D30" t="n">
-        <v>-0.77</v>
+        <v>0.05</v>
       </c>
       <c r="E30" t="n">
-        <v>12.05</v>
+        <v>8.76</v>
       </c>
       <c r="F30" t="n">
-        <v>0.57</v>
+        <v>1.85</v>
       </c>
       <c r="G30" t="n">
-        <v>4.07</v>
+        <v>3.29</v>
       </c>
       <c r="H30" t="n">
-        <v>1.2</v>
+        <v>0.13</v>
       </c>
       <c r="I30" t="n">
-        <v>37.63</v>
+        <v>36.74</v>
       </c>
       <c r="J30" t="n">
-        <v>44.64</v>
+        <v>46.27</v>
       </c>
       <c r="K30" t="inlineStr">
         <is>
@@ -1622,31 +1622,31 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>1.19</v>
+        <v>-0.71</v>
       </c>
       <c r="C31" t="n">
-        <v>0.09</v>
+        <v>-0.58</v>
       </c>
       <c r="D31" t="n">
-        <v>-0.93</v>
+        <v>-0.17</v>
       </c>
       <c r="E31" t="n">
-        <v>15.99</v>
+        <v>13.05</v>
       </c>
       <c r="F31" t="n">
-        <v>1.78</v>
+        <v>3.43</v>
       </c>
       <c r="G31" t="n">
-        <v>3.14</v>
+        <v>1.45</v>
       </c>
       <c r="H31" t="n">
-        <v>-8.880000000000001</v>
+        <v>-9.49</v>
       </c>
       <c r="I31" t="n">
-        <v>9.720000000000001</v>
+        <v>9.25</v>
       </c>
       <c r="J31" t="n">
-        <v>-1.39</v>
+        <v>-0.17</v>
       </c>
       <c r="K31" t="inlineStr">
         <is>
@@ -1661,31 +1661,31 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>1.41</v>
+        <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>1.83</v>
+        <v>2.44</v>
       </c>
       <c r="D32" t="n">
-        <v>6.64</v>
+        <v>6.58</v>
       </c>
       <c r="E32" t="n">
-        <v>17.2</v>
+        <v>14.01</v>
       </c>
       <c r="F32" t="n">
-        <v>2.59</v>
+        <v>4.19</v>
       </c>
       <c r="G32" t="n">
-        <v>28.23</v>
+        <v>29.38</v>
       </c>
       <c r="H32" t="n">
-        <v>37.28</v>
+        <v>36.96</v>
       </c>
       <c r="I32" t="n">
-        <v>80.16</v>
+        <v>80.3</v>
       </c>
       <c r="J32" t="n">
-        <v>-39.75</v>
+        <v>-39.32</v>
       </c>
       <c r="K32" t="inlineStr">
         <is>
@@ -1700,31 +1700,31 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.92</v>
+        <v>0</v>
       </c>
       <c r="C33" t="n">
-        <v>0.21</v>
+        <v>-0</v>
       </c>
       <c r="D33" t="n">
-        <v>2.78</v>
+        <v>4.64</v>
       </c>
       <c r="E33" t="n">
-        <v>18.82</v>
+        <v>16.86</v>
       </c>
       <c r="F33" t="n">
-        <v>5.49</v>
+        <v>7.37</v>
       </c>
       <c r="G33" t="n">
-        <v>17.68</v>
+        <v>16.58</v>
       </c>
       <c r="H33" t="n">
-        <v>11.96</v>
+        <v>10.58</v>
       </c>
       <c r="I33" t="n">
-        <v>55.44</v>
+        <v>55.66</v>
       </c>
       <c r="J33" t="n">
-        <v>75.55</v>
+        <v>76.09</v>
       </c>
       <c r="K33" t="inlineStr">
         <is>
@@ -1739,31 +1739,31 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1.1</v>
+        <v>-0.5</v>
       </c>
       <c r="C34" t="n">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.21</v>
+        <v>0.15</v>
       </c>
       <c r="E34" t="n">
-        <v>12.23</v>
+        <v>9.16</v>
       </c>
       <c r="F34" t="n">
-        <v>2.36</v>
+        <v>3.88</v>
       </c>
       <c r="G34" t="n">
-        <v>10.51</v>
+        <v>10.15</v>
       </c>
       <c r="H34" t="n">
-        <v>3.04</v>
+        <v>1.84</v>
       </c>
       <c r="I34" t="n">
-        <v>30.43</v>
+        <v>29.97</v>
       </c>
       <c r="J34" t="n">
-        <v>8.94</v>
+        <v>12.17</v>
       </c>
       <c r="K34" t="inlineStr">
         <is>
@@ -1778,31 +1778,31 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.88</v>
+        <v>-0.87</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>-0.89</v>
       </c>
       <c r="D35" t="n">
-        <v>2.94</v>
+        <v>4.99</v>
       </c>
       <c r="E35" t="n">
-        <v>21.89</v>
+        <v>18.15</v>
       </c>
       <c r="F35" t="n">
-        <v>3.4</v>
+        <v>5.47</v>
       </c>
       <c r="G35" t="n">
-        <v>6.39</v>
+        <v>5.01</v>
       </c>
       <c r="H35" t="n">
-        <v>-1.88</v>
+        <v>-3.01</v>
       </c>
       <c r="I35" t="n">
-        <v>61.53</v>
+        <v>60.65</v>
       </c>
       <c r="J35" t="n">
-        <v>88.90000000000001</v>
+        <v>90.22</v>
       </c>
       <c r="K35" t="inlineStr">
         <is>
@@ -1817,31 +1817,31 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.99</v>
+        <v>0</v>
       </c>
       <c r="C36" t="n">
-        <v>-1.39</v>
+        <v>-1.21</v>
       </c>
       <c r="D36" t="n">
-        <v>-4.14</v>
+        <v>-2.33</v>
       </c>
       <c r="E36" t="n">
-        <v>4.71</v>
+        <v>3.52</v>
       </c>
       <c r="F36" t="n">
-        <v>-1.72</v>
+        <v>0.14</v>
       </c>
       <c r="G36" t="n">
-        <v>-5.92</v>
+        <v>-4.21</v>
       </c>
       <c r="H36" t="n">
-        <v>-19.5</v>
+        <v>-20.3</v>
       </c>
       <c r="I36" t="n">
-        <v>-6.07</v>
+        <v>-6.1</v>
       </c>
       <c r="J36" t="n">
-        <v>-20.25</v>
+        <v>-18.46</v>
       </c>
       <c r="K36" t="inlineStr">
         <is>
@@ -1856,31 +1856,31 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>-0.29</v>
+        <v>0</v>
       </c>
       <c r="C37" t="n">
-        <v>0.39</v>
+        <v>0.1</v>
       </c>
       <c r="D37" t="n">
-        <v>-3.48</v>
+        <v>-2.64</v>
       </c>
       <c r="E37" t="n">
-        <v>5.01</v>
+        <v>3.41</v>
       </c>
       <c r="F37" t="n">
-        <v>-0.87</v>
+        <v>1.48</v>
       </c>
       <c r="G37" t="n">
-        <v>-3.39</v>
+        <v>-2.74</v>
       </c>
       <c r="H37" t="n">
-        <v>-3.11</v>
+        <v>-2.37</v>
       </c>
       <c r="I37" t="n">
-        <v>-4.73</v>
+        <v>-4.36</v>
       </c>
       <c r="J37" t="n">
-        <v>-35.12</v>
+        <v>-33.66</v>
       </c>
       <c r="K37" t="inlineStr">
         <is>
@@ -1895,31 +1895,31 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.64</v>
+        <v>-0.3</v>
       </c>
       <c r="C38" t="n">
-        <v>1.26</v>
+        <v>1.64</v>
       </c>
       <c r="D38" t="n">
-        <v>-2.91</v>
+        <v>-2.66</v>
       </c>
       <c r="E38" t="n">
-        <v>10.36</v>
+        <v>7.26</v>
       </c>
       <c r="F38" t="n">
-        <v>3.48</v>
+        <v>5.36</v>
       </c>
       <c r="G38" t="n">
-        <v>8.66</v>
+        <v>7.34</v>
       </c>
       <c r="H38" t="n">
-        <v>11.02</v>
+        <v>10.54</v>
       </c>
       <c r="I38" t="n">
-        <v>4.83</v>
+        <v>4.69</v>
       </c>
       <c r="J38" t="n">
-        <v>-21.52</v>
+        <v>-19.52</v>
       </c>
       <c r="K38" t="inlineStr">
         <is>
@@ -1934,31 +1934,31 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>1.31</v>
+        <v>0</v>
       </c>
       <c r="C39" t="n">
-        <v>1.48</v>
+        <v>1.36</v>
       </c>
       <c r="D39" t="n">
-        <v>-4.16</v>
+        <v>-2.04</v>
       </c>
       <c r="E39" t="n">
-        <v>20.67</v>
+        <v>17.78</v>
       </c>
       <c r="F39" t="n">
-        <v>6.99</v>
+        <v>9.539999999999999</v>
       </c>
       <c r="G39" t="n">
-        <v>5.7</v>
+        <v>3.19</v>
       </c>
       <c r="H39" t="n">
-        <v>-11.65</v>
+        <v>-12.45</v>
       </c>
       <c r="I39" t="n">
-        <v>26.65</v>
+        <v>26.85</v>
       </c>
       <c r="J39" t="n">
-        <v>10.87</v>
+        <v>13.65</v>
       </c>
       <c r="K39" t="inlineStr">
         <is>
@@ -1973,31 +1973,31 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.49</v>
+        <v>-0.79</v>
       </c>
       <c r="C40" t="n">
-        <v>-0.16</v>
+        <v>-1.64</v>
       </c>
       <c r="D40" t="n">
-        <v>-1.09</v>
+        <v>-0.98</v>
       </c>
       <c r="E40" t="n">
-        <v>12.5</v>
+        <v>10.32</v>
       </c>
       <c r="F40" t="n">
-        <v>1.11</v>
+        <v>1.43</v>
       </c>
       <c r="G40" t="n">
-        <v>5</v>
+        <v>4.9</v>
       </c>
       <c r="H40" t="n">
-        <v>-4.55</v>
+        <v>-5.1</v>
       </c>
       <c r="I40" t="n">
-        <v>43.85</v>
+        <v>43.06</v>
       </c>
       <c r="J40" t="n">
-        <v>49.2</v>
+        <v>50.35</v>
       </c>
       <c r="K40" t="inlineStr">
         <is>
@@ -2012,31 +2012,31 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.89</v>
+        <v>-0.79</v>
       </c>
       <c r="C41" t="n">
-        <v>0.25</v>
+        <v>-0.55</v>
       </c>
       <c r="D41" t="n">
-        <v>-1</v>
+        <v>-0.67</v>
       </c>
       <c r="E41" t="n">
-        <v>6.79</v>
+        <v>4.2</v>
       </c>
       <c r="F41" t="n">
-        <v>-0.88</v>
+        <v>0.43</v>
       </c>
       <c r="G41" t="n">
-        <v>0.12</v>
+        <v>0.46</v>
       </c>
       <c r="H41" t="n">
-        <v>-4.55</v>
+        <v>-5.98</v>
       </c>
       <c r="I41" t="n">
-        <v>3.54</v>
+        <v>2.91</v>
       </c>
       <c r="J41" t="n">
-        <v>-17.83</v>
+        <v>-16.49</v>
       </c>
       <c r="K41" t="inlineStr">
         <is>
@@ -2051,31 +2051,31 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>-0.43</v>
+        <v>-0.66</v>
       </c>
       <c r="C42" t="n">
-        <v>0.2</v>
+        <v>-2.21</v>
       </c>
       <c r="D42" t="n">
-        <v>0.37</v>
+        <v>-0.1</v>
       </c>
       <c r="E42" t="n">
-        <v>23.92</v>
+        <v>20.51</v>
       </c>
       <c r="F42" t="n">
-        <v>1.49</v>
+        <v>3.8</v>
       </c>
       <c r="G42" t="n">
-        <v>-1.89</v>
+        <v>-4.29</v>
       </c>
       <c r="H42" t="n">
-        <v>-21.44</v>
+        <v>-21.32</v>
       </c>
       <c r="I42" t="n">
-        <v>8.48</v>
+        <v>8.67</v>
       </c>
       <c r="J42" t="n">
-        <v>22.75</v>
+        <v>25.26</v>
       </c>
       <c r="K42" t="inlineStr">
         <is>
@@ -2090,31 +2090,31 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.06</v>
+        <v>-0.36</v>
       </c>
       <c r="C43" t="n">
-        <v>-0.23</v>
+        <v>-0.86</v>
       </c>
       <c r="D43" t="n">
-        <v>-2.9</v>
+        <v>-2.05</v>
       </c>
       <c r="E43" t="n">
-        <v>11.91</v>
+        <v>9.77</v>
       </c>
       <c r="F43" t="n">
-        <v>3.21</v>
+        <v>5.89</v>
       </c>
       <c r="G43" t="n">
-        <v>-5.91</v>
+        <v>-5.15</v>
       </c>
       <c r="H43" t="n">
-        <v>2.14</v>
+        <v>1.61</v>
       </c>
       <c r="I43" t="n">
-        <v>14.96</v>
+        <v>15.05</v>
       </c>
       <c r="J43" t="n">
-        <v>2.58</v>
+        <v>4.25</v>
       </c>
       <c r="K43" t="inlineStr">
         <is>
@@ -2129,31 +2129,31 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>1.1</v>
+        <v>-1.58</v>
       </c>
       <c r="C44" t="n">
-        <v>-2.51</v>
+        <v>-3.34</v>
       </c>
       <c r="D44" t="n">
-        <v>-8.74</v>
+        <v>-7.74</v>
       </c>
       <c r="E44" t="n">
-        <v>-5.64</v>
+        <v>-8.81</v>
       </c>
       <c r="F44" t="n">
-        <v>-19.53</v>
+        <v>-19.32</v>
       </c>
       <c r="G44" t="n">
-        <v>-28.76</v>
+        <v>-29.06</v>
       </c>
       <c r="H44" t="n">
-        <v>-33.51</v>
+        <v>-34.53</v>
       </c>
       <c r="I44" t="n">
-        <v>-35.06</v>
+        <v>-36.01</v>
       </c>
       <c r="J44" t="n">
-        <v>-17.09</v>
+        <v>-16.87</v>
       </c>
       <c r="K44" t="inlineStr">
         <is>
@@ -2168,31 +2168,31 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.78</v>
+        <v>-1.01</v>
       </c>
       <c r="C45" t="n">
-        <v>2.05</v>
+        <v>0.11</v>
       </c>
       <c r="D45" t="n">
-        <v>4.04</v>
+        <v>4.22</v>
       </c>
       <c r="E45" t="n">
-        <v>11.27</v>
+        <v>8.69</v>
       </c>
       <c r="F45" t="n">
-        <v>6.48</v>
+        <v>7.73</v>
       </c>
       <c r="G45" t="n">
-        <v>13.35</v>
+        <v>12.8</v>
       </c>
       <c r="H45" t="n">
-        <v>4.1</v>
+        <v>1.79</v>
       </c>
       <c r="I45" t="n">
-        <v>23.43</v>
+        <v>22.54</v>
       </c>
       <c r="J45" t="n">
-        <v>47.24</v>
+        <v>49.2</v>
       </c>
       <c r="K45" t="inlineStr">
         <is>
@@ -2207,31 +2207,31 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>1.48</v>
+        <v>-0.66</v>
       </c>
       <c r="C46" t="n">
-        <v>-0.36</v>
+        <v>-1.27</v>
       </c>
       <c r="D46" t="n">
-        <v>-3.65</v>
+        <v>-2.39</v>
       </c>
       <c r="E46" t="n">
-        <v>10</v>
+        <v>6.68</v>
       </c>
       <c r="F46" t="n">
-        <v>-4.52</v>
+        <v>-3.64</v>
       </c>
       <c r="G46" t="n">
-        <v>-11.36</v>
+        <v>-12.19</v>
       </c>
       <c r="H46" t="n">
-        <v>-12.13</v>
+        <v>-13.54</v>
       </c>
       <c r="I46" t="n">
-        <v>-3.39</v>
+        <v>-3.62</v>
       </c>
       <c r="J46" t="n">
-        <v>24.02</v>
+        <v>24.99</v>
       </c>
       <c r="K46" t="inlineStr">
         <is>
@@ -2246,31 +2246,31 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="C47" t="n">
-        <v>-0.75</v>
+        <v>-0.11</v>
       </c>
       <c r="D47" t="n">
-        <v>-5</v>
+        <v>-3.1</v>
       </c>
       <c r="E47" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.39</v>
       </c>
       <c r="F47" t="n">
-        <v>-10.73</v>
+        <v>-8.01</v>
       </c>
       <c r="G47" t="n">
-        <v>-13.34</v>
+        <v>-12.7</v>
       </c>
       <c r="H47" t="n">
-        <v>-16.95</v>
+        <v>-16.15</v>
       </c>
       <c r="I47" t="n">
-        <v>-24.18</v>
+        <v>-23.99</v>
       </c>
       <c r="J47" t="n">
-        <v>-27.31</v>
+        <v>-25.61</v>
       </c>
       <c r="K47" t="inlineStr">
         <is>
@@ -2285,31 +2285,31 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>1.95</v>
+        <v>-0.19</v>
       </c>
       <c r="C48" t="n">
-        <v>2.36</v>
+        <v>1.7</v>
       </c>
       <c r="D48" t="n">
-        <v>0.16</v>
+        <v>0.46</v>
       </c>
       <c r="E48" t="n">
-        <v>20.28</v>
+        <v>14.5</v>
       </c>
       <c r="F48" t="n">
-        <v>6.79</v>
+        <v>8.960000000000001</v>
       </c>
       <c r="G48" t="n">
-        <v>15.3</v>
+        <v>17.18</v>
       </c>
       <c r="H48" t="n">
-        <v>38.19</v>
+        <v>36.72</v>
       </c>
       <c r="I48" t="n">
-        <v>51.53</v>
+        <v>50.52</v>
       </c>
       <c r="J48" t="n">
-        <v>8.06</v>
+        <v>11.49</v>
       </c>
       <c r="K48" t="inlineStr">
         <is>
@@ -2324,31 +2324,31 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.68</v>
+        <v>-1.68</v>
       </c>
       <c r="C49" t="n">
-        <v>-0.67</v>
+        <v>-1.21</v>
       </c>
       <c r="D49" t="n">
-        <v>-5.19</v>
+        <v>-4.77</v>
       </c>
       <c r="E49" t="n">
-        <v>8.109999999999999</v>
+        <v>3.77</v>
       </c>
       <c r="F49" t="n">
-        <v>-0.23</v>
+        <v>-0.73</v>
       </c>
       <c r="G49" t="n">
-        <v>10.52</v>
+        <v>11.1</v>
       </c>
       <c r="H49" t="n">
-        <v>3.06</v>
+        <v>2.47</v>
       </c>
       <c r="I49" t="n">
-        <v>-26.99</v>
+        <v>-27.91</v>
       </c>
       <c r="J49" t="n">
-        <v>-15.53</v>
+        <v>-13.94</v>
       </c>
       <c r="K49" t="inlineStr">
         <is>
@@ -2363,31 +2363,31 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>1.22</v>
+        <v>-1.76</v>
       </c>
       <c r="C50" t="n">
-        <v>-0.73</v>
+        <v>-2.59</v>
       </c>
       <c r="D50" t="n">
-        <v>-8.76</v>
+        <v>-9.82</v>
       </c>
       <c r="E50" t="n">
-        <v>5.32</v>
+        <v>2.11</v>
       </c>
       <c r="F50" t="n">
-        <v>-16.75</v>
+        <v>-16.41</v>
       </c>
       <c r="G50" t="n">
-        <v>-11.85</v>
+        <v>-16.1</v>
       </c>
       <c r="H50" t="n">
-        <v>-2.39</v>
+        <v>-2.1</v>
       </c>
       <c r="I50" t="n">
-        <v>-44.99</v>
+        <v>-46.21</v>
       </c>
       <c r="J50" t="n">
-        <v>-36.65</v>
+        <v>-36.7</v>
       </c>
       <c r="K50" t="inlineStr">
         <is>
@@ -2402,31 +2402,31 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="C51" t="n">
-        <v>-0.25</v>
+        <v>0.21</v>
       </c>
       <c r="D51" t="n">
-        <v>2.08</v>
+        <v>2.02</v>
       </c>
       <c r="E51" t="n">
-        <v>16.96</v>
+        <v>15.01</v>
       </c>
       <c r="F51" t="n">
-        <v>4.61</v>
+        <v>8.4</v>
       </c>
       <c r="G51" t="n">
-        <v>11.07</v>
+        <v>13.64</v>
       </c>
       <c r="H51" t="n">
-        <v>-24.81</v>
+        <v>-23.9</v>
       </c>
       <c r="I51" t="n">
-        <v>-35.71</v>
+        <v>-35.25</v>
       </c>
       <c r="J51" t="n">
-        <v>-62.24</v>
+        <v>-61.12</v>
       </c>
       <c r="K51" t="inlineStr">
         <is>
@@ -2441,31 +2441,31 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>1.37</v>
+        <v>0</v>
       </c>
       <c r="C52" t="n">
-        <v>1.04</v>
+        <v>0.09</v>
       </c>
       <c r="D52" t="n">
-        <v>-0.76</v>
+        <v>0.32</v>
       </c>
       <c r="E52" t="n">
-        <v>16.81</v>
+        <v>16.16</v>
       </c>
       <c r="F52" t="n">
-        <v>1.7</v>
+        <v>3.64</v>
       </c>
       <c r="G52" t="n">
-        <v>8.56</v>
+        <v>10.05</v>
       </c>
       <c r="H52" t="n">
-        <v>6.09</v>
+        <v>6.69</v>
       </c>
       <c r="I52" t="n">
-        <v>-10.16</v>
+        <v>-10.08</v>
       </c>
       <c r="J52" t="n">
-        <v>5.11</v>
+        <v>7.63</v>
       </c>
       <c r="K52" t="inlineStr">
         <is>
@@ -2480,31 +2480,31 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.5</v>
+        <v>-0.08</v>
       </c>
       <c r="C53" t="n">
-        <v>1.93</v>
+        <v>0.42</v>
       </c>
       <c r="D53" t="n">
-        <v>2.72</v>
+        <v>3.12</v>
       </c>
       <c r="E53" t="n">
-        <v>15.53</v>
+        <v>14.51</v>
       </c>
       <c r="F53" t="n">
-        <v>12.72</v>
+        <v>14.82</v>
       </c>
       <c r="G53" t="n">
-        <v>24.82</v>
+        <v>24.88</v>
       </c>
       <c r="H53" t="n">
-        <v>9.26</v>
+        <v>8.73</v>
       </c>
       <c r="I53" t="n">
-        <v>54.37</v>
+        <v>54.53</v>
       </c>
       <c r="J53" t="n">
-        <v>114.55</v>
+        <v>120.04</v>
       </c>
       <c r="K53" t="inlineStr">
         <is>
@@ -2519,31 +2519,31 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.52</v>
+        <v>-1.61</v>
       </c>
       <c r="C54" t="n">
-        <v>-3.77</v>
+        <v>-3.68</v>
       </c>
       <c r="D54" t="n">
-        <v>-9.84</v>
+        <v>-9.09</v>
       </c>
       <c r="E54" t="n">
-        <v>-12.13</v>
+        <v>-14.35</v>
       </c>
       <c r="F54" t="n">
-        <v>-24.59</v>
+        <v>-23.69</v>
       </c>
       <c r="G54" t="n">
-        <v>-33</v>
+        <v>-32.94</v>
       </c>
       <c r="H54" t="n">
-        <v>-41.69</v>
+        <v>-42.19</v>
       </c>
       <c r="I54" t="n">
-        <v>-37.69</v>
+        <v>-38.76</v>
       </c>
       <c r="J54" t="n">
-        <v>-16.35</v>
+        <v>-15.6</v>
       </c>
       <c r="K54" t="inlineStr">
         <is>
@@ -2558,28 +2558,28 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>-4.29</v>
+        <v>-2.92</v>
       </c>
       <c r="D55" t="n">
-        <v>-8.18</v>
+        <v>-6.9</v>
       </c>
       <c r="E55" t="n">
-        <v>-12.68</v>
+        <v>-12.55</v>
       </c>
       <c r="F55" t="n">
-        <v>-22.92</v>
+        <v>-22.42</v>
       </c>
       <c r="G55" t="n">
-        <v>-32.22</v>
+        <v>-31.51</v>
       </c>
       <c r="H55" t="n">
-        <v>-40.99</v>
+        <v>-41.26</v>
       </c>
       <c r="I55" t="n">
-        <v>-5.28</v>
+        <v>-5.59</v>
       </c>
       <c r="J55" t="inlineStr"/>
       <c r="K55" t="inlineStr">
@@ -2595,31 +2595,31 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.59</v>
+        <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>3</v>
+        <v>2.13</v>
       </c>
       <c r="D56" t="n">
-        <v>-1.48</v>
+        <v>-0.8100000000000001</v>
       </c>
       <c r="E56" t="n">
-        <v>9.289999999999999</v>
+        <v>6.43</v>
       </c>
       <c r="F56" t="n">
-        <v>-5.34</v>
+        <v>-4.09</v>
       </c>
       <c r="G56" t="n">
-        <v>-6.82</v>
+        <v>-6.41</v>
       </c>
       <c r="H56" t="n">
-        <v>-5.17</v>
+        <v>-4.84</v>
       </c>
       <c r="I56" t="n">
-        <v>-19.92</v>
+        <v>-19.77</v>
       </c>
       <c r="J56" t="n">
-        <v>-5.22</v>
+        <v>-1.39</v>
       </c>
       <c r="K56" t="inlineStr">
         <is>
@@ -2634,31 +2634,31 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>2.61</v>
+        <v>2.15</v>
       </c>
       <c r="C57" t="n">
-        <v>2.55</v>
+        <v>4.09</v>
       </c>
       <c r="D57" t="n">
-        <v>-6.88</v>
+        <v>-3.27</v>
       </c>
       <c r="E57" t="n">
-        <v>8.48</v>
+        <v>7.87</v>
       </c>
       <c r="F57" t="n">
-        <v>-9.68</v>
+        <v>-4.37</v>
       </c>
       <c r="G57" t="n">
-        <v>-6.28</v>
+        <v>-3.81</v>
       </c>
       <c r="H57" t="n">
-        <v>-16.39</v>
+        <v>-14.8</v>
       </c>
       <c r="I57" t="n">
-        <v>-4.72</v>
+        <v>-2.22</v>
       </c>
       <c r="J57" t="n">
-        <v>3.35</v>
+        <v>8.960000000000001</v>
       </c>
       <c r="K57" t="inlineStr">
         <is>
@@ -2673,31 +2673,31 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.28</v>
+        <v>-0.24</v>
       </c>
       <c r="C58" t="n">
-        <v>0.38</v>
+        <v>-0.28</v>
       </c>
       <c r="D58" t="n">
-        <v>-0.24</v>
+        <v>0.71</v>
       </c>
       <c r="E58" t="n">
-        <v>2.86</v>
+        <v>1.82</v>
       </c>
       <c r="F58" t="n">
-        <v>-1.9</v>
+        <v>-0.98</v>
       </c>
       <c r="G58" t="n">
-        <v>-11.45</v>
+        <v>-11.14</v>
       </c>
       <c r="H58" t="n">
-        <v>-13.72</v>
+        <v>-13.25</v>
       </c>
       <c r="I58" t="n">
-        <v>-30.61</v>
+        <v>-30.54</v>
       </c>
       <c r="J58" t="n">
-        <v>-63.95</v>
+        <v>-63.29</v>
       </c>
       <c r="K58" t="inlineStr">
         <is>
@@ -2712,31 +2712,31 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.09</v>
+        <v>0.26</v>
       </c>
       <c r="C59" t="n">
-        <v>0.25</v>
+        <v>0.64</v>
       </c>
       <c r="D59" t="n">
-        <v>1.98</v>
+        <v>2</v>
       </c>
       <c r="E59" t="n">
-        <v>12.5</v>
+        <v>10.75</v>
       </c>
       <c r="F59" t="n">
-        <v>-1.17</v>
+        <v>1.84</v>
       </c>
       <c r="G59" t="n">
-        <v>-9.48</v>
+        <v>-9.25</v>
       </c>
       <c r="H59" t="n">
-        <v>-17.92</v>
+        <v>-18.67</v>
       </c>
       <c r="I59" t="n">
-        <v>-24.01</v>
+        <v>-23.8</v>
       </c>
       <c r="J59" t="n">
-        <v>-14.39</v>
+        <v>-11.9</v>
       </c>
       <c r="K59" t="inlineStr">
         <is>
@@ -2751,31 +2751,31 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.54</v>
+        <v>-0.6899999999999999</v>
       </c>
       <c r="C60" t="n">
-        <v>-0.24</v>
+        <v>-1.65</v>
       </c>
       <c r="D60" t="n">
-        <v>-2.48</v>
+        <v>-0.71</v>
       </c>
       <c r="E60" t="n">
-        <v>1.93</v>
+        <v>-0.76</v>
       </c>
       <c r="F60" t="n">
-        <v>-5.93</v>
+        <v>-3.73</v>
       </c>
       <c r="G60" t="n">
-        <v>-1.86</v>
+        <v>-2.7</v>
       </c>
       <c r="H60" t="n">
-        <v>-31.09</v>
+        <v>-31.72</v>
       </c>
       <c r="I60" t="n">
-        <v>35.95</v>
+        <v>35.22</v>
       </c>
       <c r="J60" t="n">
-        <v>65.40000000000001</v>
+        <v>68.11</v>
       </c>
       <c r="K60" t="inlineStr">
         <is>
@@ -2790,31 +2790,31 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0.72</v>
+        <v>0</v>
       </c>
       <c r="C61" t="n">
-        <v>0.32</v>
+        <v>-0.43</v>
       </c>
       <c r="D61" t="n">
-        <v>-6.23</v>
+        <v>-6.96</v>
       </c>
       <c r="E61" t="n">
-        <v>-0.61</v>
+        <v>-2.68</v>
       </c>
       <c r="F61" t="n">
-        <v>-14.48</v>
+        <v>-13.1</v>
       </c>
       <c r="G61" t="n">
-        <v>-25.59</v>
+        <v>-24.63</v>
       </c>
       <c r="H61" t="n">
-        <v>-22.16</v>
+        <v>-22.25</v>
       </c>
       <c r="I61" t="n">
-        <v>-34.11</v>
+        <v>-33.99</v>
       </c>
       <c r="J61" t="n">
-        <v>-8.33</v>
+        <v>-7.75</v>
       </c>
       <c r="K61" t="inlineStr">
         <is>
@@ -2829,31 +2829,31 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>2.49</v>
+        <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>5.57</v>
+        <v>6.03</v>
       </c>
       <c r="D62" t="n">
-        <v>-0.91</v>
+        <v>2.55</v>
       </c>
       <c r="E62" t="n">
-        <v>12.62</v>
+        <v>12</v>
       </c>
       <c r="F62" t="n">
-        <v>8.33</v>
+        <v>10.95</v>
       </c>
       <c r="G62" t="n">
-        <v>33.84</v>
+        <v>34.03</v>
       </c>
       <c r="H62" t="n">
-        <v>7.86</v>
+        <v>5.98</v>
       </c>
       <c r="I62" t="n">
-        <v>-7.02</v>
+        <v>-6.84</v>
       </c>
       <c r="J62" t="n">
-        <v>-19.64</v>
+        <v>-18.25</v>
       </c>
       <c r="K62" t="inlineStr">
         <is>
@@ -2868,31 +2868,31 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>1.84</v>
+        <v>-1.04</v>
       </c>
       <c r="C63" t="n">
-        <v>3.32</v>
+        <v>1.15</v>
       </c>
       <c r="D63" t="n">
-        <v>12.95</v>
+        <v>10.63</v>
       </c>
       <c r="E63" t="n">
-        <v>7.3</v>
+        <v>4.55</v>
       </c>
       <c r="F63" t="n">
-        <v>9.359999999999999</v>
+        <v>6.68</v>
       </c>
       <c r="G63" t="n">
-        <v>13.9</v>
+        <v>11.8</v>
       </c>
       <c r="H63" t="n">
-        <v>78.73</v>
+        <v>81.7</v>
       </c>
       <c r="I63" t="n">
-        <v>28.43</v>
+        <v>27.23</v>
       </c>
       <c r="J63" t="n">
-        <v>-12.27</v>
+        <v>-9.970000000000001</v>
       </c>
       <c r="K63" t="inlineStr">
         <is>
@@ -2907,31 +2907,31 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>1.73</v>
+        <v>0</v>
       </c>
       <c r="C64" t="n">
-        <v>0.68</v>
+        <v>1.55</v>
       </c>
       <c r="D64" t="n">
-        <v>-4.52</v>
+        <v>-2.18</v>
       </c>
       <c r="E64" t="n">
-        <v>5.44</v>
+        <v>2.23</v>
       </c>
       <c r="F64" t="n">
-        <v>-7.49</v>
+        <v>-3.78</v>
       </c>
       <c r="G64" t="n">
-        <v>-13.86</v>
+        <v>-14.22</v>
       </c>
       <c r="H64" t="n">
-        <v>-21.36</v>
+        <v>-20.23</v>
       </c>
       <c r="I64" t="n">
-        <v>-29.41</v>
+        <v>-29.33</v>
       </c>
       <c r="J64" t="n">
-        <v>-30.85</v>
+        <v>-28.04</v>
       </c>
       <c r="K64" t="inlineStr">
         <is>
@@ -2946,31 +2946,31 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>-0.34</v>
+        <v>0</v>
       </c>
       <c r="C65" t="n">
-        <v>-1.34</v>
+        <v>-0.87</v>
       </c>
       <c r="D65" t="n">
-        <v>-0.85</v>
+        <v>-1.58</v>
       </c>
       <c r="E65" t="n">
-        <v>-2.19</v>
+        <v>-4.75</v>
       </c>
       <c r="F65" t="n">
-        <v>-4.53</v>
+        <v>-2.94</v>
       </c>
       <c r="G65" t="n">
-        <v>-5.71</v>
+        <v>-3.19</v>
       </c>
       <c r="H65" t="n">
-        <v>21.76</v>
+        <v>21.77</v>
       </c>
       <c r="I65" t="n">
-        <v>28.1</v>
+        <v>28.53</v>
       </c>
       <c r="J65" t="n">
-        <v>-0.31</v>
+        <v>1.84</v>
       </c>
       <c r="K65" t="inlineStr">
         <is>
@@ -2985,31 +2985,31 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>-0.64</v>
+        <v>-0.32</v>
       </c>
       <c r="C66" t="n">
-        <v>-5.17</v>
+        <v>-5.2</v>
       </c>
       <c r="D66" t="n">
-        <v>-6.1</v>
+        <v>-5.49</v>
       </c>
       <c r="E66" t="n">
-        <v>-11.03</v>
+        <v>-13.66</v>
       </c>
       <c r="F66" t="n">
-        <v>-14.94</v>
+        <v>-14.31</v>
       </c>
       <c r="G66" t="n">
-        <v>-11.22</v>
+        <v>-7.38</v>
       </c>
       <c r="H66" t="n">
-        <v>23.59</v>
+        <v>24.95</v>
       </c>
       <c r="I66" t="n">
-        <v>-15.61</v>
+        <v>-15.59</v>
       </c>
       <c r="J66" t="n">
-        <v>-68.05</v>
+        <v>-67.5</v>
       </c>
       <c r="K66" t="inlineStr">
         <is>
@@ -3024,31 +3024,31 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>-0.84</v>
+        <v>0</v>
       </c>
       <c r="C67" t="n">
-        <v>-1.62</v>
+        <v>-1.48</v>
       </c>
       <c r="D67" t="n">
-        <v>-3.66</v>
+        <v>-4.18</v>
       </c>
       <c r="E67" t="n">
-        <v>-9</v>
+        <v>-11.11</v>
       </c>
       <c r="F67" t="n">
-        <v>-7.48</v>
+        <v>-5.74</v>
       </c>
       <c r="G67" t="n">
-        <v>-4.21</v>
+        <v>-2.49</v>
       </c>
       <c r="H67" t="n">
-        <v>18.72</v>
+        <v>18.2</v>
       </c>
       <c r="I67" t="n">
-        <v>7.41</v>
+        <v>7.65</v>
       </c>
       <c r="J67" t="n">
-        <v>-49.85</v>
+        <v>-48.4</v>
       </c>
       <c r="K67" t="inlineStr">
         <is>
@@ -3063,31 +3063,31 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>1.06</v>
+        <v>-1.29</v>
       </c>
       <c r="C68" t="n">
-        <v>1.45</v>
+        <v>0.34</v>
       </c>
       <c r="D68" t="n">
-        <v>-1.94</v>
+        <v>-3.8</v>
       </c>
       <c r="E68" t="n">
-        <v>2.87</v>
+        <v>0.5</v>
       </c>
       <c r="F68" t="n">
-        <v>-6.26</v>
+        <v>-6.7</v>
       </c>
       <c r="G68" t="n">
-        <v>-10.27</v>
+        <v>-10.89</v>
       </c>
       <c r="H68" t="n">
-        <v>-9.119999999999999</v>
+        <v>-10.86</v>
       </c>
       <c r="I68" t="n">
-        <v>13.84</v>
+        <v>13.31</v>
       </c>
       <c r="J68" t="n">
-        <v>58.82</v>
+        <v>59.35</v>
       </c>
       <c r="K68" t="inlineStr">
         <is>
@@ -3102,31 +3102,31 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>1.6</v>
+        <v>-0.17</v>
       </c>
       <c r="C69" t="n">
-        <v>2.01</v>
+        <v>1.68</v>
       </c>
       <c r="D69" t="n">
-        <v>2.86</v>
+        <v>1.98</v>
       </c>
       <c r="E69" t="n">
-        <v>9.289999999999999</v>
+        <v>8.17</v>
       </c>
       <c r="F69" t="n">
-        <v>-1.66</v>
+        <v>-1.76</v>
       </c>
       <c r="G69" t="n">
-        <v>-0.32</v>
+        <v>0.8</v>
       </c>
       <c r="H69" t="n">
-        <v>-2.38</v>
+        <v>-3.29</v>
       </c>
       <c r="I69" t="n">
-        <v>39.21</v>
+        <v>39.57</v>
       </c>
       <c r="J69" t="n">
-        <v>81.77</v>
+        <v>86.26000000000001</v>
       </c>
       <c r="K69" t="inlineStr">
         <is>
@@ -3141,28 +3141,28 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="C70" t="n">
-        <v>1.25</v>
+        <v>1.3</v>
       </c>
       <c r="D70" t="n">
-        <v>-1.08</v>
+        <v>-2.19</v>
       </c>
       <c r="E70" t="n">
-        <v>6.18</v>
+        <v>5.05</v>
       </c>
       <c r="F70" t="n">
-        <v>-9.68</v>
+        <v>-9.82</v>
       </c>
       <c r="G70" t="n">
-        <v>-10.39</v>
+        <v>-8.94</v>
       </c>
       <c r="H70" t="n">
-        <v>-9.140000000000001</v>
+        <v>-9.380000000000001</v>
       </c>
       <c r="I70" t="n">
-        <v>24.21</v>
+        <v>25</v>
       </c>
       <c r="J70" t="inlineStr"/>
       <c r="K70" t="inlineStr">
@@ -3178,31 +3178,31 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>1.01</v>
+        <v>0.24</v>
       </c>
       <c r="C71" t="n">
-        <v>0.57</v>
+        <v>0.25</v>
       </c>
       <c r="D71" t="n">
-        <v>-3.44</v>
+        <v>-1.42</v>
       </c>
       <c r="E71" t="n">
-        <v>12.12</v>
+        <v>10.53</v>
       </c>
       <c r="F71" t="n">
-        <v>0.51</v>
+        <v>3.52</v>
       </c>
       <c r="G71" t="n">
-        <v>13.95</v>
+        <v>11.83</v>
       </c>
       <c r="H71" t="n">
-        <v>-7.21</v>
+        <v>-5.58</v>
       </c>
       <c r="I71" t="n">
-        <v>61.07</v>
+        <v>62.92</v>
       </c>
       <c r="J71" t="n">
-        <v>174.83</v>
+        <v>185.48</v>
       </c>
       <c r="K71" t="inlineStr">
         <is>
@@ -3217,31 +3217,31 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0</v>
+        <v>-1.57</v>
       </c>
       <c r="C72" t="n">
-        <v>-0.95</v>
+        <v>-0.88</v>
       </c>
       <c r="D72" t="n">
-        <v>-1.94</v>
+        <v>0.19</v>
       </c>
       <c r="E72" t="n">
-        <v>27.07</v>
+        <v>25.51</v>
       </c>
       <c r="F72" t="n">
-        <v>10.33</v>
+        <v>12.38</v>
       </c>
       <c r="G72" t="n">
-        <v>32.32</v>
+        <v>30.98</v>
       </c>
       <c r="H72" t="n">
-        <v>26.01</v>
+        <v>26.4</v>
       </c>
       <c r="I72" t="n">
-        <v>156.35</v>
+        <v>158.7</v>
       </c>
       <c r="J72" t="n">
-        <v>197.12</v>
+        <v>209.55</v>
       </c>
       <c r="K72" t="inlineStr">
         <is>
@@ -3256,31 +3256,31 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>1.46</v>
+        <v>-1.18</v>
       </c>
       <c r="C73" t="n">
-        <v>-0.49</v>
+        <v>-1.35</v>
       </c>
       <c r="D73" t="n">
-        <v>-3.76</v>
+        <v>-3.72</v>
       </c>
       <c r="E73" t="n">
-        <v>18.91</v>
+        <v>15.32</v>
       </c>
       <c r="F73" t="n">
-        <v>3.2</v>
+        <v>4.13</v>
       </c>
       <c r="G73" t="n">
-        <v>-3.72</v>
+        <v>-6.58</v>
       </c>
       <c r="H73" t="n">
-        <v>-15.86</v>
+        <v>-13.5</v>
       </c>
       <c r="I73" t="n">
-        <v>58.76</v>
+        <v>58.69</v>
       </c>
       <c r="J73" t="n">
-        <v>74.33</v>
+        <v>79.61</v>
       </c>
       <c r="K73" t="inlineStr">
         <is>
@@ -3295,28 +3295,28 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>0.96</v>
+        <v>-1.55</v>
       </c>
       <c r="C74" t="n">
-        <v>0.01</v>
+        <v>-1.47</v>
       </c>
       <c r="D74" t="n">
-        <v>-3.91</v>
+        <v>-5.52</v>
       </c>
       <c r="E74" t="n">
-        <v>15.7</v>
+        <v>11.37</v>
       </c>
       <c r="F74" t="n">
-        <v>0.98</v>
+        <v>0.63</v>
       </c>
       <c r="G74" t="n">
-        <v>-5.86</v>
+        <v>-8.68</v>
       </c>
       <c r="H74" t="n">
-        <v>-18.13</v>
+        <v>-20.13</v>
       </c>
       <c r="I74" t="n">
-        <v>12.82</v>
+        <v>11.96</v>
       </c>
       <c r="J74" t="inlineStr"/>
       <c r="K74" t="inlineStr">
@@ -3332,31 +3332,31 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>0.63</v>
+        <v>0</v>
       </c>
       <c r="C75" t="n">
-        <v>-2.33</v>
+        <v>-2.21</v>
       </c>
       <c r="D75" t="n">
-        <v>-3.35</v>
+        <v>-2.25</v>
       </c>
       <c r="E75" t="n">
-        <v>19.37</v>
+        <v>17.53</v>
       </c>
       <c r="F75" t="n">
-        <v>4.7</v>
+        <v>6.89</v>
       </c>
       <c r="G75" t="n">
-        <v>-11.96</v>
+        <v>-12.39</v>
       </c>
       <c r="H75" t="n">
-        <v>-15.52</v>
+        <v>-14.15</v>
       </c>
       <c r="I75" t="n">
-        <v>12.2</v>
+        <v>13.22</v>
       </c>
       <c r="J75" t="n">
-        <v>38.71</v>
+        <v>44.91</v>
       </c>
       <c r="K75" t="inlineStr">
         <is>
@@ -3371,31 +3371,31 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>1.09</v>
+        <v>0</v>
       </c>
       <c r="C76" t="n">
-        <v>0.61</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="D76" t="n">
-        <v>0.12</v>
+        <v>1.75</v>
       </c>
       <c r="E76" t="n">
-        <v>15.65</v>
+        <v>14</v>
       </c>
       <c r="F76" t="n">
-        <v>3.05</v>
+        <v>4.76</v>
       </c>
       <c r="G76" t="n">
-        <v>11.24</v>
+        <v>11.05</v>
       </c>
       <c r="H76" t="n">
-        <v>11.74</v>
+        <v>11.64</v>
       </c>
       <c r="I76" t="n">
-        <v>58.77</v>
+        <v>59.72</v>
       </c>
       <c r="J76" t="n">
-        <v>128.11</v>
+        <v>136.04</v>
       </c>
       <c r="K76" t="inlineStr">
         <is>
@@ -3410,31 +3410,31 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0.49</v>
+        <v>-0.38</v>
       </c>
       <c r="C77" t="n">
-        <v>0.99</v>
+        <v>0.79</v>
       </c>
       <c r="D77" t="n">
-        <v>-2.65</v>
+        <v>-1.76</v>
       </c>
       <c r="E77" t="n">
-        <v>11.47</v>
+        <v>9.220000000000001</v>
       </c>
       <c r="F77" t="n">
-        <v>4.7</v>
+        <v>6.88</v>
       </c>
       <c r="G77" t="n">
-        <v>7.39</v>
+        <v>7.97</v>
       </c>
       <c r="H77" t="n">
-        <v>20.43</v>
+        <v>19.69</v>
       </c>
       <c r="I77" t="n">
-        <v>26.54</v>
+        <v>26.52</v>
       </c>
       <c r="J77" t="n">
-        <v>134.23</v>
+        <v>141.37</v>
       </c>
       <c r="K77" t="inlineStr">
         <is>
@@ -3449,31 +3449,31 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>-0.75</v>
+        <v>0</v>
       </c>
       <c r="C78" t="n">
-        <v>-3.18</v>
+        <v>-1.89</v>
       </c>
       <c r="D78" t="n">
-        <v>-6.58</v>
+        <v>-3.41</v>
       </c>
       <c r="E78" t="n">
-        <v>15.45</v>
+        <v>14.56</v>
       </c>
       <c r="F78" t="n">
-        <v>-10.46</v>
+        <v>-7.48</v>
       </c>
       <c r="G78" t="n">
-        <v>-1.9</v>
+        <v>-3.57</v>
       </c>
       <c r="H78" t="n">
-        <v>-11.02</v>
+        <v>-8.74</v>
       </c>
       <c r="I78" t="n">
-        <v>28.97</v>
+        <v>31.25</v>
       </c>
       <c r="J78" t="n">
-        <v>91.88</v>
+        <v>101.88</v>
       </c>
       <c r="K78" t="inlineStr">
         <is>
@@ -3488,31 +3488,31 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>0</v>
+        <v>-0.03</v>
       </c>
       <c r="C79" t="n">
-        <v>0.8</v>
+        <v>1.36</v>
       </c>
       <c r="D79" t="n">
-        <v>2.93</v>
+        <v>2.44</v>
       </c>
       <c r="E79" t="n">
-        <v>12.48</v>
+        <v>12.13</v>
       </c>
       <c r="F79" t="n">
-        <v>5.19</v>
+        <v>6.46</v>
       </c>
       <c r="G79" t="n">
-        <v>4.77</v>
+        <v>6.82</v>
       </c>
       <c r="H79" t="n">
-        <v>6.69</v>
+        <v>6.61</v>
       </c>
       <c r="I79" t="n">
-        <v>54.69</v>
+        <v>56.65</v>
       </c>
       <c r="J79" t="n">
-        <v>150.86</v>
+        <v>159.13</v>
       </c>
       <c r="K79" t="inlineStr">
         <is>
@@ -3527,31 +3527,31 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="C80" t="n">
-        <v>1.14</v>
+        <v>-0.27</v>
       </c>
       <c r="D80" t="n">
-        <v>0.9399999999999999</v>
+        <v>2.36</v>
       </c>
       <c r="E80" t="n">
-        <v>23.39</v>
+        <v>22.85</v>
       </c>
       <c r="F80" t="n">
-        <v>-12.51</v>
+        <v>-10.33</v>
       </c>
       <c r="G80" t="n">
-        <v>-12.66</v>
+        <v>-15.57</v>
       </c>
       <c r="H80" t="n">
-        <v>-18.67</v>
+        <v>-17.67</v>
       </c>
       <c r="I80" t="n">
-        <v>11.74</v>
+        <v>12.23</v>
       </c>
       <c r="J80" t="n">
-        <v>119.44</v>
+        <v>127.81</v>
       </c>
       <c r="K80" t="inlineStr">
         <is>
@@ -3566,31 +3566,31 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>-0.24</v>
+        <v>0</v>
       </c>
       <c r="C81" t="n">
-        <v>-0.65</v>
+        <v>-0.13</v>
       </c>
       <c r="D81" t="n">
-        <v>-2.44</v>
+        <v>-2.13</v>
       </c>
       <c r="E81" t="n">
-        <v>9.880000000000001</v>
+        <v>10.82</v>
       </c>
       <c r="F81" t="n">
-        <v>-7.2</v>
+        <v>-5.84</v>
       </c>
       <c r="G81" t="n">
-        <v>-7.19</v>
+        <v>-6.51</v>
       </c>
       <c r="H81" t="n">
-        <v>-5.84</v>
+        <v>-3.87</v>
       </c>
       <c r="I81" t="n">
-        <v>24.83</v>
+        <v>26.73</v>
       </c>
       <c r="J81" t="n">
-        <v>90.37</v>
+        <v>98.58</v>
       </c>
       <c r="K81" t="inlineStr">
         <is>
@@ -3605,31 +3605,31 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>0.19</v>
+        <v>-0.82</v>
       </c>
       <c r="C82" t="n">
-        <v>-0.59</v>
+        <v>-1.62</v>
       </c>
       <c r="D82" t="n">
-        <v>0.3</v>
+        <v>-2.04</v>
       </c>
       <c r="E82" t="n">
-        <v>13.1</v>
+        <v>11.66</v>
       </c>
       <c r="F82" t="n">
-        <v>4.15</v>
+        <v>5.15</v>
       </c>
       <c r="G82" t="n">
-        <v>-1.21</v>
+        <v>-1.5</v>
       </c>
       <c r="H82" t="n">
-        <v>-1.31</v>
+        <v>-1.07</v>
       </c>
       <c r="I82" t="n">
-        <v>29.24</v>
+        <v>29.28</v>
       </c>
       <c r="J82" t="n">
-        <v>71.15000000000001</v>
+        <v>75.98999999999999</v>
       </c>
       <c r="K82" t="inlineStr">
         <is>
@@ -3644,31 +3644,31 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>0.67</v>
+        <v>-0.24</v>
       </c>
       <c r="C83" t="n">
-        <v>1.16</v>
+        <v>0.91</v>
       </c>
       <c r="D83" t="n">
-        <v>5.54</v>
+        <v>4.2</v>
       </c>
       <c r="E83" t="n">
-        <v>13.85</v>
+        <v>13.04</v>
       </c>
       <c r="F83" t="n">
-        <v>7.83</v>
+        <v>7.8</v>
       </c>
       <c r="G83" t="n">
-        <v>10.09</v>
+        <v>11.24</v>
       </c>
       <c r="H83" t="n">
-        <v>12.47</v>
+        <v>12.02</v>
       </c>
       <c r="I83" t="n">
-        <v>45.33</v>
+        <v>45.71</v>
       </c>
       <c r="J83" t="n">
-        <v>58.64</v>
+        <v>61.96</v>
       </c>
       <c r="K83" t="inlineStr">
         <is>
@@ -3683,31 +3683,31 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>0.89</v>
+        <v>0</v>
       </c>
       <c r="C84" t="n">
-        <v>-1.15</v>
+        <v>-1.68</v>
       </c>
       <c r="D84" t="n">
-        <v>3.62</v>
+        <v>6.79</v>
       </c>
       <c r="E84" t="n">
-        <v>19.3</v>
+        <v>17.74</v>
       </c>
       <c r="F84" t="n">
-        <v>11.64</v>
+        <v>14.89</v>
       </c>
       <c r="G84" t="n">
-        <v>43.32</v>
+        <v>40.02</v>
       </c>
       <c r="H84" t="n">
-        <v>22.82</v>
+        <v>22.27</v>
       </c>
       <c r="I84" t="n">
-        <v>199.14</v>
+        <v>200.24</v>
       </c>
       <c r="J84" t="n">
-        <v>472.77</v>
+        <v>487.18</v>
       </c>
       <c r="K84" t="inlineStr">
         <is>
@@ -3722,31 +3722,31 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>0.54</v>
+        <v>0.18</v>
       </c>
       <c r="C85" t="n">
-        <v>-0.75</v>
+        <v>-1.35</v>
       </c>
       <c r="D85" t="n">
-        <v>6.86</v>
+        <v>11.21</v>
       </c>
       <c r="E85" t="n">
-        <v>31.22</v>
+        <v>28.62</v>
       </c>
       <c r="F85" t="n">
-        <v>16.41</v>
+        <v>21.51</v>
       </c>
       <c r="G85" t="n">
-        <v>50.53</v>
+        <v>48.2</v>
       </c>
       <c r="H85" t="n">
-        <v>35.13</v>
+        <v>32.5</v>
       </c>
       <c r="I85" t="n">
-        <v>282.06</v>
+        <v>284.2</v>
       </c>
       <c r="J85" t="n">
-        <v>807.78</v>
+        <v>828.87</v>
       </c>
       <c r="K85" t="inlineStr">
         <is>
@@ -3761,31 +3761,31 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>0.34</v>
+        <v>0</v>
       </c>
       <c r="C86" t="n">
-        <v>-0.92</v>
+        <v>-2.32</v>
       </c>
       <c r="D86" t="n">
-        <v>-1.33</v>
+        <v>2.32</v>
       </c>
       <c r="E86" t="n">
-        <v>24.47</v>
+        <v>22.3</v>
       </c>
       <c r="F86" t="n">
-        <v>4.46</v>
+        <v>9.1</v>
       </c>
       <c r="G86" t="n">
-        <v>17.63</v>
+        <v>14.59</v>
       </c>
       <c r="H86" t="n">
-        <v>-1.51</v>
+        <v>1.34</v>
       </c>
       <c r="I86" t="n">
-        <v>72.97</v>
+        <v>74.48999999999999</v>
       </c>
       <c r="J86" t="n">
-        <v>232.75</v>
+        <v>247.93</v>
       </c>
       <c r="K86" t="inlineStr">
         <is>
@@ -3837,31 +3837,31 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>1.34</v>
+        <v>-0.74</v>
       </c>
       <c r="C88" t="n">
-        <v>0.97</v>
+        <v>0.05</v>
       </c>
       <c r="D88" t="n">
-        <v>-2.61</v>
+        <v>-2.85</v>
       </c>
       <c r="E88" t="n">
-        <v>9.470000000000001</v>
+        <v>6.95</v>
       </c>
       <c r="F88" t="n">
-        <v>-2.38</v>
+        <v>-1.57</v>
       </c>
       <c r="G88" t="n">
-        <v>-2.23</v>
+        <v>-2.33</v>
       </c>
       <c r="H88" t="n">
-        <v>-2.85</v>
+        <v>-3.56</v>
       </c>
       <c r="I88" t="n">
-        <v>55.69</v>
+        <v>55.04</v>
       </c>
       <c r="J88" t="n">
-        <v>89.17</v>
+        <v>92.89</v>
       </c>
       <c r="K88" t="inlineStr">
         <is>
@@ -3876,31 +3876,31 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>0.7</v>
+        <v>-1.25</v>
       </c>
       <c r="C89" t="n">
-        <v>0.91</v>
+        <v>-1.26</v>
       </c>
       <c r="D89" t="n">
-        <v>-3.76</v>
+        <v>-3.79</v>
       </c>
       <c r="E89" t="n">
-        <v>15.95</v>
+        <v>12.61</v>
       </c>
       <c r="F89" t="n">
-        <v>8.050000000000001</v>
+        <v>10.28</v>
       </c>
       <c r="G89" t="n">
-        <v>-1.01</v>
+        <v>-2.41</v>
       </c>
       <c r="H89" t="n">
-        <v>31.97</v>
+        <v>29.15</v>
       </c>
       <c r="I89" t="n">
-        <v>88.73</v>
+        <v>87.05</v>
       </c>
       <c r="J89" t="n">
-        <v>44.35</v>
+        <v>47.85</v>
       </c>
       <c r="K89" t="inlineStr">
         <is>
@@ -3915,31 +3915,31 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>3.22</v>
+        <v>-3.07</v>
       </c>
       <c r="C90" t="n">
-        <v>2.74</v>
+        <v>-0.78</v>
       </c>
       <c r="D90" t="n">
-        <v>-7</v>
+        <v>-7.92</v>
       </c>
       <c r="E90" t="n">
-        <v>2.59</v>
+        <v>-0.42</v>
       </c>
       <c r="F90" t="n">
-        <v>-4.6</v>
+        <v>-3.89</v>
       </c>
       <c r="G90" t="n">
-        <v>-11.92</v>
+        <v>-11.29</v>
       </c>
       <c r="H90" t="n">
-        <v>-5.54</v>
+        <v>-8.130000000000001</v>
       </c>
       <c r="I90" t="n">
-        <v>27.78</v>
+        <v>24.68</v>
       </c>
       <c r="J90" t="n">
-        <v>22.82</v>
+        <v>20.77</v>
       </c>
       <c r="K90" t="inlineStr">
         <is>
@@ -3954,31 +3954,31 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>2.68</v>
+        <v>-2.86</v>
       </c>
       <c r="C91" t="n">
-        <v>2.23</v>
+        <v>-2.75</v>
       </c>
       <c r="D91" t="n">
-        <v>-8.07</v>
+        <v>-8.15</v>
       </c>
       <c r="E91" t="n">
-        <v>8.890000000000001</v>
+        <v>6.39</v>
       </c>
       <c r="F91" t="n">
-        <v>-2.72</v>
+        <v>-2.11</v>
       </c>
       <c r="G91" t="n">
-        <v>-15.57</v>
+        <v>-15.63</v>
       </c>
       <c r="H91" t="n">
-        <v>-21.99</v>
+        <v>-23.19</v>
       </c>
       <c r="I91" t="n">
-        <v>-2.98</v>
+        <v>-5.25</v>
       </c>
       <c r="J91" t="n">
-        <v>-27.8</v>
+        <v>-29.19</v>
       </c>
       <c r="K91" t="inlineStr">
         <is>
@@ -3993,31 +3993,31 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>0.36</v>
+        <v>0</v>
       </c>
       <c r="C92" t="n">
-        <v>-0.26</v>
+        <v>-0.36</v>
       </c>
       <c r="D92" t="n">
-        <v>-5.55</v>
+        <v>-4.67</v>
       </c>
       <c r="E92" t="n">
-        <v>9.94</v>
+        <v>6.64</v>
       </c>
       <c r="F92" t="n">
-        <v>-0.13</v>
+        <v>2.83</v>
       </c>
       <c r="G92" t="n">
-        <v>1.16</v>
+        <v>2.58</v>
       </c>
       <c r="H92" t="n">
-        <v>27.09</v>
+        <v>25.33</v>
       </c>
       <c r="I92" t="n">
-        <v>77.87</v>
+        <v>77.81</v>
       </c>
       <c r="J92" t="n">
-        <v>54.27</v>
+        <v>59.74</v>
       </c>
       <c r="K92" t="inlineStr">
         <is>
@@ -4032,31 +4032,31 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C93" t="n">
         <v>0.28</v>
       </c>
       <c r="D93" t="n">
-        <v>3.09</v>
+        <v>2.91</v>
       </c>
       <c r="E93" t="n">
-        <v>19.01</v>
+        <v>16.56</v>
       </c>
       <c r="F93" t="n">
-        <v>9.710000000000001</v>
+        <v>10.93</v>
       </c>
       <c r="G93" t="n">
-        <v>6.02</v>
+        <v>6</v>
       </c>
       <c r="H93" t="n">
-        <v>-2.12</v>
+        <v>-2.53</v>
       </c>
       <c r="I93" t="n">
-        <v>48.79</v>
+        <v>49.17</v>
       </c>
       <c r="J93" t="n">
-        <v>126.56</v>
+        <v>133.01</v>
       </c>
       <c r="K93" t="inlineStr">
         <is>
@@ -4071,31 +4071,31 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>-0.04</v>
+        <v>0</v>
       </c>
       <c r="C94" t="n">
-        <v>-0.88</v>
+        <v>-1.07</v>
       </c>
       <c r="D94" t="n">
-        <v>-2.03</v>
+        <v>-0.2</v>
       </c>
       <c r="E94" t="n">
-        <v>20.66</v>
+        <v>18.68</v>
       </c>
       <c r="F94" t="n">
-        <v>9.25</v>
+        <v>11.47</v>
       </c>
       <c r="G94" t="n">
-        <v>10.21</v>
+        <v>8.51</v>
       </c>
       <c r="H94" t="n">
-        <v>3.7</v>
+        <v>4.75</v>
       </c>
       <c r="I94" t="n">
-        <v>90.86</v>
+        <v>92.48999999999999</v>
       </c>
       <c r="J94" t="n">
-        <v>111.29</v>
+        <v>121.77</v>
       </c>
       <c r="K94" t="inlineStr">
         <is>
@@ -4110,31 +4110,31 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>-2.34</v>
+        <v>-0.92</v>
       </c>
       <c r="C95" t="n">
-        <v>-5.26</v>
+        <v>-7.13</v>
       </c>
       <c r="D95" t="n">
-        <v>-4.98</v>
+        <v>-6.03</v>
       </c>
       <c r="E95" t="n">
-        <v>23.22</v>
+        <v>16.55</v>
       </c>
       <c r="F95" t="n">
-        <v>5.27</v>
+        <v>5.07</v>
       </c>
       <c r="G95" t="n">
-        <v>-11.46</v>
+        <v>-13.89</v>
       </c>
       <c r="H95" t="n">
-        <v>-21.73</v>
+        <v>-22.1</v>
       </c>
       <c r="I95" t="n">
-        <v>1.77</v>
+        <v>1.04</v>
       </c>
       <c r="J95" t="n">
-        <v>37.04</v>
+        <v>41.05</v>
       </c>
       <c r="K95" t="inlineStr">
         <is>
@@ -4149,31 +4149,31 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>-3.04</v>
+        <v>-1.32</v>
       </c>
       <c r="C96" t="n">
-        <v>-7.56</v>
+        <v>-10.35</v>
       </c>
       <c r="D96" t="n">
-        <v>-8.09</v>
+        <v>-9.67</v>
       </c>
       <c r="E96" t="n">
-        <v>20.99</v>
+        <v>12.89</v>
       </c>
       <c r="F96" t="n">
-        <v>0.04</v>
+        <v>-0.91</v>
       </c>
       <c r="G96" t="n">
-        <v>-23.51</v>
+        <v>-26.54</v>
       </c>
       <c r="H96" t="n">
-        <v>-33.7</v>
+        <v>-34.45</v>
       </c>
       <c r="I96" t="n">
-        <v>-9.789999999999999</v>
+        <v>-11.05</v>
       </c>
       <c r="J96" t="n">
-        <v>25.99</v>
+        <v>28.98</v>
       </c>
       <c r="K96" t="inlineStr">
         <is>
@@ -4188,31 +4188,31 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>-1.67</v>
+        <v>0.74</v>
       </c>
       <c r="C97" t="n">
-        <v>-1.74</v>
+        <v>-0.72</v>
       </c>
       <c r="D97" t="n">
-        <v>5.03</v>
+        <v>4.91</v>
       </c>
       <c r="E97" t="n">
-        <v>10.45</v>
+        <v>11.47</v>
       </c>
       <c r="F97" t="n">
-        <v>15.5</v>
+        <v>16.19</v>
       </c>
       <c r="G97" t="n">
-        <v>12.29</v>
+        <v>15.43</v>
       </c>
       <c r="H97" t="n">
-        <v>22.36</v>
+        <v>21.86</v>
       </c>
       <c r="I97" t="n">
-        <v>67.88</v>
+        <v>69.55</v>
       </c>
       <c r="J97" t="n">
-        <v>139.93</v>
+        <v>150.42</v>
       </c>
       <c r="K97" t="inlineStr">
         <is>
@@ -4227,31 +4227,31 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>0</v>
+        <v>-0.31</v>
       </c>
       <c r="C98" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="D98" t="n">
-        <v>1.19</v>
+        <v>1.81</v>
       </c>
       <c r="E98" t="n">
-        <v>14.64</v>
+        <v>13.45</v>
       </c>
       <c r="F98" t="n">
-        <v>7.07</v>
+        <v>8.84</v>
       </c>
       <c r="G98" t="n">
-        <v>11.88</v>
+        <v>12.77</v>
       </c>
       <c r="H98" t="n">
-        <v>7.75</v>
+        <v>7.83</v>
       </c>
       <c r="I98" t="n">
-        <v>52.26</v>
+        <v>53.27</v>
       </c>
       <c r="J98" t="n">
-        <v>143.3</v>
+        <v>150.06</v>
       </c>
       <c r="K98" t="inlineStr">
         <is>
@@ -4266,31 +4266,31 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>0.93</v>
+        <v>0</v>
       </c>
       <c r="C99" t="n">
-        <v>-0.53</v>
+        <v>-0.96</v>
       </c>
       <c r="D99" t="n">
-        <v>3.87</v>
+        <v>5.24</v>
       </c>
       <c r="E99" t="n">
-        <v>15.27</v>
+        <v>13.79</v>
       </c>
       <c r="F99" t="n">
-        <v>8.83</v>
+        <v>11.25</v>
       </c>
       <c r="G99" t="n">
-        <v>31.13</v>
+        <v>28.66</v>
       </c>
       <c r="H99" t="n">
-        <v>11.07</v>
+        <v>10.7</v>
       </c>
       <c r="I99" t="n">
-        <v>103.91</v>
+        <v>104.85</v>
       </c>
       <c r="J99" t="n">
-        <v>215.94</v>
+        <v>223.82</v>
       </c>
       <c r="K99" t="inlineStr">
         <is>
@@ -4305,31 +4305,31 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>0.83</v>
+        <v>-0.04</v>
       </c>
       <c r="C100" t="n">
-        <v>-0.08</v>
+        <v>-0.53</v>
       </c>
       <c r="D100" t="n">
-        <v>2.18</v>
+        <v>3.23</v>
       </c>
       <c r="E100" t="n">
-        <v>15.66</v>
+        <v>13.97</v>
       </c>
       <c r="F100" t="n">
-        <v>6.57</v>
+        <v>8.539999999999999</v>
       </c>
       <c r="G100" t="n">
-        <v>18.02</v>
+        <v>16.72</v>
       </c>
       <c r="H100" t="n">
-        <v>6.67</v>
+        <v>6.3</v>
       </c>
       <c r="I100" t="n">
-        <v>78.28</v>
+        <v>79.03</v>
       </c>
       <c r="J100" t="n">
-        <v>168.43</v>
+        <v>175.89</v>
       </c>
       <c r="K100" t="inlineStr">
         <is>
@@ -4344,31 +4344,31 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>0.78</v>
+        <v>-1.37</v>
       </c>
       <c r="C101" t="n">
-        <v>-0.82</v>
+        <v>-3.33</v>
       </c>
       <c r="D101" t="n">
-        <v>-3.15</v>
+        <v>-3.38</v>
       </c>
       <c r="E101" t="n">
-        <v>17.48</v>
+        <v>13.48</v>
       </c>
       <c r="F101" t="n">
-        <v>-1.73</v>
+        <v>-1.2</v>
       </c>
       <c r="G101" t="n">
-        <v>-0.06</v>
+        <v>-2.8</v>
       </c>
       <c r="H101" t="n">
-        <v>-4.42</v>
+        <v>-4.26</v>
       </c>
       <c r="I101" t="n">
-        <v>30.3</v>
+        <v>29.22</v>
       </c>
       <c r="J101" t="n">
-        <v>73.31</v>
+        <v>77.42</v>
       </c>
       <c r="K101" t="inlineStr">
         <is>
@@ -4383,31 +4383,31 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>0.5</v>
+        <v>-0.9399999999999999</v>
       </c>
       <c r="C102" t="n">
-        <v>-1.09</v>
+        <v>-3.19</v>
       </c>
       <c r="D102" t="n">
-        <v>-3.54</v>
+        <v>-3.08</v>
       </c>
       <c r="E102" t="n">
-        <v>20.16</v>
+        <v>17.07</v>
       </c>
       <c r="F102" t="n">
-        <v>-2.84</v>
+        <v>-1.23</v>
       </c>
       <c r="G102" t="n">
-        <v>-6.52</v>
+        <v>-8.300000000000001</v>
       </c>
       <c r="H102" t="n">
-        <v>-12.36</v>
+        <v>-11.05</v>
       </c>
       <c r="I102" t="n">
-        <v>22.77</v>
+        <v>22.6</v>
       </c>
       <c r="J102" t="n">
-        <v>49.79</v>
+        <v>54.35</v>
       </c>
       <c r="K102" t="inlineStr">
         <is>
@@ -4422,31 +4422,31 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>1.1</v>
+        <v>0.34</v>
       </c>
       <c r="C103" t="n">
-        <v>-0.41</v>
+        <v>-0.67</v>
       </c>
       <c r="D103" t="n">
-        <v>4.01</v>
+        <v>6.54</v>
       </c>
       <c r="E103" t="n">
-        <v>15.57</v>
+        <v>14.33</v>
       </c>
       <c r="F103" t="n">
-        <v>7.96</v>
+        <v>10.5</v>
       </c>
       <c r="G103" t="n">
-        <v>25.03</v>
+        <v>24.56</v>
       </c>
       <c r="H103" t="n">
-        <v>1.22</v>
+        <v>0.89</v>
       </c>
       <c r="I103" t="n">
-        <v>93.78</v>
+        <v>95.33</v>
       </c>
       <c r="J103" t="n">
-        <v>226.51</v>
+        <v>237.3</v>
       </c>
       <c r="K103" t="inlineStr">
         <is>
@@ -4461,28 +4461,28 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>0.14</v>
+        <v>-0.98</v>
       </c>
       <c r="C104" t="n">
-        <v>-1.16</v>
+        <v>-1.81</v>
       </c>
       <c r="D104" t="n">
-        <v>-1.49</v>
+        <v>-3.1</v>
       </c>
       <c r="E104" t="n">
-        <v>14.66</v>
+        <v>10.84</v>
       </c>
       <c r="F104" t="n">
-        <v>0.22</v>
+        <v>0.29</v>
       </c>
       <c r="G104" t="n">
-        <v>-8.99</v>
+        <v>-10.77</v>
       </c>
       <c r="H104" t="n">
-        <v>-10.53</v>
+        <v>-11.41</v>
       </c>
       <c r="I104" t="n">
-        <v>4.93</v>
+        <v>4.51</v>
       </c>
       <c r="J104" t="inlineStr"/>
       <c r="K104" t="inlineStr">
@@ -4498,31 +4498,31 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>0.51</v>
+        <v>-0.38</v>
       </c>
       <c r="C105" t="n">
-        <v>0.34</v>
+        <v>-0.09</v>
       </c>
       <c r="D105" t="n">
-        <v>0.79</v>
+        <v>0.17</v>
       </c>
       <c r="E105" t="n">
-        <v>14.91</v>
+        <v>12.9</v>
       </c>
       <c r="F105" t="n">
-        <v>5.43</v>
+        <v>6.7</v>
       </c>
       <c r="G105" t="n">
-        <v>11.85</v>
+        <v>9.91</v>
       </c>
       <c r="H105" t="n">
-        <v>13.03</v>
+        <v>12.33</v>
       </c>
       <c r="I105" t="n">
-        <v>59.16</v>
+        <v>59.19</v>
       </c>
       <c r="J105" t="n">
-        <v>110.9</v>
+        <v>116.41</v>
       </c>
       <c r="K105" t="inlineStr">
         <is>
@@ -4537,31 +4537,31 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>0.5600000000000001</v>
+        <v>-0.49</v>
       </c>
       <c r="C106" t="n">
-        <v>0.23</v>
+        <v>-0.2</v>
       </c>
       <c r="D106" t="n">
-        <v>-0.6</v>
+        <v>-1.01</v>
       </c>
       <c r="E106" t="n">
-        <v>10.71</v>
+        <v>8.58</v>
       </c>
       <c r="F106" t="n">
-        <v>-1.71</v>
+        <v>-1.44</v>
       </c>
       <c r="G106" t="n">
-        <v>-4.93</v>
+        <v>-6.03</v>
       </c>
       <c r="H106" t="n">
-        <v>-2.29</v>
+        <v>-2.52</v>
       </c>
       <c r="I106" t="n">
-        <v>30.45</v>
+        <v>30.43</v>
       </c>
       <c r="J106" t="n">
-        <v>76.36</v>
+        <v>81.14</v>
       </c>
       <c r="K106" t="inlineStr">
         <is>
@@ -4576,31 +4576,31 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>0.66</v>
+        <v>-0.35</v>
       </c>
       <c r="C107" t="n">
-        <v>0.33</v>
+        <v>-0.17</v>
       </c>
       <c r="D107" t="n">
-        <v>1.9</v>
+        <v>2.12</v>
       </c>
       <c r="E107" t="n">
-        <v>12.86</v>
+        <v>10.91</v>
       </c>
       <c r="F107" t="n">
-        <v>4.45</v>
+        <v>5.3</v>
       </c>
       <c r="G107" t="n">
-        <v>10.21</v>
+        <v>9.69</v>
       </c>
       <c r="H107" t="n">
-        <v>6.19</v>
+        <v>5.09</v>
       </c>
       <c r="I107" t="n">
-        <v>67.08</v>
+        <v>67.13</v>
       </c>
       <c r="J107" t="n">
-        <v>142.94</v>
+        <v>148.75</v>
       </c>
       <c r="K107" t="inlineStr">
         <is>
@@ -4615,31 +4615,31 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>-0.49</v>
+        <v>-0.62</v>
       </c>
       <c r="C108" t="n">
-        <v>-0.27</v>
+        <v>-0.59</v>
       </c>
       <c r="D108" t="n">
-        <v>2.29</v>
+        <v>2.44</v>
       </c>
       <c r="E108" t="n">
-        <v>10.28</v>
+        <v>8.1</v>
       </c>
       <c r="F108" t="n">
-        <v>3.32</v>
+        <v>3.81</v>
       </c>
       <c r="G108" t="n">
-        <v>-5.05</v>
+        <v>-5.62</v>
       </c>
       <c r="H108" t="n">
-        <v>-15.06</v>
+        <v>-14.52</v>
       </c>
       <c r="I108" t="n">
-        <v>-11.01</v>
+        <v>-10.99</v>
       </c>
       <c r="J108" t="n">
-        <v>-15.86</v>
+        <v>-15.25</v>
       </c>
       <c r="K108" t="inlineStr">
         <is>
@@ -4654,31 +4654,31 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.26</v>
       </c>
       <c r="C109" t="n">
-        <v>0.25</v>
+        <v>-0.02</v>
       </c>
       <c r="D109" t="n">
-        <v>3.11</v>
+        <v>4.53</v>
       </c>
       <c r="E109" t="n">
-        <v>15.66</v>
+        <v>14.09</v>
       </c>
       <c r="F109" t="n">
-        <v>8.4</v>
+        <v>10.82</v>
       </c>
       <c r="G109" t="n">
-        <v>22.77</v>
+        <v>20.99</v>
       </c>
       <c r="H109" t="n">
-        <v>11.39</v>
+        <v>10.59</v>
       </c>
       <c r="I109" t="n">
-        <v>81.79000000000001</v>
+        <v>82.95</v>
       </c>
       <c r="J109" t="n">
-        <v>180.19</v>
+        <v>188.75</v>
       </c>
       <c r="K109" t="inlineStr">
         <is>
@@ -4693,31 +4693,31 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>1.22</v>
+        <v>1.19</v>
       </c>
       <c r="C110" t="n">
-        <v>0.31</v>
+        <v>0.85</v>
       </c>
       <c r="D110" t="n">
-        <v>6.87</v>
+        <v>10.69</v>
       </c>
       <c r="E110" t="n">
-        <v>20.14</v>
+        <v>19.95</v>
       </c>
       <c r="F110" t="n">
-        <v>14.24</v>
+        <v>18.12</v>
       </c>
       <c r="G110" t="n">
-        <v>16.43</v>
+        <v>20.69</v>
       </c>
       <c r="H110" t="n">
-        <v>0.22</v>
+        <v>1.11</v>
       </c>
       <c r="I110" t="n">
-        <v>56.85</v>
+        <v>59.49</v>
       </c>
       <c r="J110" t="n">
-        <v>185.93</v>
+        <v>198.74</v>
       </c>
       <c r="K110" t="inlineStr">
         <is>
@@ -4732,28 +4732,28 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>0.86</v>
+        <v>0.16</v>
       </c>
       <c r="C111" t="n">
-        <v>-0.11</v>
+        <v>-0.33</v>
       </c>
       <c r="D111" t="n">
-        <v>2.18</v>
+        <v>3.47</v>
       </c>
       <c r="E111" t="n">
-        <v>15.74</v>
+        <v>14.18</v>
       </c>
       <c r="F111" t="n">
-        <v>6.58</v>
+        <v>8.779999999999999</v>
       </c>
       <c r="G111" t="n">
-        <v>17.54</v>
+        <v>16.39</v>
       </c>
       <c r="H111" t="n">
-        <v>4.98</v>
+        <v>4.89</v>
       </c>
       <c r="I111" t="n">
-        <v>81.09999999999999</v>
+        <v>82.13</v>
       </c>
       <c r="J111" t="inlineStr"/>
       <c r="K111" t="inlineStr">
@@ -4769,25 +4769,25 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>0.99</v>
+        <v>-0.34</v>
       </c>
       <c r="C112" t="n">
-        <v>-0.05</v>
+        <v>-0.79</v>
       </c>
       <c r="D112" t="n">
-        <v>2.99</v>
+        <v>3.86</v>
       </c>
       <c r="E112" t="n">
-        <v>17.1</v>
+        <v>14.98</v>
       </c>
       <c r="F112" t="n">
-        <v>8.949999999999999</v>
+        <v>10.81</v>
       </c>
       <c r="G112" t="n">
-        <v>21.78</v>
+        <v>20.21</v>
       </c>
       <c r="H112" t="n">
-        <v>9.289999999999999</v>
+        <v>8.210000000000001</v>
       </c>
       <c r="I112" t="inlineStr"/>
       <c r="J112" t="inlineStr"/>
@@ -4804,28 +4804,28 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>0.43</v>
+        <v>-1.05</v>
       </c>
       <c r="C113" t="n">
-        <v>-1.04</v>
+        <v>-2.62</v>
       </c>
       <c r="D113" t="n">
-        <v>-2.79</v>
+        <v>-2.56</v>
       </c>
       <c r="E113" t="n">
-        <v>16.78</v>
+        <v>13.73</v>
       </c>
       <c r="F113" t="n">
-        <v>-0.67</v>
+        <v>0.38</v>
       </c>
       <c r="G113" t="n">
-        <v>0.14</v>
+        <v>-1.73</v>
       </c>
       <c r="H113" t="n">
-        <v>-1.91</v>
+        <v>-1.58</v>
       </c>
       <c r="I113" t="n">
-        <v>44.74</v>
+        <v>44.39</v>
       </c>
       <c r="J113" t="inlineStr"/>
       <c r="K113" t="inlineStr">
@@ -4841,31 +4841,31 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>0.6</v>
+        <v>-0.58</v>
       </c>
       <c r="C114" t="n">
-        <v>-0.59</v>
+        <v>-2.1</v>
       </c>
       <c r="D114" t="n">
-        <v>-1.87</v>
+        <v>-0.33</v>
       </c>
       <c r="E114" t="n">
-        <v>25.85</v>
+        <v>22.15</v>
       </c>
       <c r="F114" t="n">
-        <v>0.99</v>
+        <v>4.15</v>
       </c>
       <c r="G114" t="n">
-        <v>8.44</v>
+        <v>5.16</v>
       </c>
       <c r="H114" t="n">
-        <v>6.72</v>
+        <v>6.45</v>
       </c>
       <c r="I114" t="n">
-        <v>101.85</v>
+        <v>101.8</v>
       </c>
       <c r="J114" t="n">
-        <v>174.29</v>
+        <v>182.56</v>
       </c>
       <c r="K114" t="inlineStr">
         <is>
@@ -4880,31 +4880,31 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>0.65</v>
+        <v>-0.04</v>
       </c>
       <c r="C115" t="n">
-        <v>2.04</v>
+        <v>3.77</v>
       </c>
       <c r="D115" t="n">
-        <v>8.970000000000001</v>
+        <v>6.96</v>
       </c>
       <c r="E115" t="n">
-        <v>-13.16</v>
+        <v>-11.62</v>
       </c>
       <c r="F115" t="n">
-        <v>3.07</v>
+        <v>-0.42</v>
       </c>
       <c r="G115" t="n">
-        <v>-5.14</v>
+        <v>-2.88</v>
       </c>
       <c r="H115" t="n">
-        <v>0.44</v>
+        <v>-0.42</v>
       </c>
       <c r="I115" t="n">
-        <v>-12.8</v>
+        <v>-12.79</v>
       </c>
       <c r="J115" t="n">
-        <v>-2.02</v>
+        <v>-3.19</v>
       </c>
       <c r="K115" t="inlineStr">
         <is>
@@ -4919,31 +4919,31 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>0.78</v>
+        <v>-0.2</v>
       </c>
       <c r="C116" t="n">
-        <v>0.98</v>
+        <v>0.87</v>
       </c>
       <c r="D116" t="n">
-        <v>1.52</v>
+        <v>0.87</v>
       </c>
       <c r="E116" t="n">
-        <v>8.34</v>
+        <v>7.07</v>
       </c>
       <c r="F116" t="n">
-        <v>0.91</v>
+        <v>1.01</v>
       </c>
       <c r="G116" t="n">
-        <v>-0.4</v>
+        <v>0.08</v>
       </c>
       <c r="H116" t="n">
-        <v>-2.16</v>
+        <v>-3.06</v>
       </c>
       <c r="I116" t="n">
-        <v>27.97</v>
+        <v>28.26</v>
       </c>
       <c r="J116" t="n">
-        <v>97.31999999999999</v>
+        <v>101.77</v>
       </c>
       <c r="K116" t="inlineStr">
         <is>
@@ -4958,25 +4958,25 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>2.77</v>
+        <v>-0.61</v>
       </c>
       <c r="C117" t="n">
-        <v>3.71</v>
+        <v>3.22</v>
       </c>
       <c r="D117" t="n">
-        <v>-1.27</v>
+        <v>-1.73</v>
       </c>
       <c r="E117" t="n">
-        <v>8.970000000000001</v>
+        <v>5.36</v>
       </c>
       <c r="F117" t="n">
-        <v>-5</v>
+        <v>-3.78</v>
       </c>
       <c r="G117" t="n">
-        <v>-4.03</v>
+        <v>-4.35</v>
       </c>
       <c r="H117" t="n">
-        <v>-41.95</v>
+        <v>-42.47</v>
       </c>
       <c r="I117" t="inlineStr"/>
       <c r="J117" t="inlineStr"/>
@@ -4993,25 +4993,25 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>0.93</v>
+        <v>-0.43</v>
       </c>
       <c r="C118" t="n">
-        <v>0.3</v>
+        <v>-0.53</v>
       </c>
       <c r="D118" t="n">
-        <v>-3.4</v>
+        <v>-2.88</v>
       </c>
       <c r="E118" t="n">
-        <v>1.81</v>
+        <v>0.26</v>
       </c>
       <c r="F118" t="n">
-        <v>-4.76</v>
+        <v>-3.72</v>
       </c>
       <c r="G118" t="n">
-        <v>-7.03</v>
+        <v>-6.91</v>
       </c>
       <c r="H118" t="n">
-        <v>-1.62</v>
+        <v>-2.7</v>
       </c>
       <c r="I118" t="inlineStr"/>
       <c r="J118" t="inlineStr"/>
@@ -5028,31 +5028,31 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>0.33</v>
+        <v>-0.97</v>
       </c>
       <c r="C119" t="n">
-        <v>0.75</v>
+        <v>-0.51</v>
       </c>
       <c r="D119" t="n">
-        <v>-0.89</v>
+        <v>-0.78</v>
       </c>
       <c r="E119" t="n">
-        <v>7.79</v>
+        <v>5.78</v>
       </c>
       <c r="F119" t="n">
-        <v>2.09</v>
+        <v>1.92</v>
       </c>
       <c r="G119" t="n">
-        <v>-1.11</v>
+        <v>-2.3</v>
       </c>
       <c r="H119" t="n">
-        <v>-16.16</v>
+        <v>-17.27</v>
       </c>
       <c r="I119" t="n">
-        <v>-18.71</v>
+        <v>-19.43</v>
       </c>
       <c r="J119" t="n">
-        <v>-17.72</v>
+        <v>-18</v>
       </c>
       <c r="K119" t="inlineStr">
         <is>
@@ -5067,31 +5067,31 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>0.58</v>
+        <v>0</v>
       </c>
       <c r="C120" t="n">
-        <v>0.72</v>
+        <v>0.64</v>
       </c>
       <c r="D120" t="n">
-        <v>-1.28</v>
+        <v>-0.82</v>
       </c>
       <c r="E120" t="n">
-        <v>4.38</v>
+        <v>3.48</v>
       </c>
       <c r="F120" t="n">
-        <v>-3.13</v>
+        <v>-2.61</v>
       </c>
       <c r="G120" t="n">
-        <v>-0.41</v>
+        <v>-0.63</v>
       </c>
       <c r="H120" t="n">
-        <v>-8.58</v>
+        <v>-8.859999999999999</v>
       </c>
       <c r="I120" t="n">
-        <v>-20.17</v>
+        <v>-20.22</v>
       </c>
       <c r="J120" t="n">
-        <v>-23.28</v>
+        <v>-22.73</v>
       </c>
       <c r="K120" t="inlineStr">
         <is>
@@ -5106,31 +5106,31 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>0.35</v>
+        <v>-0.93</v>
       </c>
       <c r="C121" t="n">
-        <v>1.35</v>
+        <v>0.05</v>
       </c>
       <c r="D121" t="n">
-        <v>-0.09</v>
+        <v>-0.28</v>
       </c>
       <c r="E121" t="n">
-        <v>10.32</v>
+        <v>8.08</v>
       </c>
       <c r="F121" t="n">
-        <v>3.9</v>
+        <v>3.63</v>
       </c>
       <c r="G121" t="n">
-        <v>-0.98</v>
+        <v>-1.98</v>
       </c>
       <c r="H121" t="n">
-        <v>-13.44</v>
+        <v>-14.2</v>
       </c>
       <c r="I121" t="n">
-        <v>-4.68</v>
+        <v>-5.51</v>
       </c>
       <c r="J121" t="n">
-        <v>-4.97</v>
+        <v>-6.12</v>
       </c>
       <c r="K121" t="inlineStr">
         <is>
@@ -5145,28 +5145,28 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>-0.07000000000000001</v>
+        <v>0</v>
       </c>
       <c r="C122" t="n">
-        <v>-0.4</v>
+        <v>-0.19</v>
       </c>
       <c r="D122" t="n">
-        <v>0.82</v>
+        <v>1.25</v>
       </c>
       <c r="E122" t="n">
-        <v>1.87</v>
+        <v>2.19</v>
       </c>
       <c r="F122" t="n">
-        <v>0.63</v>
+        <v>1.46</v>
       </c>
       <c r="G122" t="n">
-        <v>0.61</v>
+        <v>1.04</v>
       </c>
       <c r="H122" t="n">
-        <v>-0.87</v>
+        <v>-0.41</v>
       </c>
       <c r="I122" t="n">
-        <v>0.19</v>
+        <v>0.28</v>
       </c>
       <c r="J122" t="inlineStr"/>
       <c r="K122" t="inlineStr">
@@ -5182,31 +5182,31 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>-0.08</v>
+        <v>-0.46</v>
       </c>
       <c r="C123" t="n">
-        <v>-0.27</v>
+        <v>-0.8</v>
       </c>
       <c r="D123" t="n">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="E123" t="n">
-        <v>6.24</v>
+        <v>4.74</v>
       </c>
       <c r="F123" t="n">
-        <v>3.54</v>
+        <v>3.67</v>
       </c>
       <c r="G123" t="n">
-        <v>0.86</v>
+        <v>-0.03</v>
       </c>
       <c r="H123" t="n">
-        <v>-8.630000000000001</v>
+        <v>-9.050000000000001</v>
       </c>
       <c r="I123" t="n">
-        <v>-8.57</v>
+        <v>-8.859999999999999</v>
       </c>
       <c r="J123" t="n">
-        <v>-16.98</v>
+        <v>-16.57</v>
       </c>
       <c r="K123" t="inlineStr">
         <is>
@@ -5221,28 +5221,28 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>0.09</v>
+        <v>0</v>
       </c>
       <c r="C124" t="n">
-        <v>-0.42</v>
+        <v>-0.22</v>
       </c>
       <c r="D124" t="n">
-        <v>0.77</v>
+        <v>0.9</v>
       </c>
       <c r="E124" t="n">
         <v>2.54</v>
       </c>
       <c r="F124" t="n">
-        <v>0.76</v>
+        <v>1.89</v>
       </c>
       <c r="G124" t="n">
-        <v>0.25</v>
+        <v>0.53</v>
       </c>
       <c r="H124" t="n">
-        <v>-2.77</v>
+        <v>-2.23</v>
       </c>
       <c r="I124" t="n">
-        <v>-4.81</v>
+        <v>-4.61</v>
       </c>
       <c r="J124" t="inlineStr"/>
       <c r="K124" t="inlineStr">

</xml_diff>

<commit_message>
RSI and MACD finished. la tabla esta lista según pedido inicial
</commit_message>
<xml_diff>
--- a/stocksPercentage.xlsx
+++ b/stocksPercentage.xlsx
@@ -497,31 +497,31 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.38</v>
+        <v>0.4</v>
       </c>
       <c r="D2" t="n">
-        <v>2.07</v>
+        <v>1.93</v>
       </c>
       <c r="E2" t="n">
-        <v>-6.71</v>
+        <v>-5.74</v>
       </c>
       <c r="F2" t="n">
-        <v>-1.99</v>
+        <v>-1.24</v>
       </c>
       <c r="G2" t="n">
-        <v>1.66</v>
+        <v>-0.04</v>
       </c>
       <c r="H2" t="n">
-        <v>8.5</v>
+        <v>9.35</v>
       </c>
       <c r="I2" t="n">
-        <v>9.82</v>
+        <v>9.44</v>
       </c>
       <c r="J2" t="n">
-        <v>28.14</v>
+        <v>28.46</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
@@ -539,28 +539,28 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5</v>
+        <v>-0.39</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.71</v>
+        <v>-1.37</v>
       </c>
       <c r="E3" t="n">
-        <v>-1.41</v>
+        <v>-3.17</v>
       </c>
       <c r="F3" t="n">
-        <v>-4.12</v>
+        <v>-5.51</v>
       </c>
       <c r="G3" t="n">
-        <v>-3.66</v>
+        <v>-2.81</v>
       </c>
       <c r="H3" t="n">
-        <v>-9.970000000000001</v>
+        <v>-11.24</v>
       </c>
       <c r="I3" t="n">
-        <v>-13.97</v>
+        <v>-14.2</v>
       </c>
       <c r="J3" t="n">
-        <v>-32.06</v>
+        <v>-32.71</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
@@ -578,28 +578,28 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.91</v>
+        <v>-0.51</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.45</v>
+        <v>-1.62</v>
       </c>
       <c r="E4" t="n">
-        <v>0.91</v>
+        <v>-1.35</v>
       </c>
       <c r="F4" t="n">
-        <v>0.28</v>
+        <v>-0.62</v>
       </c>
       <c r="G4" t="n">
-        <v>1.19</v>
+        <v>2.21</v>
       </c>
       <c r="H4" t="n">
-        <v>1.83</v>
+        <v>0.86</v>
       </c>
       <c r="I4" t="n">
-        <v>-4.46</v>
+        <v>-5.73</v>
       </c>
       <c r="J4" t="n">
-        <v>-8.199999999999999</v>
+        <v>-10.3</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
@@ -617,28 +617,28 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7</v>
+        <v>0.02</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.71</v>
+        <v>-0.83</v>
       </c>
       <c r="E5" t="n">
-        <v>-2.13</v>
+        <v>-2.99</v>
       </c>
       <c r="F5" t="n">
-        <v>-1.07</v>
+        <v>-2.18</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.37</v>
+        <v>1.96</v>
       </c>
       <c r="H5" t="n">
-        <v>2.84</v>
+        <v>1.83</v>
       </c>
       <c r="I5" t="n">
-        <v>32.78</v>
+        <v>31.7</v>
       </c>
       <c r="J5" t="n">
-        <v>21.98</v>
+        <v>20.17</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
@@ -653,31 +653,31 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-1.23</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.14</v>
+        <v>0.08</v>
       </c>
       <c r="D6" t="n">
-        <v>-1.39</v>
+        <v>-0.39</v>
       </c>
       <c r="E6" t="n">
-        <v>2.14</v>
+        <v>2.87</v>
       </c>
       <c r="F6" t="n">
-        <v>4.71</v>
+        <v>4.67</v>
       </c>
       <c r="G6" t="n">
-        <v>5.71</v>
+        <v>8.51</v>
       </c>
       <c r="H6" t="n">
-        <v>11.38</v>
+        <v>11.7</v>
       </c>
       <c r="I6" t="n">
-        <v>51.05</v>
+        <v>51.76</v>
       </c>
       <c r="J6" t="n">
-        <v>55.01</v>
+        <v>55.5</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
@@ -692,31 +692,31 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-2.92</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>-2.92</v>
+        <v>-0.77</v>
       </c>
       <c r="D7" t="n">
-        <v>-4.9</v>
+        <v>-2.17</v>
       </c>
       <c r="E7" t="n">
-        <v>-1.34</v>
+        <v>-1.57</v>
       </c>
       <c r="F7" t="n">
-        <v>-5.33</v>
+        <v>-4.2</v>
       </c>
       <c r="G7" t="n">
-        <v>-4.54</v>
+        <v>1.32</v>
       </c>
       <c r="H7" t="n">
-        <v>-1.62</v>
+        <v>-0.19</v>
       </c>
       <c r="I7" t="n">
-        <v>38</v>
+        <v>39.54</v>
       </c>
       <c r="J7" t="n">
-        <v>10.64</v>
+        <v>8.81</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
@@ -731,31 +731,31 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-1.44</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>-3.18</v>
+        <v>-2.56</v>
       </c>
       <c r="D8" t="n">
-        <v>-8.130000000000001</v>
+        <v>-7.35</v>
       </c>
       <c r="E8" t="n">
-        <v>-2.44</v>
+        <v>-1.64</v>
       </c>
       <c r="F8" t="n">
-        <v>-2.61</v>
+        <v>-3.44</v>
       </c>
       <c r="G8" t="n">
-        <v>-12.23</v>
+        <v>-8.550000000000001</v>
       </c>
       <c r="H8" t="n">
-        <v>-13.8</v>
+        <v>-13.98</v>
       </c>
       <c r="I8" t="n">
-        <v>6.12</v>
+        <v>5.79</v>
       </c>
       <c r="J8" t="n">
-        <v>-38.5</v>
+        <v>-39.01</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
@@ -773,28 +773,28 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>-2.99</v>
+        <v>-3.46</v>
       </c>
       <c r="D9" t="n">
-        <v>2.5</v>
+        <v>-2.03</v>
       </c>
       <c r="E9" t="n">
-        <v>-14.14</v>
+        <v>-14.2</v>
       </c>
       <c r="F9" t="n">
-        <v>-10.98</v>
+        <v>-14.16</v>
       </c>
       <c r="G9" t="n">
-        <v>-7.04</v>
+        <v>-6.54</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.67</v>
+        <v>-3.41</v>
       </c>
       <c r="I9" t="n">
-        <v>40.07</v>
+        <v>39.91</v>
       </c>
       <c r="J9" t="n">
-        <v>-30.81</v>
+        <v>-32.21</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
@@ -809,31 +809,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-1.15</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>-4.51</v>
+        <v>-3.59</v>
       </c>
       <c r="D10" t="n">
-        <v>1.57</v>
+        <v>-1.76</v>
       </c>
       <c r="E10" t="n">
-        <v>-16.45</v>
+        <v>-15.44</v>
       </c>
       <c r="F10" t="n">
-        <v>-11.16</v>
+        <v>-14.19</v>
       </c>
       <c r="G10" t="n">
-        <v>-4.05</v>
+        <v>-3.25</v>
       </c>
       <c r="H10" t="n">
-        <v>-7.41</v>
+        <v>-10.39</v>
       </c>
       <c r="I10" t="n">
-        <v>38.16</v>
+        <v>40.97</v>
       </c>
       <c r="J10" t="n">
-        <v>-47.45</v>
+        <v>-48.22</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
@@ -848,31 +848,31 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.26</v>
+        <v>-1.38</v>
       </c>
       <c r="D11" t="n">
-        <v>-8.09</v>
+        <v>-17.12</v>
       </c>
       <c r="E11" t="n">
-        <v>-34.57</v>
+        <v>-29.03</v>
       </c>
       <c r="F11" t="n">
-        <v>-28.49</v>
+        <v>-30.36</v>
       </c>
       <c r="G11" t="n">
-        <v>-43.08</v>
+        <v>-43.06</v>
       </c>
       <c r="H11" t="n">
-        <v>-74.87</v>
+        <v>-69.44</v>
       </c>
       <c r="I11" t="n">
-        <v>-80.47</v>
+        <v>-79.8</v>
       </c>
       <c r="J11" t="n">
-        <v>-95.09</v>
+        <v>-95.22</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
@@ -890,28 +890,28 @@
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>-1.58</v>
+        <v>-2.03</v>
       </c>
       <c r="D12" t="n">
-        <v>-2.84</v>
+        <v>-1.08</v>
       </c>
       <c r="E12" t="n">
-        <v>-5.41</v>
+        <v>-7.5</v>
       </c>
       <c r="F12" t="n">
-        <v>-6.13</v>
+        <v>-7.01</v>
       </c>
       <c r="G12" t="n">
-        <v>-18.71</v>
+        <v>-16.39</v>
       </c>
       <c r="H12" t="n">
-        <v>-24.37</v>
+        <v>-25.52</v>
       </c>
       <c r="I12" t="n">
-        <v>7.11</v>
+        <v>5.52</v>
       </c>
       <c r="J12" t="n">
-        <v>10.92</v>
+        <v>9.369999999999999</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
@@ -926,31 +926,31 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0.51</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>-1.3</v>
+        <v>-1.65</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.51</v>
+        <v>0.59</v>
       </c>
       <c r="E13" t="n">
-        <v>3.82</v>
+        <v>2.81</v>
       </c>
       <c r="F13" t="n">
-        <v>0.28</v>
+        <v>-0.42</v>
       </c>
       <c r="G13" t="n">
-        <v>-4</v>
+        <v>-3.02</v>
       </c>
       <c r="H13" t="n">
-        <v>-12.79</v>
+        <v>-13.33</v>
       </c>
       <c r="I13" t="n">
-        <v>37.57</v>
+        <v>34.86</v>
       </c>
       <c r="J13" t="n">
-        <v>11.55</v>
+        <v>11.38</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
@@ -965,31 +965,31 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-1.97</v>
+        <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>-4.24</v>
+        <v>-3.41</v>
       </c>
       <c r="D14" t="n">
-        <v>-12.82</v>
+        <v>-8.039999999999999</v>
       </c>
       <c r="E14" t="n">
-        <v>-15.25</v>
+        <v>-14.83</v>
       </c>
       <c r="F14" t="n">
-        <v>-24.33</v>
+        <v>-25.1</v>
       </c>
       <c r="G14" t="n">
-        <v>-43.28</v>
+        <v>-41.43</v>
       </c>
       <c r="H14" t="n">
-        <v>-60.53</v>
+        <v>-59.06</v>
       </c>
       <c r="I14" t="n">
-        <v>-31.84</v>
+        <v>-33.53</v>
       </c>
       <c r="J14" t="n">
-        <v>27.19</v>
+        <v>25.81</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
@@ -1004,31 +1004,31 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>1.78</v>
+        <v>0.32</v>
       </c>
       <c r="D15" t="n">
-        <v>5.03</v>
+        <v>5.44</v>
       </c>
       <c r="E15" t="n">
-        <v>-2.29</v>
+        <v>-3.38</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.28</v>
+        <v>0.28</v>
       </c>
       <c r="G15" t="n">
-        <v>7.73</v>
+        <v>8.449999999999999</v>
       </c>
       <c r="H15" t="n">
-        <v>6.42</v>
+        <v>5.39</v>
       </c>
       <c r="I15" t="n">
-        <v>28.35</v>
+        <v>27.12</v>
       </c>
       <c r="J15" t="n">
-        <v>-12.94</v>
+        <v>-14.47</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
@@ -1058,16 +1058,16 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>29.01</v>
+        <v>29.42</v>
       </c>
       <c r="H16" t="n">
-        <v>20.35</v>
+        <v>17.79</v>
       </c>
       <c r="I16" t="n">
-        <v>45.92</v>
+        <v>41.59</v>
       </c>
       <c r="J16" t="n">
-        <v>-6.18</v>
+        <v>-5.07</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
@@ -1082,31 +1082,31 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1.23</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>1.59</v>
+        <v>0.7</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.86</v>
+        <v>-2.72</v>
       </c>
       <c r="E17" t="n">
-        <v>0.88</v>
+        <v>-1.21</v>
       </c>
       <c r="F17" t="n">
-        <v>-11.52</v>
+        <v>-12.14</v>
       </c>
       <c r="G17" t="n">
-        <v>-25.29</v>
+        <v>-25.13</v>
       </c>
       <c r="H17" t="n">
-        <v>-20.77</v>
+        <v>-22.49</v>
       </c>
       <c r="I17" t="n">
-        <v>-5.42</v>
+        <v>-6.23</v>
       </c>
       <c r="J17" t="n">
-        <v>-57.46</v>
+        <v>-60.28</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
@@ -1124,28 +1124,28 @@
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>0.14</v>
+        <v>-0.14</v>
       </c>
       <c r="D18" t="n">
-        <v>9.84</v>
+        <v>10.33</v>
       </c>
       <c r="E18" t="n">
-        <v>-9.800000000000001</v>
+        <v>-10.34</v>
       </c>
       <c r="F18" t="n">
-        <v>2.38</v>
+        <v>5.71</v>
       </c>
       <c r="G18" t="n">
-        <v>32.17</v>
+        <v>38.8</v>
       </c>
       <c r="H18" t="n">
-        <v>56.61</v>
+        <v>56.48</v>
       </c>
       <c r="I18" t="n">
-        <v>84.15000000000001</v>
+        <v>84.56999999999999</v>
       </c>
       <c r="J18" t="n">
-        <v>1.1</v>
+        <v>-0.57</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
@@ -1175,13 +1175,13 @@
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>5.63</v>
+        <v>6.24</v>
       </c>
       <c r="H19" t="n">
-        <v>-16.73</v>
+        <v>-18.17</v>
       </c>
       <c r="I19" t="n">
-        <v>41.14</v>
+        <v>39.68</v>
       </c>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr">
@@ -1200,28 +1200,28 @@
         <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>1.29</v>
+        <v>-0.83</v>
       </c>
       <c r="D20" t="n">
-        <v>-4.08</v>
+        <v>-4.1</v>
       </c>
       <c r="E20" t="n">
-        <v>-6.79</v>
+        <v>-8.619999999999999</v>
       </c>
       <c r="F20" t="n">
+        <v>-10.47</v>
+      </c>
+      <c r="G20" t="n">
+        <v>-23.63</v>
+      </c>
+      <c r="H20" t="n">
         <v>-9.75</v>
       </c>
-      <c r="G20" t="n">
-        <v>-22.76</v>
-      </c>
-      <c r="H20" t="n">
-        <v>-9.23</v>
-      </c>
       <c r="I20" t="n">
-        <v>25.99</v>
+        <v>24.68</v>
       </c>
       <c r="J20" t="n">
-        <v>-34.06</v>
+        <v>-35.39</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
@@ -1239,28 +1239,28 @@
         <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>0.59</v>
+        <v>-2.6</v>
       </c>
       <c r="D21" t="n">
-        <v>-4.37</v>
+        <v>-4.28</v>
       </c>
       <c r="E21" t="n">
-        <v>-8.6</v>
+        <v>-11.95</v>
       </c>
       <c r="F21" t="n">
-        <v>-7.34</v>
+        <v>-10.11</v>
       </c>
       <c r="G21" t="n">
-        <v>-9.93</v>
+        <v>-10.69</v>
       </c>
       <c r="H21" t="n">
-        <v>-0.98</v>
+        <v>-2.83</v>
       </c>
       <c r="I21" t="n">
-        <v>52.95</v>
+        <v>50.51</v>
       </c>
       <c r="J21" t="n">
-        <v>11.95</v>
+        <v>9.529999999999999</v>
       </c>
       <c r="K21" t="inlineStr">
         <is>
@@ -1290,13 +1290,13 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.92</v>
+        <v>2.63</v>
       </c>
       <c r="H22" t="n">
-        <v>-14.63</v>
+        <v>-14.99</v>
       </c>
       <c r="I22" t="n">
-        <v>35.18</v>
+        <v>35.79</v>
       </c>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr">
@@ -1327,13 +1327,13 @@
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>1.46</v>
+        <v>2.56</v>
       </c>
       <c r="H23" t="n">
-        <v>0.05</v>
+        <v>-0.67</v>
       </c>
       <c r="I23" t="n">
-        <v>-17.25</v>
+        <v>-18.51</v>
       </c>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr">
@@ -1349,31 +1349,31 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.11</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.32</v>
+        <v>2.38</v>
       </c>
       <c r="D24" t="n">
-        <v>3.61</v>
+        <v>5.65</v>
       </c>
       <c r="E24" t="n">
-        <v>13.69</v>
+        <v>13.46</v>
       </c>
       <c r="F24" t="n">
-        <v>8.800000000000001</v>
+        <v>10.64</v>
       </c>
       <c r="G24" t="n">
-        <v>17.5</v>
+        <v>20.62</v>
       </c>
       <c r="H24" t="n">
-        <v>7.08</v>
+        <v>10.17</v>
       </c>
       <c r="I24" t="n">
-        <v>81.34</v>
+        <v>81.01000000000001</v>
       </c>
       <c r="J24" t="n">
-        <v>181.17</v>
+        <v>182.21</v>
       </c>
       <c r="K24" t="inlineStr">
         <is>
@@ -1388,31 +1388,31 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-0.7</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.97</v>
+        <v>0.11</v>
       </c>
       <c r="D25" t="n">
-        <v>0.12</v>
+        <v>0.05</v>
       </c>
       <c r="E25" t="n">
-        <v>9.050000000000001</v>
+        <v>8.210000000000001</v>
       </c>
       <c r="F25" t="n">
-        <v>4.11</v>
+        <v>4.51</v>
       </c>
       <c r="G25" t="n">
-        <v>1.72</v>
+        <v>3.59</v>
       </c>
       <c r="H25" t="n">
-        <v>-6.42</v>
+        <v>-5.21</v>
       </c>
       <c r="I25" t="n">
-        <v>33.97</v>
+        <v>33</v>
       </c>
       <c r="J25" t="n">
-        <v>31.83</v>
+        <v>31.09</v>
       </c>
       <c r="K25" t="inlineStr">
         <is>
@@ -1430,28 +1430,28 @@
         <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>0.33</v>
+        <v>-0.14</v>
       </c>
       <c r="D26" t="n">
-        <v>0.37</v>
+        <v>-1.31</v>
       </c>
       <c r="E26" t="n">
-        <v>8.09</v>
+        <v>4.6</v>
       </c>
       <c r="F26" t="n">
-        <v>3.99</v>
+        <v>2.27</v>
       </c>
       <c r="G26" t="n">
-        <v>0.47</v>
+        <v>2.27</v>
       </c>
       <c r="H26" t="n">
-        <v>-17.62</v>
+        <v>-19.09</v>
       </c>
       <c r="I26" t="n">
-        <v>6.74</v>
+        <v>5.22</v>
       </c>
       <c r="J26" t="n">
-        <v>10.72</v>
+        <v>8.18</v>
       </c>
       <c r="K26" t="inlineStr">
         <is>
@@ -1466,31 +1466,31 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>-0.38</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
         <v>-0.55</v>
       </c>
       <c r="D27" t="n">
-        <v>-2.58</v>
+        <v>-3.32</v>
       </c>
       <c r="E27" t="n">
-        <v>4.85</v>
+        <v>3.03</v>
       </c>
       <c r="F27" t="n">
-        <v>-2.05</v>
+        <v>-2.91</v>
       </c>
       <c r="G27" t="n">
-        <v>-4.77</v>
+        <v>-3.38</v>
       </c>
       <c r="H27" t="n">
-        <v>-13.12</v>
+        <v>-12.31</v>
       </c>
       <c r="I27" t="n">
-        <v>2.31</v>
+        <v>0.67</v>
       </c>
       <c r="J27" t="n">
-        <v>17.7</v>
+        <v>15.43</v>
       </c>
       <c r="K27" t="inlineStr">
         <is>
@@ -1508,28 +1508,28 @@
         <v>0</v>
       </c>
       <c r="C28" t="n">
-        <v>2.14</v>
+        <v>-0.03</v>
       </c>
       <c r="D28" t="n">
-        <v>4.46</v>
+        <v>1.81</v>
       </c>
       <c r="E28" t="n">
-        <v>16.38</v>
+        <v>14.67</v>
       </c>
       <c r="F28" t="n">
-        <v>11.5</v>
+        <v>10.5</v>
       </c>
       <c r="G28" t="n">
-        <v>14.74</v>
+        <v>13.5</v>
       </c>
       <c r="H28" t="n">
-        <v>12.1</v>
+        <v>14.82</v>
       </c>
       <c r="I28" t="n">
-        <v>93.88</v>
+        <v>88.33</v>
       </c>
       <c r="J28" t="n">
-        <v>157.75</v>
+        <v>150.33</v>
       </c>
       <c r="K28" t="inlineStr">
         <is>
@@ -1547,28 +1547,28 @@
         <v>0</v>
       </c>
       <c r="C29" t="n">
-        <v>-1.4</v>
+        <v>-0.8</v>
       </c>
       <c r="D29" t="n">
-        <v>-1.38</v>
+        <v>-2.87</v>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>5.93</v>
       </c>
       <c r="F29" t="n">
-        <v>2.51</v>
+        <v>2.11</v>
       </c>
       <c r="G29" t="n">
-        <v>-11.86</v>
+        <v>-10.3</v>
       </c>
       <c r="H29" t="n">
-        <v>-23.67</v>
+        <v>-23.21</v>
       </c>
       <c r="I29" t="n">
-        <v>-7.68</v>
+        <v>-9.93</v>
       </c>
       <c r="J29" t="n">
-        <v>10.59</v>
+        <v>7.77</v>
       </c>
       <c r="K29" t="inlineStr">
         <is>
@@ -1583,31 +1583,31 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-0.85</v>
+        <v>0</v>
       </c>
       <c r="C30" t="n">
-        <v>-1.23</v>
+        <v>-0.44</v>
       </c>
       <c r="D30" t="n">
-        <v>0.05</v>
+        <v>1.37</v>
       </c>
       <c r="E30" t="n">
-        <v>8.76</v>
+        <v>8.92</v>
       </c>
       <c r="F30" t="n">
-        <v>1.85</v>
+        <v>1.39</v>
       </c>
       <c r="G30" t="n">
-        <v>3.29</v>
+        <v>5.46</v>
       </c>
       <c r="H30" t="n">
-        <v>0.13</v>
+        <v>0.99</v>
       </c>
       <c r="I30" t="n">
-        <v>36.74</v>
+        <v>35.44</v>
       </c>
       <c r="J30" t="n">
-        <v>46.27</v>
+        <v>43.92</v>
       </c>
       <c r="K30" t="inlineStr">
         <is>
@@ -1622,31 +1622,31 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-0.71</v>
+        <v>0</v>
       </c>
       <c r="C31" t="n">
-        <v>-0.58</v>
+        <v>0.55</v>
       </c>
       <c r="D31" t="n">
-        <v>-0.17</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="E31" t="n">
-        <v>13.05</v>
+        <v>12.16</v>
       </c>
       <c r="F31" t="n">
-        <v>3.43</v>
+        <v>3.54</v>
       </c>
       <c r="G31" t="n">
-        <v>1.45</v>
+        <v>4.1</v>
       </c>
       <c r="H31" t="n">
-        <v>-9.49</v>
+        <v>-8.6</v>
       </c>
       <c r="I31" t="n">
-        <v>9.25</v>
+        <v>7.66</v>
       </c>
       <c r="J31" t="n">
-        <v>-0.17</v>
+        <v>-1.05</v>
       </c>
       <c r="K31" t="inlineStr">
         <is>
@@ -1664,28 +1664,28 @@
         <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>2.44</v>
+        <v>1.39</v>
       </c>
       <c r="D32" t="n">
-        <v>6.58</v>
+        <v>5.9</v>
       </c>
       <c r="E32" t="n">
-        <v>14.01</v>
+        <v>11.05</v>
       </c>
       <c r="F32" t="n">
-        <v>4.19</v>
+        <v>2.49</v>
       </c>
       <c r="G32" t="n">
-        <v>29.38</v>
+        <v>30.66</v>
       </c>
       <c r="H32" t="n">
-        <v>36.96</v>
+        <v>35.74</v>
       </c>
       <c r="I32" t="n">
-        <v>80.3</v>
+        <v>77.20999999999999</v>
       </c>
       <c r="J32" t="n">
-        <v>-39.32</v>
+        <v>-42.15</v>
       </c>
       <c r="K32" t="inlineStr">
         <is>
@@ -1703,28 +1703,28 @@
         <v>0</v>
       </c>
       <c r="C33" t="n">
-        <v>-0</v>
+        <v>0.77</v>
       </c>
       <c r="D33" t="n">
-        <v>4.64</v>
+        <v>5.48</v>
       </c>
       <c r="E33" t="n">
-        <v>16.86</v>
+        <v>14.99</v>
       </c>
       <c r="F33" t="n">
-        <v>7.37</v>
+        <v>5.61</v>
       </c>
       <c r="G33" t="n">
-        <v>16.58</v>
+        <v>19.6</v>
       </c>
       <c r="H33" t="n">
-        <v>10.58</v>
+        <v>12.38</v>
       </c>
       <c r="I33" t="n">
-        <v>55.66</v>
+        <v>54.57</v>
       </c>
       <c r="J33" t="n">
-        <v>76.09</v>
+        <v>74.28</v>
       </c>
       <c r="K33" t="inlineStr">
         <is>
@@ -1739,31 +1739,31 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="C34" t="n">
-        <v>1.5</v>
+        <v>0.42</v>
       </c>
       <c r="D34" t="n">
-        <v>0.15</v>
+        <v>0.06</v>
       </c>
       <c r="E34" t="n">
-        <v>9.16</v>
+        <v>7.79</v>
       </c>
       <c r="F34" t="n">
-        <v>3.88</v>
+        <v>4.67</v>
       </c>
       <c r="G34" t="n">
-        <v>10.15</v>
+        <v>11.91</v>
       </c>
       <c r="H34" t="n">
-        <v>1.84</v>
+        <v>2.84</v>
       </c>
       <c r="I34" t="n">
-        <v>29.97</v>
+        <v>28.02</v>
       </c>
       <c r="J34" t="n">
-        <v>12.17</v>
+        <v>9.26</v>
       </c>
       <c r="K34" t="inlineStr">
         <is>
@@ -1778,31 +1778,31 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>-0.87</v>
+        <v>0</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.89</v>
+        <v>0.61</v>
       </c>
       <c r="D35" t="n">
-        <v>4.99</v>
+        <v>6.83</v>
       </c>
       <c r="E35" t="n">
-        <v>18.15</v>
+        <v>16.86</v>
       </c>
       <c r="F35" t="n">
-        <v>5.47</v>
+        <v>5.75</v>
       </c>
       <c r="G35" t="n">
-        <v>5.01</v>
+        <v>9.02</v>
       </c>
       <c r="H35" t="n">
-        <v>-3.01</v>
+        <v>-0.74</v>
       </c>
       <c r="I35" t="n">
-        <v>60.65</v>
+        <v>58.71</v>
       </c>
       <c r="J35" t="n">
-        <v>90.22</v>
+        <v>88.40000000000001</v>
       </c>
       <c r="K35" t="inlineStr">
         <is>
@@ -1820,28 +1820,28 @@
         <v>0</v>
       </c>
       <c r="C36" t="n">
-        <v>-1.21</v>
+        <v>-0.86</v>
       </c>
       <c r="D36" t="n">
-        <v>-2.33</v>
+        <v>-5.4</v>
       </c>
       <c r="E36" t="n">
-        <v>3.52</v>
+        <v>1.46</v>
       </c>
       <c r="F36" t="n">
-        <v>0.14</v>
+        <v>-3.53</v>
       </c>
       <c r="G36" t="n">
-        <v>-4.21</v>
+        <v>-3.74</v>
       </c>
       <c r="H36" t="n">
-        <v>-20.3</v>
+        <v>-21.23</v>
       </c>
       <c r="I36" t="n">
-        <v>-6.1</v>
+        <v>-9.039999999999999</v>
       </c>
       <c r="J36" t="n">
-        <v>-18.46</v>
+        <v>-21.55</v>
       </c>
       <c r="K36" t="inlineStr">
         <is>
@@ -1862,25 +1862,25 @@
         <v>0.1</v>
       </c>
       <c r="D37" t="n">
-        <v>-2.64</v>
+        <v>-2.92</v>
       </c>
       <c r="E37" t="n">
-        <v>3.41</v>
+        <v>1.78</v>
       </c>
       <c r="F37" t="n">
-        <v>1.48</v>
+        <v>1.28</v>
       </c>
       <c r="G37" t="n">
-        <v>-2.74</v>
+        <v>-0.67</v>
       </c>
       <c r="H37" t="n">
-        <v>-2.37</v>
+        <v>-3.1</v>
       </c>
       <c r="I37" t="n">
-        <v>-4.36</v>
+        <v>-4.63</v>
       </c>
       <c r="J37" t="n">
-        <v>-33.66</v>
+        <v>-35.03</v>
       </c>
       <c r="K37" t="inlineStr">
         <is>
@@ -1895,31 +1895,31 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>-0.3</v>
+        <v>0</v>
       </c>
       <c r="C38" t="n">
-        <v>1.64</v>
+        <v>0.51</v>
       </c>
       <c r="D38" t="n">
-        <v>-2.66</v>
+        <v>-2.88</v>
       </c>
       <c r="E38" t="n">
-        <v>7.26</v>
+        <v>7.11</v>
       </c>
       <c r="F38" t="n">
-        <v>5.36</v>
+        <v>4.76</v>
       </c>
       <c r="G38" t="n">
-        <v>7.34</v>
+        <v>9.960000000000001</v>
       </c>
       <c r="H38" t="n">
-        <v>10.54</v>
+        <v>10.29</v>
       </c>
       <c r="I38" t="n">
-        <v>4.69</v>
+        <v>4.14</v>
       </c>
       <c r="J38" t="n">
-        <v>-19.52</v>
+        <v>-21.08</v>
       </c>
       <c r="K38" t="inlineStr">
         <is>
@@ -1937,28 +1937,28 @@
         <v>0</v>
       </c>
       <c r="C39" t="n">
-        <v>1.36</v>
+        <v>0.4</v>
       </c>
       <c r="D39" t="n">
-        <v>-2.04</v>
+        <v>-0.45</v>
       </c>
       <c r="E39" t="n">
-        <v>17.78</v>
+        <v>14.26</v>
       </c>
       <c r="F39" t="n">
-        <v>9.539999999999999</v>
+        <v>8.01</v>
       </c>
       <c r="G39" t="n">
-        <v>3.19</v>
+        <v>5.87</v>
       </c>
       <c r="H39" t="n">
-        <v>-12.45</v>
+        <v>-11.37</v>
       </c>
       <c r="I39" t="n">
-        <v>26.85</v>
+        <v>24.72</v>
       </c>
       <c r="J39" t="n">
-        <v>13.65</v>
+        <v>9.84</v>
       </c>
       <c r="K39" t="inlineStr">
         <is>
@@ -1973,31 +1973,31 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>-0.79</v>
+        <v>0</v>
       </c>
       <c r="C40" t="n">
-        <v>-1.64</v>
+        <v>-0.38</v>
       </c>
       <c r="D40" t="n">
-        <v>-0.98</v>
+        <v>-0.78</v>
       </c>
       <c r="E40" t="n">
-        <v>10.32</v>
+        <v>9.789999999999999</v>
       </c>
       <c r="F40" t="n">
-        <v>1.43</v>
+        <v>1.74</v>
       </c>
       <c r="G40" t="n">
-        <v>4.9</v>
+        <v>5.62</v>
       </c>
       <c r="H40" t="n">
-        <v>-5.1</v>
+        <v>-3.15</v>
       </c>
       <c r="I40" t="n">
-        <v>43.06</v>
+        <v>40.86</v>
       </c>
       <c r="J40" t="n">
-        <v>50.35</v>
+        <v>48.28</v>
       </c>
       <c r="K40" t="inlineStr">
         <is>
@@ -2012,31 +2012,31 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>-0.79</v>
+        <v>0</v>
       </c>
       <c r="C41" t="n">
-        <v>-0.55</v>
+        <v>0.09</v>
       </c>
       <c r="D41" t="n">
-        <v>-0.67</v>
+        <v>-1.1</v>
       </c>
       <c r="E41" t="n">
-        <v>4.2</v>
+        <v>3.44</v>
       </c>
       <c r="F41" t="n">
-        <v>0.43</v>
+        <v>0.34</v>
       </c>
       <c r="G41" t="n">
-        <v>0.46</v>
+        <v>1.66</v>
       </c>
       <c r="H41" t="n">
-        <v>-5.98</v>
+        <v>-4.95</v>
       </c>
       <c r="I41" t="n">
-        <v>2.91</v>
+        <v>1.53</v>
       </c>
       <c r="J41" t="n">
-        <v>-16.49</v>
+        <v>-17.74</v>
       </c>
       <c r="K41" t="inlineStr">
         <is>
@@ -2051,31 +2051,31 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>-0.66</v>
+        <v>0</v>
       </c>
       <c r="C42" t="n">
-        <v>-2.21</v>
+        <v>0.46</v>
       </c>
       <c r="D42" t="n">
-        <v>-0.1</v>
+        <v>1.34</v>
       </c>
       <c r="E42" t="n">
-        <v>20.51</v>
+        <v>18</v>
       </c>
       <c r="F42" t="n">
-        <v>3.8</v>
+        <v>4.21</v>
       </c>
       <c r="G42" t="n">
-        <v>-4.29</v>
+        <v>0.22</v>
       </c>
       <c r="H42" t="n">
-        <v>-21.32</v>
+        <v>-19.47</v>
       </c>
       <c r="I42" t="n">
-        <v>8.67</v>
+        <v>7.99</v>
       </c>
       <c r="J42" t="n">
-        <v>25.26</v>
+        <v>23.03</v>
       </c>
       <c r="K42" t="inlineStr">
         <is>
@@ -2090,31 +2090,31 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>-0.36</v>
+        <v>0</v>
       </c>
       <c r="C43" t="n">
-        <v>-0.86</v>
+        <v>-0.08</v>
       </c>
       <c r="D43" t="n">
-        <v>-2.05</v>
+        <v>-0.84</v>
       </c>
       <c r="E43" t="n">
-        <v>9.77</v>
+        <v>8.66</v>
       </c>
       <c r="F43" t="n">
-        <v>5.89</v>
+        <v>5.03</v>
       </c>
       <c r="G43" t="n">
-        <v>-5.15</v>
+        <v>-2.88</v>
       </c>
       <c r="H43" t="n">
-        <v>1.61</v>
+        <v>2.12</v>
       </c>
       <c r="I43" t="n">
-        <v>15.05</v>
+        <v>12.01</v>
       </c>
       <c r="J43" t="n">
-        <v>4.25</v>
+        <v>2.34</v>
       </c>
       <c r="K43" t="inlineStr">
         <is>
@@ -2129,31 +2129,31 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>-1.58</v>
+        <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>-3.34</v>
+        <v>-0.38</v>
       </c>
       <c r="D44" t="n">
-        <v>-7.74</v>
+        <v>-6.3</v>
       </c>
       <c r="E44" t="n">
-        <v>-8.81</v>
+        <v>-11.25</v>
       </c>
       <c r="F44" t="n">
-        <v>-19.32</v>
+        <v>-18.26</v>
       </c>
       <c r="G44" t="n">
-        <v>-29.06</v>
+        <v>-28.02</v>
       </c>
       <c r="H44" t="n">
-        <v>-34.53</v>
+        <v>-35.11</v>
       </c>
       <c r="I44" t="n">
-        <v>-36.01</v>
+        <v>-37.54</v>
       </c>
       <c r="J44" t="n">
-        <v>-16.87</v>
+        <v>-16.78</v>
       </c>
       <c r="K44" t="inlineStr">
         <is>
@@ -2168,31 +2168,31 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>-1.01</v>
+        <v>0</v>
       </c>
       <c r="C45" t="n">
-        <v>0.11</v>
+        <v>0.45</v>
       </c>
       <c r="D45" t="n">
-        <v>4.22</v>
+        <v>4.69</v>
       </c>
       <c r="E45" t="n">
-        <v>8.69</v>
+        <v>8.68</v>
       </c>
       <c r="F45" t="n">
-        <v>7.73</v>
+        <v>7.66</v>
       </c>
       <c r="G45" t="n">
-        <v>12.8</v>
+        <v>15.61</v>
       </c>
       <c r="H45" t="n">
-        <v>1.79</v>
+        <v>3.57</v>
       </c>
       <c r="I45" t="n">
-        <v>22.54</v>
+        <v>22.26</v>
       </c>
       <c r="J45" t="n">
-        <v>49.2</v>
+        <v>49.39</v>
       </c>
       <c r="K45" t="inlineStr">
         <is>
@@ -2207,31 +2207,31 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>-0.66</v>
+        <v>0</v>
       </c>
       <c r="C46" t="n">
-        <v>-1.27</v>
+        <v>0.52</v>
       </c>
       <c r="D46" t="n">
-        <v>-2.39</v>
+        <v>-3.02</v>
       </c>
       <c r="E46" t="n">
-        <v>6.68</v>
+        <v>4.02</v>
       </c>
       <c r="F46" t="n">
-        <v>-3.64</v>
+        <v>-4.2</v>
       </c>
       <c r="G46" t="n">
-        <v>-12.19</v>
+        <v>-10.29</v>
       </c>
       <c r="H46" t="n">
-        <v>-13.54</v>
+        <v>-13.91</v>
       </c>
       <c r="I46" t="n">
-        <v>-3.62</v>
+        <v>-5.45</v>
       </c>
       <c r="J46" t="n">
-        <v>24.99</v>
+        <v>22.49</v>
       </c>
       <c r="K46" t="inlineStr">
         <is>
@@ -2249,28 +2249,28 @@
         <v>0</v>
       </c>
       <c r="C47" t="n">
-        <v>-0.11</v>
+        <v>1.02</v>
       </c>
       <c r="D47" t="n">
-        <v>-3.1</v>
+        <v>-1.16</v>
       </c>
       <c r="E47" t="n">
-        <v>0.39</v>
+        <v>-2.66</v>
       </c>
       <c r="F47" t="n">
-        <v>-8.01</v>
+        <v>-7.45</v>
       </c>
       <c r="G47" t="n">
-        <v>-12.7</v>
+        <v>-10.77</v>
       </c>
       <c r="H47" t="n">
-        <v>-16.15</v>
+        <v>-16.59</v>
       </c>
       <c r="I47" t="n">
-        <v>-23.99</v>
+        <v>-24.44</v>
       </c>
       <c r="J47" t="n">
-        <v>-25.61</v>
+        <v>-26.16</v>
       </c>
       <c r="K47" t="inlineStr">
         <is>
@@ -2285,31 +2285,31 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>-0.19</v>
+        <v>0</v>
       </c>
       <c r="C48" t="n">
-        <v>1.7</v>
+        <v>1.92</v>
       </c>
       <c r="D48" t="n">
-        <v>0.46</v>
+        <v>1.58</v>
       </c>
       <c r="E48" t="n">
-        <v>14.5</v>
+        <v>13.82</v>
       </c>
       <c r="F48" t="n">
-        <v>8.960000000000001</v>
+        <v>8.25</v>
       </c>
       <c r="G48" t="n">
-        <v>17.18</v>
+        <v>20.35</v>
       </c>
       <c r="H48" t="n">
-        <v>36.72</v>
+        <v>40.75</v>
       </c>
       <c r="I48" t="n">
-        <v>50.52</v>
+        <v>49.06</v>
       </c>
       <c r="J48" t="n">
-        <v>11.49</v>
+        <v>10.06</v>
       </c>
       <c r="K48" t="inlineStr">
         <is>
@@ -2324,31 +2324,31 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>-1.68</v>
+        <v>0</v>
       </c>
       <c r="C49" t="n">
-        <v>-1.21</v>
+        <v>-0.76</v>
       </c>
       <c r="D49" t="n">
-        <v>-4.77</v>
+        <v>-5.19</v>
       </c>
       <c r="E49" t="n">
-        <v>3.77</v>
+        <v>2.03</v>
       </c>
       <c r="F49" t="n">
-        <v>-0.73</v>
+        <v>1.9</v>
       </c>
       <c r="G49" t="n">
-        <v>11.1</v>
+        <v>14.59</v>
       </c>
       <c r="H49" t="n">
-        <v>2.47</v>
+        <v>3.12</v>
       </c>
       <c r="I49" t="n">
-        <v>-27.91</v>
+        <v>-27.74</v>
       </c>
       <c r="J49" t="n">
-        <v>-13.94</v>
+        <v>-16.4</v>
       </c>
       <c r="K49" t="inlineStr">
         <is>
@@ -2363,31 +2363,31 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>-1.76</v>
+        <v>0</v>
       </c>
       <c r="C50" t="n">
-        <v>-2.59</v>
+        <v>-1.3</v>
       </c>
       <c r="D50" t="n">
-        <v>-9.82</v>
+        <v>-7.17</v>
       </c>
       <c r="E50" t="n">
-        <v>2.11</v>
+        <v>-1.03</v>
       </c>
       <c r="F50" t="n">
-        <v>-16.41</v>
+        <v>-15.72</v>
       </c>
       <c r="G50" t="n">
-        <v>-16.1</v>
+        <v>-12.42</v>
       </c>
       <c r="H50" t="n">
-        <v>-2.1</v>
+        <v>2.16</v>
       </c>
       <c r="I50" t="n">
-        <v>-46.21</v>
+        <v>-46.97</v>
       </c>
       <c r="J50" t="n">
-        <v>-36.7</v>
+        <v>-37.83</v>
       </c>
       <c r="K50" t="inlineStr">
         <is>
@@ -2405,28 +2405,28 @@
         <v>0</v>
       </c>
       <c r="C51" t="n">
-        <v>0.21</v>
+        <v>-2.2</v>
       </c>
       <c r="D51" t="n">
-        <v>2.02</v>
+        <v>-5.4</v>
       </c>
       <c r="E51" t="n">
-        <v>15.01</v>
+        <v>10.67</v>
       </c>
       <c r="F51" t="n">
-        <v>8.4</v>
+        <v>4.43</v>
       </c>
       <c r="G51" t="n">
-        <v>13.64</v>
+        <v>14.12</v>
       </c>
       <c r="H51" t="n">
-        <v>-23.9</v>
+        <v>-24.52</v>
       </c>
       <c r="I51" t="n">
-        <v>-35.25</v>
+        <v>-38.31</v>
       </c>
       <c r="J51" t="n">
-        <v>-61.12</v>
+        <v>-62.61</v>
       </c>
       <c r="K51" t="inlineStr">
         <is>
@@ -2444,28 +2444,28 @@
         <v>0</v>
       </c>
       <c r="C52" t="n">
-        <v>0.09</v>
+        <v>0.03</v>
       </c>
       <c r="D52" t="n">
-        <v>0.32</v>
+        <v>-0.18</v>
       </c>
       <c r="E52" t="n">
-        <v>16.16</v>
+        <v>13.41</v>
       </c>
       <c r="F52" t="n">
-        <v>3.64</v>
+        <v>2.12</v>
       </c>
       <c r="G52" t="n">
-        <v>10.05</v>
+        <v>10.21</v>
       </c>
       <c r="H52" t="n">
-        <v>6.69</v>
+        <v>6.75</v>
       </c>
       <c r="I52" t="n">
-        <v>-10.08</v>
+        <v>-12</v>
       </c>
       <c r="J52" t="n">
-        <v>7.63</v>
+        <v>6.32</v>
       </c>
       <c r="K52" t="inlineStr">
         <is>
@@ -2480,31 +2480,31 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>-0.08</v>
+        <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>0.42</v>
+        <v>0.98</v>
       </c>
       <c r="D53" t="n">
-        <v>3.12</v>
+        <v>2.63</v>
       </c>
       <c r="E53" t="n">
-        <v>14.51</v>
+        <v>14.01</v>
       </c>
       <c r="F53" t="n">
-        <v>14.82</v>
+        <v>14.42</v>
       </c>
       <c r="G53" t="n">
-        <v>24.88</v>
+        <v>25.92</v>
       </c>
       <c r="H53" t="n">
-        <v>8.73</v>
+        <v>11.02</v>
       </c>
       <c r="I53" t="n">
-        <v>54.53</v>
+        <v>53.5</v>
       </c>
       <c r="J53" t="n">
-        <v>120.04</v>
+        <v>116.97</v>
       </c>
       <c r="K53" t="inlineStr">
         <is>
@@ -2519,31 +2519,31 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>-1.61</v>
+        <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>-3.68</v>
+        <v>-1.37</v>
       </c>
       <c r="D54" t="n">
-        <v>-9.09</v>
+        <v>-8.6</v>
       </c>
       <c r="E54" t="n">
-        <v>-14.35</v>
+        <v>-17.17</v>
       </c>
       <c r="F54" t="n">
-        <v>-23.69</v>
+        <v>-24.84</v>
       </c>
       <c r="G54" t="n">
-        <v>-32.94</v>
+        <v>-30.49</v>
       </c>
       <c r="H54" t="n">
-        <v>-42.19</v>
+        <v>-42.24</v>
       </c>
       <c r="I54" t="n">
-        <v>-38.76</v>
+        <v>-40.13</v>
       </c>
       <c r="J54" t="n">
-        <v>-15.6</v>
+        <v>-15.89</v>
       </c>
       <c r="K54" t="inlineStr">
         <is>
@@ -2561,25 +2561,25 @@
         <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>-2.92</v>
+        <v>-2.7</v>
       </c>
       <c r="D55" t="n">
-        <v>-6.9</v>
+        <v>-7.42</v>
       </c>
       <c r="E55" t="n">
-        <v>-12.55</v>
+        <v>-16.41</v>
       </c>
       <c r="F55" t="n">
-        <v>-22.42</v>
+        <v>-25.51</v>
       </c>
       <c r="G55" t="n">
-        <v>-31.51</v>
+        <v>-31.26</v>
       </c>
       <c r="H55" t="n">
-        <v>-41.26</v>
+        <v>-42.58</v>
       </c>
       <c r="I55" t="n">
-        <v>-5.59</v>
+        <v>-8.49</v>
       </c>
       <c r="J55" t="inlineStr"/>
       <c r="K55" t="inlineStr">
@@ -2598,28 +2598,28 @@
         <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>2.13</v>
+        <v>0.91</v>
       </c>
       <c r="D56" t="n">
-        <v>-0.8100000000000001</v>
+        <v>-2.35</v>
       </c>
       <c r="E56" t="n">
-        <v>6.43</v>
+        <v>2.51</v>
       </c>
       <c r="F56" t="n">
-        <v>-4.09</v>
+        <v>-4.38</v>
       </c>
       <c r="G56" t="n">
-        <v>-6.41</v>
+        <v>-4.75</v>
       </c>
       <c r="H56" t="n">
-        <v>-4.84</v>
+        <v>-4.79</v>
       </c>
       <c r="I56" t="n">
-        <v>-19.77</v>
+        <v>-20.33</v>
       </c>
       <c r="J56" t="n">
-        <v>-1.39</v>
+        <v>-5.24</v>
       </c>
       <c r="K56" t="inlineStr">
         <is>
@@ -2634,31 +2634,31 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>2.15</v>
+        <v>0</v>
       </c>
       <c r="C57" t="n">
-        <v>4.09</v>
+        <v>5.28</v>
       </c>
       <c r="D57" t="n">
-        <v>-3.27</v>
+        <v>-0.43</v>
       </c>
       <c r="E57" t="n">
-        <v>7.87</v>
+        <v>-0.11</v>
       </c>
       <c r="F57" t="n">
-        <v>-4.37</v>
+        <v>-3.42</v>
       </c>
       <c r="G57" t="n">
-        <v>-3.81</v>
+        <v>1.66</v>
       </c>
       <c r="H57" t="n">
-        <v>-14.8</v>
+        <v>-13.9</v>
       </c>
       <c r="I57" t="n">
-        <v>-2.22</v>
+        <v>-4.03</v>
       </c>
       <c r="J57" t="n">
-        <v>8.960000000000001</v>
+        <v>7.89</v>
       </c>
       <c r="K57" t="inlineStr">
         <is>
@@ -2673,31 +2673,31 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>-0.24</v>
+        <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>-0.28</v>
+        <v>0.33</v>
       </c>
       <c r="D58" t="n">
-        <v>0.71</v>
+        <v>-1.16</v>
       </c>
       <c r="E58" t="n">
-        <v>1.82</v>
+        <v>-1.71</v>
       </c>
       <c r="F58" t="n">
-        <v>-0.98</v>
+        <v>-0.84</v>
       </c>
       <c r="G58" t="n">
-        <v>-11.14</v>
+        <v>-9.779999999999999</v>
       </c>
       <c r="H58" t="n">
-        <v>-13.25</v>
+        <v>-13.18</v>
       </c>
       <c r="I58" t="n">
-        <v>-30.54</v>
+        <v>-31.69</v>
       </c>
       <c r="J58" t="n">
-        <v>-63.29</v>
+        <v>-64.08</v>
       </c>
       <c r="K58" t="inlineStr">
         <is>
@@ -2712,31 +2712,31 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.26</v>
+        <v>0</v>
       </c>
       <c r="C59" t="n">
-        <v>0.64</v>
+        <v>0.49</v>
       </c>
       <c r="D59" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E59" t="n">
-        <v>10.75</v>
+        <v>9.640000000000001</v>
       </c>
       <c r="F59" t="n">
-        <v>1.84</v>
+        <v>1.99</v>
       </c>
       <c r="G59" t="n">
-        <v>-9.25</v>
+        <v>-6.37</v>
       </c>
       <c r="H59" t="n">
-        <v>-18.67</v>
+        <v>-17.15</v>
       </c>
       <c r="I59" t="n">
-        <v>-23.8</v>
+        <v>-25.15</v>
       </c>
       <c r="J59" t="n">
-        <v>-11.9</v>
+        <v>-13.12</v>
       </c>
       <c r="K59" t="inlineStr">
         <is>
@@ -2751,31 +2751,31 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>-0.6899999999999999</v>
+        <v>0</v>
       </c>
       <c r="C60" t="n">
-        <v>-1.65</v>
+        <v>0.25</v>
       </c>
       <c r="D60" t="n">
-        <v>-0.71</v>
+        <v>0.83</v>
       </c>
       <c r="E60" t="n">
-        <v>-0.76</v>
+        <v>-2.36</v>
       </c>
       <c r="F60" t="n">
-        <v>-3.73</v>
+        <v>-4.24</v>
       </c>
       <c r="G60" t="n">
-        <v>-2.7</v>
+        <v>0.9</v>
       </c>
       <c r="H60" t="n">
-        <v>-31.72</v>
+        <v>-30.58</v>
       </c>
       <c r="I60" t="n">
-        <v>35.22</v>
+        <v>33.21</v>
       </c>
       <c r="J60" t="n">
-        <v>68.11</v>
+        <v>67.26000000000001</v>
       </c>
       <c r="K60" t="inlineStr">
         <is>
@@ -2793,28 +2793,28 @@
         <v>0</v>
       </c>
       <c r="C61" t="n">
-        <v>-0.43</v>
+        <v>1.46</v>
       </c>
       <c r="D61" t="n">
-        <v>-6.96</v>
+        <v>-5.5</v>
       </c>
       <c r="E61" t="n">
-        <v>-2.68</v>
+        <v>-3.92</v>
       </c>
       <c r="F61" t="n">
-        <v>-13.1</v>
+        <v>-11.52</v>
       </c>
       <c r="G61" t="n">
-        <v>-24.63</v>
+        <v>-21.97</v>
       </c>
       <c r="H61" t="n">
-        <v>-22.25</v>
+        <v>-22.38</v>
       </c>
       <c r="I61" t="n">
-        <v>-33.99</v>
+        <v>-34.32</v>
       </c>
       <c r="J61" t="n">
-        <v>-7.75</v>
+        <v>-9.050000000000001</v>
       </c>
       <c r="K61" t="inlineStr">
         <is>
@@ -2832,28 +2832,28 @@
         <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>6.03</v>
+        <v>3.65</v>
       </c>
       <c r="D62" t="n">
-        <v>2.55</v>
+        <v>4.42</v>
       </c>
       <c r="E62" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F62" t="n">
-        <v>10.95</v>
+        <v>11.22</v>
       </c>
       <c r="G62" t="n">
-        <v>34.03</v>
+        <v>42.77</v>
       </c>
       <c r="H62" t="n">
-        <v>5.98</v>
+        <v>9.029999999999999</v>
       </c>
       <c r="I62" t="n">
-        <v>-6.84</v>
+        <v>-6.97</v>
       </c>
       <c r="J62" t="n">
-        <v>-18.25</v>
+        <v>-20.96</v>
       </c>
       <c r="K62" t="inlineStr">
         <is>
@@ -2868,31 +2868,31 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>-1.04</v>
+        <v>0</v>
       </c>
       <c r="C63" t="n">
-        <v>1.15</v>
+        <v>0.34</v>
       </c>
       <c r="D63" t="n">
-        <v>10.63</v>
+        <v>10.12</v>
       </c>
       <c r="E63" t="n">
-        <v>4.55</v>
+        <v>1.33</v>
       </c>
       <c r="F63" t="n">
-        <v>6.68</v>
+        <v>3.85</v>
       </c>
       <c r="G63" t="n">
-        <v>11.8</v>
+        <v>8.42</v>
       </c>
       <c r="H63" t="n">
-        <v>81.7</v>
+        <v>88.45999999999999</v>
       </c>
       <c r="I63" t="n">
-        <v>27.23</v>
+        <v>25.9</v>
       </c>
       <c r="J63" t="n">
-        <v>-9.970000000000001</v>
+        <v>-14.76</v>
       </c>
       <c r="K63" t="inlineStr">
         <is>
@@ -2910,28 +2910,28 @@
         <v>0</v>
       </c>
       <c r="C64" t="n">
-        <v>1.55</v>
+        <v>-0.54</v>
       </c>
       <c r="D64" t="n">
-        <v>-2.18</v>
+        <v>-1.66</v>
       </c>
       <c r="E64" t="n">
-        <v>2.23</v>
+        <v>-3.03</v>
       </c>
       <c r="F64" t="n">
-        <v>-3.78</v>
+        <v>-5.93</v>
       </c>
       <c r="G64" t="n">
-        <v>-14.22</v>
+        <v>-12.16</v>
       </c>
       <c r="H64" t="n">
-        <v>-20.23</v>
+        <v>-21.84</v>
       </c>
       <c r="I64" t="n">
-        <v>-29.33</v>
+        <v>-31.56</v>
       </c>
       <c r="J64" t="n">
-        <v>-28.04</v>
+        <v>-31.3</v>
       </c>
       <c r="K64" t="inlineStr">
         <is>
@@ -2949,28 +2949,28 @@
         <v>0</v>
       </c>
       <c r="C65" t="n">
-        <v>-0.87</v>
+        <v>0.13</v>
       </c>
       <c r="D65" t="n">
-        <v>-1.58</v>
+        <v>-1.37</v>
       </c>
       <c r="E65" t="n">
-        <v>-4.75</v>
+        <v>-2.54</v>
       </c>
       <c r="F65" t="n">
-        <v>-2.94</v>
+        <v>-3.91</v>
       </c>
       <c r="G65" t="n">
-        <v>-3.19</v>
+        <v>-2.4</v>
       </c>
       <c r="H65" t="n">
-        <v>21.77</v>
+        <v>21.22</v>
       </c>
       <c r="I65" t="n">
-        <v>28.53</v>
+        <v>28.22</v>
       </c>
       <c r="J65" t="n">
-        <v>1.84</v>
+        <v>1.95</v>
       </c>
       <c r="K65" t="inlineStr">
         <is>
@@ -2985,31 +2985,31 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>-0.32</v>
+        <v>0</v>
       </c>
       <c r="C66" t="n">
-        <v>-5.2</v>
+        <v>-2.36</v>
       </c>
       <c r="D66" t="n">
-        <v>-5.49</v>
+        <v>-6.44</v>
       </c>
       <c r="E66" t="n">
-        <v>-13.66</v>
+        <v>-13.46</v>
       </c>
       <c r="F66" t="n">
-        <v>-14.31</v>
+        <v>-16.44</v>
       </c>
       <c r="G66" t="n">
-        <v>-7.38</v>
+        <v>-9.77</v>
       </c>
       <c r="H66" t="n">
-        <v>24.95</v>
+        <v>21.86</v>
       </c>
       <c r="I66" t="n">
-        <v>-15.59</v>
+        <v>-18.2</v>
       </c>
       <c r="J66" t="n">
-        <v>-67.5</v>
+        <v>-68.06</v>
       </c>
       <c r="K66" t="inlineStr">
         <is>
@@ -3027,28 +3027,28 @@
         <v>0</v>
       </c>
       <c r="C67" t="n">
-        <v>-1.48</v>
+        <v>-1.71</v>
       </c>
       <c r="D67" t="n">
-        <v>-4.18</v>
+        <v>-4.29</v>
       </c>
       <c r="E67" t="n">
-        <v>-11.11</v>
+        <v>-9.01</v>
       </c>
       <c r="F67" t="n">
-        <v>-5.74</v>
+        <v>-9.359999999999999</v>
       </c>
       <c r="G67" t="n">
-        <v>-2.49</v>
+        <v>-1.15</v>
       </c>
       <c r="H67" t="n">
-        <v>18.2</v>
+        <v>16.82</v>
       </c>
       <c r="I67" t="n">
-        <v>7.65</v>
+        <v>7.3</v>
       </c>
       <c r="J67" t="n">
-        <v>-48.4</v>
+        <v>-49.18</v>
       </c>
       <c r="K67" t="inlineStr">
         <is>
@@ -3063,31 +3063,31 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>-1.29</v>
+        <v>0</v>
       </c>
       <c r="C68" t="n">
-        <v>0.34</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="D68" t="n">
-        <v>-3.8</v>
+        <v>-4.71</v>
       </c>
       <c r="E68" t="n">
-        <v>0.5</v>
+        <v>-0.34</v>
       </c>
       <c r="F68" t="n">
-        <v>-6.7</v>
+        <v>-3.91</v>
       </c>
       <c r="G68" t="n">
-        <v>-10.89</v>
+        <v>-10.22</v>
       </c>
       <c r="H68" t="n">
-        <v>-10.86</v>
+        <v>-10.21</v>
       </c>
       <c r="I68" t="n">
-        <v>13.31</v>
+        <v>12.31</v>
       </c>
       <c r="J68" t="n">
-        <v>59.35</v>
+        <v>60.17</v>
       </c>
       <c r="K68" t="inlineStr">
         <is>
@@ -3102,31 +3102,31 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>-0.17</v>
+        <v>0</v>
       </c>
       <c r="C69" t="n">
-        <v>1.68</v>
+        <v>1.71</v>
       </c>
       <c r="D69" t="n">
-        <v>1.98</v>
+        <v>3</v>
       </c>
       <c r="E69" t="n">
-        <v>8.17</v>
+        <v>7.71</v>
       </c>
       <c r="F69" t="n">
-        <v>-1.76</v>
+        <v>-0.64</v>
       </c>
       <c r="G69" t="n">
-        <v>0.8</v>
+        <v>0.93</v>
       </c>
       <c r="H69" t="n">
-        <v>-3.29</v>
+        <v>-2.27</v>
       </c>
       <c r="I69" t="n">
-        <v>39.57</v>
+        <v>38.45</v>
       </c>
       <c r="J69" t="n">
-        <v>86.26000000000001</v>
+        <v>84.87</v>
       </c>
       <c r="K69" t="inlineStr">
         <is>
@@ -3144,25 +3144,25 @@
         <v>0</v>
       </c>
       <c r="C70" t="n">
-        <v>1.3</v>
+        <v>1.68</v>
       </c>
       <c r="D70" t="n">
-        <v>-2.19</v>
+        <v>-0.78</v>
       </c>
       <c r="E70" t="n">
-        <v>5.05</v>
+        <v>4.24</v>
       </c>
       <c r="F70" t="n">
-        <v>-9.82</v>
+        <v>-9.19</v>
       </c>
       <c r="G70" t="n">
-        <v>-8.94</v>
+        <v>-9.289999999999999</v>
       </c>
       <c r="H70" t="n">
-        <v>-9.380000000000001</v>
+        <v>-8.050000000000001</v>
       </c>
       <c r="I70" t="n">
-        <v>25</v>
+        <v>25.41</v>
       </c>
       <c r="J70" t="inlineStr"/>
       <c r="K70" t="inlineStr">
@@ -3178,31 +3178,31 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.24</v>
+        <v>0</v>
       </c>
       <c r="C71" t="n">
-        <v>0.25</v>
+        <v>3.74</v>
       </c>
       <c r="D71" t="n">
-        <v>-1.42</v>
+        <v>2.72</v>
       </c>
       <c r="E71" t="n">
         <v>10.53</v>
       </c>
       <c r="F71" t="n">
-        <v>3.52</v>
+        <v>3.36</v>
       </c>
       <c r="G71" t="n">
-        <v>11.83</v>
+        <v>17.33</v>
       </c>
       <c r="H71" t="n">
-        <v>-5.58</v>
+        <v>-3.84</v>
       </c>
       <c r="I71" t="n">
-        <v>62.92</v>
+        <v>62.83</v>
       </c>
       <c r="J71" t="n">
-        <v>185.48</v>
+        <v>186</v>
       </c>
       <c r="K71" t="inlineStr">
         <is>
@@ -3217,31 +3217,31 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>-1.57</v>
+        <v>0</v>
       </c>
       <c r="C72" t="n">
-        <v>-0.88</v>
+        <v>2.67</v>
       </c>
       <c r="D72" t="n">
-        <v>0.19</v>
+        <v>4.2</v>
       </c>
       <c r="E72" t="n">
-        <v>25.51</v>
+        <v>25.98</v>
       </c>
       <c r="F72" t="n">
-        <v>12.38</v>
+        <v>14.82</v>
       </c>
       <c r="G72" t="n">
-        <v>30.98</v>
+        <v>37.65</v>
       </c>
       <c r="H72" t="n">
-        <v>26.4</v>
+        <v>34.63</v>
       </c>
       <c r="I72" t="n">
-        <v>158.7</v>
+        <v>160.13</v>
       </c>
       <c r="J72" t="n">
-        <v>209.55</v>
+        <v>211.95</v>
       </c>
       <c r="K72" t="inlineStr">
         <is>
@@ -3256,31 +3256,31 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>-1.18</v>
+        <v>0</v>
       </c>
       <c r="C73" t="n">
-        <v>-1.35</v>
+        <v>3.12</v>
       </c>
       <c r="D73" t="n">
-        <v>-3.72</v>
+        <v>1.93</v>
       </c>
       <c r="E73" t="n">
-        <v>15.32</v>
+        <v>14.93</v>
       </c>
       <c r="F73" t="n">
-        <v>4.13</v>
+        <v>6.01</v>
       </c>
       <c r="G73" t="n">
-        <v>-6.58</v>
+        <v>-1.91</v>
       </c>
       <c r="H73" t="n">
-        <v>-13.5</v>
+        <v>-9.869999999999999</v>
       </c>
       <c r="I73" t="n">
-        <v>58.69</v>
+        <v>57.97</v>
       </c>
       <c r="J73" t="n">
-        <v>79.61</v>
+        <v>81.11</v>
       </c>
       <c r="K73" t="inlineStr">
         <is>
@@ -3295,28 +3295,28 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>-1.55</v>
+        <v>0</v>
       </c>
       <c r="C74" t="n">
-        <v>-1.47</v>
+        <v>0.47</v>
       </c>
       <c r="D74" t="n">
-        <v>-5.52</v>
+        <v>-2.49</v>
       </c>
       <c r="E74" t="n">
-        <v>11.37</v>
+        <v>10.63</v>
       </c>
       <c r="F74" t="n">
-        <v>0.63</v>
+        <v>3.35</v>
       </c>
       <c r="G74" t="n">
-        <v>-8.68</v>
+        <v>-5.87</v>
       </c>
       <c r="H74" t="n">
-        <v>-20.13</v>
+        <v>-17.95</v>
       </c>
       <c r="I74" t="n">
-        <v>11.96</v>
+        <v>10.88</v>
       </c>
       <c r="J74" t="inlineStr"/>
       <c r="K74" t="inlineStr">
@@ -3335,28 +3335,28 @@
         <v>0</v>
       </c>
       <c r="C75" t="n">
-        <v>-2.21</v>
+        <v>1.81</v>
       </c>
       <c r="D75" t="n">
-        <v>-2.25</v>
+        <v>-0.08</v>
       </c>
       <c r="E75" t="n">
-        <v>17.53</v>
+        <v>15.1</v>
       </c>
       <c r="F75" t="n">
-        <v>6.89</v>
+        <v>6.35</v>
       </c>
       <c r="G75" t="n">
-        <v>-12.39</v>
+        <v>-9.17</v>
       </c>
       <c r="H75" t="n">
-        <v>-14.15</v>
+        <v>-12.44</v>
       </c>
       <c r="I75" t="n">
-        <v>13.22</v>
+        <v>14.13</v>
       </c>
       <c r="J75" t="n">
-        <v>44.91</v>
+        <v>44.99</v>
       </c>
       <c r="K75" t="inlineStr">
         <is>
@@ -3374,28 +3374,28 @@
         <v>0</v>
       </c>
       <c r="C76" t="n">
-        <v>0.5600000000000001</v>
+        <v>2.38</v>
       </c>
       <c r="D76" t="n">
-        <v>1.75</v>
+        <v>3.72</v>
       </c>
       <c r="E76" t="n">
-        <v>14</v>
+        <v>14.06</v>
       </c>
       <c r="F76" t="n">
-        <v>4.76</v>
+        <v>6.78</v>
       </c>
       <c r="G76" t="n">
-        <v>11.05</v>
+        <v>12.65</v>
       </c>
       <c r="H76" t="n">
-        <v>11.64</v>
+        <v>15.45</v>
       </c>
       <c r="I76" t="n">
-        <v>59.72</v>
+        <v>57.38</v>
       </c>
       <c r="J76" t="n">
-        <v>136.04</v>
+        <v>136.22</v>
       </c>
       <c r="K76" t="inlineStr">
         <is>
@@ -3410,31 +3410,31 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>-0.38</v>
+        <v>0</v>
       </c>
       <c r="C77" t="n">
-        <v>0.79</v>
+        <v>0.8</v>
       </c>
       <c r="D77" t="n">
-        <v>-1.76</v>
+        <v>-0.17</v>
       </c>
       <c r="E77" t="n">
-        <v>9.220000000000001</v>
+        <v>9.289999999999999</v>
       </c>
       <c r="F77" t="n">
-        <v>6.88</v>
+        <v>6.9</v>
       </c>
       <c r="G77" t="n">
-        <v>7.97</v>
+        <v>8.18</v>
       </c>
       <c r="H77" t="n">
-        <v>19.69</v>
+        <v>20.71</v>
       </c>
       <c r="I77" t="n">
-        <v>26.52</v>
+        <v>23.01</v>
       </c>
       <c r="J77" t="n">
-        <v>141.37</v>
+        <v>141.65</v>
       </c>
       <c r="K77" t="inlineStr">
         <is>
@@ -3452,28 +3452,28 @@
         <v>0</v>
       </c>
       <c r="C78" t="n">
-        <v>-1.89</v>
+        <v>2.56</v>
       </c>
       <c r="D78" t="n">
-        <v>-3.41</v>
+        <v>-0.49</v>
       </c>
       <c r="E78" t="n">
-        <v>14.56</v>
+        <v>14.49</v>
       </c>
       <c r="F78" t="n">
-        <v>-7.48</v>
+        <v>-5</v>
       </c>
       <c r="G78" t="n">
-        <v>-3.57</v>
+        <v>0.09</v>
       </c>
       <c r="H78" t="n">
-        <v>-8.74</v>
+        <v>-4.32</v>
       </c>
       <c r="I78" t="n">
-        <v>31.25</v>
+        <v>31.42</v>
       </c>
       <c r="J78" t="n">
-        <v>101.88</v>
+        <v>104.72</v>
       </c>
       <c r="K78" t="inlineStr">
         <is>
@@ -3488,31 +3488,31 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>-0.03</v>
+        <v>0</v>
       </c>
       <c r="C79" t="n">
-        <v>1.36</v>
+        <v>1.15</v>
       </c>
       <c r="D79" t="n">
-        <v>2.44</v>
+        <v>2.06</v>
       </c>
       <c r="E79" t="n">
-        <v>12.13</v>
+        <v>10.7</v>
       </c>
       <c r="F79" t="n">
-        <v>6.46</v>
+        <v>7.24</v>
       </c>
       <c r="G79" t="n">
-        <v>6.82</v>
+        <v>7.61</v>
       </c>
       <c r="H79" t="n">
-        <v>6.61</v>
+        <v>7.32</v>
       </c>
       <c r="I79" t="n">
-        <v>56.65</v>
+        <v>57.14</v>
       </c>
       <c r="J79" t="n">
-        <v>159.13</v>
+        <v>157.74</v>
       </c>
       <c r="K79" t="inlineStr">
         <is>
@@ -3530,28 +3530,28 @@
         <v>0</v>
       </c>
       <c r="C80" t="n">
-        <v>-0.27</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="D80" t="n">
-        <v>2.36</v>
+        <v>4.32</v>
       </c>
       <c r="E80" t="n">
-        <v>22.85</v>
+        <v>19.61</v>
       </c>
       <c r="F80" t="n">
-        <v>-10.33</v>
+        <v>-9.460000000000001</v>
       </c>
       <c r="G80" t="n">
-        <v>-15.57</v>
+        <v>-13.07</v>
       </c>
       <c r="H80" t="n">
-        <v>-17.67</v>
+        <v>-17.86</v>
       </c>
       <c r="I80" t="n">
-        <v>12.23</v>
+        <v>10.23</v>
       </c>
       <c r="J80" t="n">
-        <v>127.81</v>
+        <v>123.69</v>
       </c>
       <c r="K80" t="inlineStr">
         <is>
@@ -3569,28 +3569,28 @@
         <v>0</v>
       </c>
       <c r="C81" t="n">
-        <v>-0.13</v>
+        <v>1.34</v>
       </c>
       <c r="D81" t="n">
-        <v>-2.13</v>
+        <v>0.19</v>
       </c>
       <c r="E81" t="n">
-        <v>10.82</v>
+        <v>8.93</v>
       </c>
       <c r="F81" t="n">
-        <v>-5.84</v>
+        <v>-5.28</v>
       </c>
       <c r="G81" t="n">
-        <v>-6.51</v>
+        <v>-3.05</v>
       </c>
       <c r="H81" t="n">
-        <v>-3.87</v>
+        <v>-3.09</v>
       </c>
       <c r="I81" t="n">
-        <v>26.73</v>
+        <v>25.62</v>
       </c>
       <c r="J81" t="n">
-        <v>98.58</v>
+        <v>99.37</v>
       </c>
       <c r="K81" t="inlineStr">
         <is>
@@ -3605,31 +3605,31 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>-0.82</v>
+        <v>0</v>
       </c>
       <c r="C82" t="n">
-        <v>-1.62</v>
+        <v>-0.09</v>
       </c>
       <c r="D82" t="n">
-        <v>-2.04</v>
+        <v>-1.55</v>
       </c>
       <c r="E82" t="n">
-        <v>11.66</v>
+        <v>8.68</v>
       </c>
       <c r="F82" t="n">
-        <v>5.15</v>
+        <v>3.73</v>
       </c>
       <c r="G82" t="n">
-        <v>-1.5</v>
+        <v>-0.42</v>
       </c>
       <c r="H82" t="n">
-        <v>-1.07</v>
+        <v>0.65</v>
       </c>
       <c r="I82" t="n">
-        <v>29.28</v>
+        <v>30.17</v>
       </c>
       <c r="J82" t="n">
-        <v>75.98999999999999</v>
+        <v>75.84999999999999</v>
       </c>
       <c r="K82" t="inlineStr">
         <is>
@@ -3644,31 +3644,31 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>-0.24</v>
+        <v>0</v>
       </c>
       <c r="C83" t="n">
-        <v>0.91</v>
+        <v>0.63</v>
       </c>
       <c r="D83" t="n">
-        <v>4.2</v>
+        <v>1.57</v>
       </c>
       <c r="E83" t="n">
-        <v>13.04</v>
+        <v>11.39</v>
       </c>
       <c r="F83" t="n">
-        <v>7.8</v>
+        <v>7.92</v>
       </c>
       <c r="G83" t="n">
-        <v>11.24</v>
+        <v>10.83</v>
       </c>
       <c r="H83" t="n">
-        <v>12.02</v>
+        <v>13.29</v>
       </c>
       <c r="I83" t="n">
-        <v>45.71</v>
+        <v>43.86</v>
       </c>
       <c r="J83" t="n">
-        <v>61.96</v>
+        <v>59.44</v>
       </c>
       <c r="K83" t="inlineStr">
         <is>
@@ -3686,28 +3686,28 @@
         <v>0</v>
       </c>
       <c r="C84" t="n">
-        <v>-1.68</v>
+        <v>2.31</v>
       </c>
       <c r="D84" t="n">
-        <v>6.79</v>
+        <v>9.84</v>
       </c>
       <c r="E84" t="n">
-        <v>17.74</v>
+        <v>16.98</v>
       </c>
       <c r="F84" t="n">
-        <v>14.89</v>
+        <v>18.16</v>
       </c>
       <c r="G84" t="n">
-        <v>40.02</v>
+        <v>44.42</v>
       </c>
       <c r="H84" t="n">
-        <v>22.27</v>
+        <v>26.72</v>
       </c>
       <c r="I84" t="n">
-        <v>200.24</v>
+        <v>196.06</v>
       </c>
       <c r="J84" t="n">
-        <v>487.18</v>
+        <v>490.48</v>
       </c>
       <c r="K84" t="inlineStr">
         <is>
@@ -3722,31 +3722,31 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="C85" t="n">
-        <v>-1.35</v>
+        <v>2.88</v>
       </c>
       <c r="D85" t="n">
-        <v>11.21</v>
+        <v>15.14</v>
       </c>
       <c r="E85" t="n">
-        <v>28.62</v>
+        <v>27.52</v>
       </c>
       <c r="F85" t="n">
-        <v>21.51</v>
+        <v>23.97</v>
       </c>
       <c r="G85" t="n">
-        <v>48.2</v>
+        <v>56.23</v>
       </c>
       <c r="H85" t="n">
-        <v>32.5</v>
+        <v>40.33</v>
       </c>
       <c r="I85" t="n">
-        <v>284.2</v>
+        <v>286.89</v>
       </c>
       <c r="J85" t="n">
-        <v>828.87</v>
+        <v>848.98</v>
       </c>
       <c r="K85" t="inlineStr">
         <is>
@@ -3764,28 +3764,28 @@
         <v>0</v>
       </c>
       <c r="C86" t="n">
-        <v>-2.32</v>
+        <v>1.55</v>
       </c>
       <c r="D86" t="n">
-        <v>2.32</v>
+        <v>5.92</v>
       </c>
       <c r="E86" t="n">
-        <v>22.3</v>
+        <v>20.65</v>
       </c>
       <c r="F86" t="n">
-        <v>9.1</v>
+        <v>10.58</v>
       </c>
       <c r="G86" t="n">
-        <v>14.59</v>
+        <v>20.08</v>
       </c>
       <c r="H86" t="n">
-        <v>1.34</v>
+        <v>2.57</v>
       </c>
       <c r="I86" t="n">
-        <v>74.48999999999999</v>
+        <v>70.59999999999999</v>
       </c>
       <c r="J86" t="n">
-        <v>247.93</v>
+        <v>247.89</v>
       </c>
       <c r="K86" t="inlineStr">
         <is>
@@ -3821,7 +3821,7 @@
         <v>0</v>
       </c>
       <c r="I87" t="n">
-        <v>0.38</v>
+        <v>-1.32</v>
       </c>
       <c r="J87" t="inlineStr"/>
       <c r="K87" t="inlineStr">
@@ -3837,31 +3837,31 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>-0.74</v>
+        <v>0</v>
       </c>
       <c r="C88" t="n">
-        <v>0.05</v>
+        <v>1.07</v>
       </c>
       <c r="D88" t="n">
-        <v>-2.85</v>
+        <v>-1.48</v>
       </c>
       <c r="E88" t="n">
-        <v>6.95</v>
+        <v>5.98</v>
       </c>
       <c r="F88" t="n">
-        <v>-1.57</v>
+        <v>-0.57</v>
       </c>
       <c r="G88" t="n">
-        <v>-2.33</v>
+        <v>0.73</v>
       </c>
       <c r="H88" t="n">
-        <v>-3.56</v>
+        <v>-0.04</v>
       </c>
       <c r="I88" t="n">
-        <v>55.04</v>
+        <v>54.41</v>
       </c>
       <c r="J88" t="n">
-        <v>92.89</v>
+        <v>91.28</v>
       </c>
       <c r="K88" t="inlineStr">
         <is>
@@ -3876,31 +3876,31 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>-1.25</v>
+        <v>0</v>
       </c>
       <c r="C89" t="n">
-        <v>-1.26</v>
+        <v>0.26</v>
       </c>
       <c r="D89" t="n">
-        <v>-3.79</v>
+        <v>-1.44</v>
       </c>
       <c r="E89" t="n">
-        <v>12.61</v>
+        <v>12.97</v>
       </c>
       <c r="F89" t="n">
-        <v>10.28</v>
+        <v>10.95</v>
       </c>
       <c r="G89" t="n">
-        <v>-2.41</v>
+        <v>0.76</v>
       </c>
       <c r="H89" t="n">
-        <v>29.15</v>
+        <v>29.53</v>
       </c>
       <c r="I89" t="n">
-        <v>87.05</v>
+        <v>86.2</v>
       </c>
       <c r="J89" t="n">
-        <v>47.85</v>
+        <v>49.1</v>
       </c>
       <c r="K89" t="inlineStr">
         <is>
@@ -3915,31 +3915,31 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>-3.07</v>
+        <v>0</v>
       </c>
       <c r="C90" t="n">
-        <v>-0.78</v>
+        <v>0.29</v>
       </c>
       <c r="D90" t="n">
-        <v>-7.92</v>
+        <v>-5.88</v>
       </c>
       <c r="E90" t="n">
-        <v>-0.42</v>
+        <v>-3.88</v>
       </c>
       <c r="F90" t="n">
-        <v>-3.89</v>
+        <v>-5.21</v>
       </c>
       <c r="G90" t="n">
-        <v>-11.29</v>
+        <v>-7.25</v>
       </c>
       <c r="H90" t="n">
-        <v>-8.130000000000001</v>
+        <v>-7.83</v>
       </c>
       <c r="I90" t="n">
-        <v>24.68</v>
+        <v>23.93</v>
       </c>
       <c r="J90" t="n">
-        <v>20.77</v>
+        <v>20.72</v>
       </c>
       <c r="K90" t="inlineStr">
         <is>
@@ -3954,31 +3954,31 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>-2.86</v>
+        <v>0</v>
       </c>
       <c r="C91" t="n">
-        <v>-2.75</v>
+        <v>0.75</v>
       </c>
       <c r="D91" t="n">
-        <v>-8.15</v>
+        <v>-5.19</v>
       </c>
       <c r="E91" t="n">
-        <v>6.39</v>
+        <v>2.4</v>
       </c>
       <c r="F91" t="n">
-        <v>-2.11</v>
+        <v>-2.22</v>
       </c>
       <c r="G91" t="n">
-        <v>-15.63</v>
+        <v>-10.99</v>
       </c>
       <c r="H91" t="n">
-        <v>-23.19</v>
+        <v>-21.33</v>
       </c>
       <c r="I91" t="n">
-        <v>-5.25</v>
+        <v>-5.75</v>
       </c>
       <c r="J91" t="n">
-        <v>-29.19</v>
+        <v>-30.08</v>
       </c>
       <c r="K91" t="inlineStr">
         <is>
@@ -3996,28 +3996,28 @@
         <v>0</v>
       </c>
       <c r="C92" t="n">
-        <v>-0.36</v>
+        <v>-0.52</v>
       </c>
       <c r="D92" t="n">
-        <v>-4.67</v>
+        <v>-3.91</v>
       </c>
       <c r="E92" t="n">
-        <v>6.64</v>
+        <v>3.55</v>
       </c>
       <c r="F92" t="n">
-        <v>2.83</v>
+        <v>3.48</v>
       </c>
       <c r="G92" t="n">
-        <v>2.58</v>
+        <v>3.72</v>
       </c>
       <c r="H92" t="n">
-        <v>25.33</v>
+        <v>24.97</v>
       </c>
       <c r="I92" t="n">
-        <v>77.81</v>
+        <v>76.53</v>
       </c>
       <c r="J92" t="n">
-        <v>59.74</v>
+        <v>55.26</v>
       </c>
       <c r="K92" t="inlineStr">
         <is>
@@ -4032,31 +4032,31 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C93" t="n">
-        <v>0.28</v>
+        <v>0.57</v>
       </c>
       <c r="D93" t="n">
-        <v>2.91</v>
+        <v>3.26</v>
       </c>
       <c r="E93" t="n">
-        <v>16.56</v>
+        <v>15.74</v>
       </c>
       <c r="F93" t="n">
-        <v>10.93</v>
+        <v>11.66</v>
       </c>
       <c r="G93" t="n">
-        <v>6</v>
+        <v>6.56</v>
       </c>
       <c r="H93" t="n">
-        <v>-2.53</v>
+        <v>-2.79</v>
       </c>
       <c r="I93" t="n">
-        <v>49.17</v>
+        <v>49.41</v>
       </c>
       <c r="J93" t="n">
-        <v>133.01</v>
+        <v>131.7</v>
       </c>
       <c r="K93" t="inlineStr">
         <is>
@@ -4074,28 +4074,28 @@
         <v>0</v>
       </c>
       <c r="C94" t="n">
-        <v>-1.07</v>
+        <v>1.45</v>
       </c>
       <c r="D94" t="n">
-        <v>-0.2</v>
+        <v>2.03</v>
       </c>
       <c r="E94" t="n">
-        <v>18.68</v>
+        <v>17.94</v>
       </c>
       <c r="F94" t="n">
-        <v>11.47</v>
+        <v>12.46</v>
       </c>
       <c r="G94" t="n">
-        <v>8.51</v>
+        <v>11.27</v>
       </c>
       <c r="H94" t="n">
-        <v>4.75</v>
+        <v>5.43</v>
       </c>
       <c r="I94" t="n">
-        <v>92.48999999999999</v>
+        <v>91.16</v>
       </c>
       <c r="J94" t="n">
-        <v>121.77</v>
+        <v>121.52</v>
       </c>
       <c r="K94" t="inlineStr">
         <is>
@@ -4110,31 +4110,31 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>-0.92</v>
+        <v>0</v>
       </c>
       <c r="C95" t="n">
-        <v>-7.13</v>
+        <v>-1.72</v>
       </c>
       <c r="D95" t="n">
-        <v>-6.03</v>
+        <v>-3.63</v>
       </c>
       <c r="E95" t="n">
-        <v>16.55</v>
+        <v>16.09</v>
       </c>
       <c r="F95" t="n">
-        <v>5.07</v>
+        <v>5.06</v>
       </c>
       <c r="G95" t="n">
-        <v>-13.89</v>
+        <v>-11.68</v>
       </c>
       <c r="H95" t="n">
-        <v>-22.1</v>
+        <v>-21.93</v>
       </c>
       <c r="I95" t="n">
-        <v>1.04</v>
+        <v>1.87</v>
       </c>
       <c r="J95" t="n">
-        <v>41.05</v>
+        <v>40.79</v>
       </c>
       <c r="K95" t="inlineStr">
         <is>
@@ -4149,31 +4149,31 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>-1.32</v>
+        <v>0</v>
       </c>
       <c r="C96" t="n">
-        <v>-10.35</v>
+        <v>-2.68</v>
       </c>
       <c r="D96" t="n">
-        <v>-9.67</v>
+        <v>-6.5</v>
       </c>
       <c r="E96" t="n">
-        <v>12.89</v>
+        <v>12.49</v>
       </c>
       <c r="F96" t="n">
-        <v>-0.91</v>
+        <v>-0.39</v>
       </c>
       <c r="G96" t="n">
-        <v>-26.54</v>
+        <v>-24.54</v>
       </c>
       <c r="H96" t="n">
-        <v>-34.45</v>
+        <v>-34.15</v>
       </c>
       <c r="I96" t="n">
-        <v>-11.05</v>
+        <v>-10.09</v>
       </c>
       <c r="J96" t="n">
-        <v>28.98</v>
+        <v>29.23</v>
       </c>
       <c r="K96" t="inlineStr">
         <is>
@@ -4188,31 +4188,31 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>0.74</v>
+        <v>0</v>
       </c>
       <c r="C97" t="n">
-        <v>-0.72</v>
+        <v>-0.61</v>
       </c>
       <c r="D97" t="n">
-        <v>4.91</v>
+        <v>4.24</v>
       </c>
       <c r="E97" t="n">
-        <v>11.47</v>
+        <v>11.46</v>
       </c>
       <c r="F97" t="n">
-        <v>16.19</v>
+        <v>16.54</v>
       </c>
       <c r="G97" t="n">
-        <v>15.43</v>
+        <v>14.09</v>
       </c>
       <c r="H97" t="n">
-        <v>21.86</v>
+        <v>21.69</v>
       </c>
       <c r="I97" t="n">
-        <v>69.55</v>
+        <v>69.03</v>
       </c>
       <c r="J97" t="n">
-        <v>150.42</v>
+        <v>147.32</v>
       </c>
       <c r="K97" t="inlineStr">
         <is>
@@ -4227,31 +4227,31 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>-0.31</v>
+        <v>0</v>
       </c>
       <c r="C98" t="n">
-        <v>0.16</v>
+        <v>1.32</v>
       </c>
       <c r="D98" t="n">
-        <v>1.81</v>
+        <v>3.14</v>
       </c>
       <c r="E98" t="n">
-        <v>13.45</v>
+        <v>13.31</v>
       </c>
       <c r="F98" t="n">
-        <v>8.84</v>
+        <v>10.2</v>
       </c>
       <c r="G98" t="n">
-        <v>12.77</v>
+        <v>14.16</v>
       </c>
       <c r="H98" t="n">
-        <v>7.83</v>
+        <v>10.13</v>
       </c>
       <c r="I98" t="n">
-        <v>53.27</v>
+        <v>52.16</v>
       </c>
       <c r="J98" t="n">
-        <v>150.06</v>
+        <v>150.63</v>
       </c>
       <c r="K98" t="inlineStr">
         <is>
@@ -4269,28 +4269,28 @@
         <v>0</v>
       </c>
       <c r="C99" t="n">
-        <v>-0.96</v>
+        <v>3.27</v>
       </c>
       <c r="D99" t="n">
-        <v>5.24</v>
+        <v>8.09</v>
       </c>
       <c r="E99" t="n">
-        <v>13.79</v>
+        <v>14.44</v>
       </c>
       <c r="F99" t="n">
-        <v>11.25</v>
+        <v>13.89</v>
       </c>
       <c r="G99" t="n">
-        <v>28.66</v>
+        <v>33.22</v>
       </c>
       <c r="H99" t="n">
-        <v>10.7</v>
+        <v>14.97</v>
       </c>
       <c r="I99" t="n">
-        <v>104.85</v>
+        <v>105.39</v>
       </c>
       <c r="J99" t="n">
-        <v>223.82</v>
+        <v>228.1</v>
       </c>
       <c r="K99" t="inlineStr">
         <is>
@@ -4305,31 +4305,31 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>-0.04</v>
+        <v>0</v>
       </c>
       <c r="C100" t="n">
-        <v>-0.53</v>
+        <v>2.29</v>
       </c>
       <c r="D100" t="n">
-        <v>3.23</v>
+        <v>5.4</v>
       </c>
       <c r="E100" t="n">
-        <v>13.97</v>
+        <v>13.84</v>
       </c>
       <c r="F100" t="n">
-        <v>8.539999999999999</v>
+        <v>10.51</v>
       </c>
       <c r="G100" t="n">
-        <v>16.72</v>
+        <v>20.04</v>
       </c>
       <c r="H100" t="n">
-        <v>6.3</v>
+        <v>9.31</v>
       </c>
       <c r="I100" t="n">
-        <v>79.03</v>
+        <v>78.77</v>
       </c>
       <c r="J100" t="n">
-        <v>175.89</v>
+        <v>177.01</v>
       </c>
       <c r="K100" t="inlineStr">
         <is>
@@ -4344,31 +4344,31 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>-1.37</v>
+        <v>0</v>
       </c>
       <c r="C101" t="n">
-        <v>-3.33</v>
+        <v>0.79</v>
       </c>
       <c r="D101" t="n">
-        <v>-3.38</v>
+        <v>0.6</v>
       </c>
       <c r="E101" t="n">
-        <v>13.48</v>
+        <v>12.83</v>
       </c>
       <c r="F101" t="n">
-        <v>-1.2</v>
+        <v>0.12</v>
       </c>
       <c r="G101" t="n">
-        <v>-2.8</v>
+        <v>0.14</v>
       </c>
       <c r="H101" t="n">
-        <v>-4.26</v>
+        <v>-2</v>
       </c>
       <c r="I101" t="n">
-        <v>29.22</v>
+        <v>28.65</v>
       </c>
       <c r="J101" t="n">
-        <v>77.42</v>
+        <v>78.93000000000001</v>
       </c>
       <c r="K101" t="inlineStr">
         <is>
@@ -4383,31 +4383,31 @@
         </is>
       </c>
       <c r="B102" t="n">
+        <v>0</v>
+      </c>
+      <c r="C102" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="D102" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E102" t="n">
+        <v>14.96</v>
+      </c>
+      <c r="F102" t="n">
         <v>-0.9399999999999999</v>
       </c>
-      <c r="C102" t="n">
-        <v>-3.19</v>
-      </c>
-      <c r="D102" t="n">
-        <v>-3.08</v>
-      </c>
-      <c r="E102" t="n">
-        <v>17.07</v>
-      </c>
-      <c r="F102" t="n">
-        <v>-1.23</v>
-      </c>
       <c r="G102" t="n">
-        <v>-8.300000000000001</v>
+        <v>-7.2</v>
       </c>
       <c r="H102" t="n">
-        <v>-11.05</v>
+        <v>-10.15</v>
       </c>
       <c r="I102" t="n">
-        <v>22.6</v>
+        <v>21.03</v>
       </c>
       <c r="J102" t="n">
-        <v>54.35</v>
+        <v>55.09</v>
       </c>
       <c r="K102" t="inlineStr">
         <is>
@@ -4422,31 +4422,31 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>0.34</v>
+        <v>0</v>
       </c>
       <c r="C103" t="n">
-        <v>-0.67</v>
+        <v>3.66</v>
       </c>
       <c r="D103" t="n">
-        <v>6.54</v>
+        <v>9.81</v>
       </c>
       <c r="E103" t="n">
-        <v>14.33</v>
+        <v>14.96</v>
       </c>
       <c r="F103" t="n">
-        <v>10.5</v>
+        <v>13.51</v>
       </c>
       <c r="G103" t="n">
-        <v>24.56</v>
+        <v>28.27</v>
       </c>
       <c r="H103" t="n">
-        <v>0.89</v>
+        <v>5.22</v>
       </c>
       <c r="I103" t="n">
-        <v>95.33</v>
+        <v>96.04000000000001</v>
       </c>
       <c r="J103" t="n">
-        <v>237.3</v>
+        <v>239.56</v>
       </c>
       <c r="K103" t="inlineStr">
         <is>
@@ -4461,28 +4461,28 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>-0.98</v>
+        <v>0</v>
       </c>
       <c r="C104" t="n">
-        <v>-1.81</v>
+        <v>0.03</v>
       </c>
       <c r="D104" t="n">
-        <v>-3.1</v>
+        <v>-2.28</v>
       </c>
       <c r="E104" t="n">
-        <v>10.84</v>
+        <v>10.17</v>
       </c>
       <c r="F104" t="n">
-        <v>0.29</v>
+        <v>1.53</v>
       </c>
       <c r="G104" t="n">
-        <v>-10.77</v>
+        <v>-8.449999999999999</v>
       </c>
       <c r="H104" t="n">
-        <v>-11.41</v>
+        <v>-10.24</v>
       </c>
       <c r="I104" t="n">
-        <v>4.51</v>
+        <v>4.1</v>
       </c>
       <c r="J104" t="inlineStr"/>
       <c r="K104" t="inlineStr">
@@ -4498,31 +4498,31 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>-0.38</v>
+        <v>0</v>
       </c>
       <c r="C105" t="n">
-        <v>-0.09</v>
+        <v>0.73</v>
       </c>
       <c r="D105" t="n">
-        <v>0.17</v>
+        <v>0.99</v>
       </c>
       <c r="E105" t="n">
-        <v>12.9</v>
+        <v>11.8</v>
       </c>
       <c r="F105" t="n">
-        <v>6.7</v>
+        <v>7.46</v>
       </c>
       <c r="G105" t="n">
-        <v>9.91</v>
+        <v>12.41</v>
       </c>
       <c r="H105" t="n">
-        <v>12.33</v>
+        <v>13.88</v>
       </c>
       <c r="I105" t="n">
-        <v>59.19</v>
+        <v>58.16</v>
       </c>
       <c r="J105" t="n">
-        <v>116.41</v>
+        <v>115.71</v>
       </c>
       <c r="K105" t="inlineStr">
         <is>
@@ -4537,31 +4537,31 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>-0.49</v>
+        <v>0</v>
       </c>
       <c r="C106" t="n">
-        <v>-0.2</v>
+        <v>0.49</v>
       </c>
       <c r="D106" t="n">
-        <v>-1.01</v>
+        <v>0.03</v>
       </c>
       <c r="E106" t="n">
-        <v>8.58</v>
+        <v>7.83</v>
       </c>
       <c r="F106" t="n">
-        <v>-1.44</v>
+        <v>-0.22</v>
       </c>
       <c r="G106" t="n">
-        <v>-6.03</v>
+        <v>-4.6</v>
       </c>
       <c r="H106" t="n">
-        <v>-2.52</v>
+        <v>-0.92</v>
       </c>
       <c r="I106" t="n">
-        <v>30.43</v>
+        <v>29.06</v>
       </c>
       <c r="J106" t="n">
-        <v>81.14</v>
+        <v>80.44</v>
       </c>
       <c r="K106" t="inlineStr">
         <is>
@@ -4576,31 +4576,31 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>-0.35</v>
+        <v>0</v>
       </c>
       <c r="C107" t="n">
-        <v>-0.17</v>
+        <v>1.08</v>
       </c>
       <c r="D107" t="n">
-        <v>2.12</v>
+        <v>3.5</v>
       </c>
       <c r="E107" t="n">
-        <v>10.91</v>
+        <v>10.43</v>
       </c>
       <c r="F107" t="n">
-        <v>5.3</v>
+        <v>6.92</v>
       </c>
       <c r="G107" t="n">
-        <v>9.69</v>
+        <v>11.48</v>
       </c>
       <c r="H107" t="n">
-        <v>5.09</v>
+        <v>7.4</v>
       </c>
       <c r="I107" t="n">
-        <v>67.13</v>
+        <v>65.84999999999999</v>
       </c>
       <c r="J107" t="n">
-        <v>148.75</v>
+        <v>148.41</v>
       </c>
       <c r="K107" t="inlineStr">
         <is>
@@ -4615,31 +4615,31 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>-0.62</v>
+        <v>0</v>
       </c>
       <c r="C108" t="n">
-        <v>-0.59</v>
+        <v>-0.25</v>
       </c>
       <c r="D108" t="n">
-        <v>2.44</v>
+        <v>2.76</v>
       </c>
       <c r="E108" t="n">
-        <v>8.1</v>
+        <v>7.24</v>
       </c>
       <c r="F108" t="n">
-        <v>3.81</v>
+        <v>4.2</v>
       </c>
       <c r="G108" t="n">
-        <v>-5.62</v>
+        <v>-3.59</v>
       </c>
       <c r="H108" t="n">
-        <v>-14.52</v>
+        <v>-13</v>
       </c>
       <c r="I108" t="n">
-        <v>-10.99</v>
+        <v>-10.82</v>
       </c>
       <c r="J108" t="n">
-        <v>-15.25</v>
+        <v>-15.26</v>
       </c>
       <c r="K108" t="inlineStr">
         <is>
@@ -4654,31 +4654,31 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>0.26</v>
+        <v>0</v>
       </c>
       <c r="C109" t="n">
-        <v>-0.02</v>
+        <v>2.52</v>
       </c>
       <c r="D109" t="n">
-        <v>4.53</v>
+        <v>6.6</v>
       </c>
       <c r="E109" t="n">
-        <v>14.09</v>
+        <v>13.91</v>
       </c>
       <c r="F109" t="n">
-        <v>10.82</v>
+        <v>12.83</v>
       </c>
       <c r="G109" t="n">
-        <v>20.99</v>
+        <v>24.79</v>
       </c>
       <c r="H109" t="n">
-        <v>10.59</v>
+        <v>15.68</v>
       </c>
       <c r="I109" t="n">
-        <v>82.95</v>
+        <v>82.47</v>
       </c>
       <c r="J109" t="n">
-        <v>188.75</v>
+        <v>190.37</v>
       </c>
       <c r="K109" t="inlineStr">
         <is>
@@ -4693,31 +4693,31 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>1.19</v>
+        <v>0</v>
       </c>
       <c r="C110" t="n">
-        <v>0.85</v>
+        <v>4.37</v>
       </c>
       <c r="D110" t="n">
-        <v>10.69</v>
+        <v>13.27</v>
       </c>
       <c r="E110" t="n">
-        <v>19.95</v>
+        <v>19.65</v>
       </c>
       <c r="F110" t="n">
-        <v>18.12</v>
+        <v>19.9</v>
       </c>
       <c r="G110" t="n">
-        <v>20.69</v>
+        <v>22.32</v>
       </c>
       <c r="H110" t="n">
-        <v>1.11</v>
+        <v>3.64</v>
       </c>
       <c r="I110" t="n">
-        <v>59.49</v>
+        <v>61.17</v>
       </c>
       <c r="J110" t="n">
-        <v>198.74</v>
+        <v>200.68</v>
       </c>
       <c r="K110" t="inlineStr">
         <is>
@@ -4732,28 +4732,28 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="C111" t="n">
-        <v>-0.33</v>
+        <v>2.31</v>
       </c>
       <c r="D111" t="n">
-        <v>3.47</v>
+        <v>5.55</v>
       </c>
       <c r="E111" t="n">
-        <v>14.18</v>
+        <v>13.9</v>
       </c>
       <c r="F111" t="n">
-        <v>8.779999999999999</v>
+        <v>10.48</v>
       </c>
       <c r="G111" t="n">
-        <v>16.39</v>
+        <v>19.58</v>
       </c>
       <c r="H111" t="n">
-        <v>4.89</v>
+        <v>7.84</v>
       </c>
       <c r="I111" t="n">
-        <v>82.13</v>
+        <v>81.48999999999999</v>
       </c>
       <c r="J111" t="inlineStr"/>
       <c r="K111" t="inlineStr">
@@ -4769,25 +4769,25 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>-0.34</v>
+        <v>0</v>
       </c>
       <c r="C112" t="n">
-        <v>-0.79</v>
+        <v>2.23</v>
       </c>
       <c r="D112" t="n">
-        <v>3.86</v>
+        <v>6.04</v>
       </c>
       <c r="E112" t="n">
-        <v>14.98</v>
+        <v>14.44</v>
       </c>
       <c r="F112" t="n">
-        <v>10.81</v>
+        <v>12.44</v>
       </c>
       <c r="G112" t="n">
-        <v>20.21</v>
+        <v>23.52</v>
       </c>
       <c r="H112" t="n">
-        <v>8.210000000000001</v>
+        <v>11.38</v>
       </c>
       <c r="I112" t="inlineStr"/>
       <c r="J112" t="inlineStr"/>
@@ -4804,28 +4804,28 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>-1.05</v>
+        <v>0</v>
       </c>
       <c r="C113" t="n">
-        <v>-2.62</v>
+        <v>1.03</v>
       </c>
       <c r="D113" t="n">
-        <v>-2.56</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E113" t="n">
-        <v>13.73</v>
+        <v>13.32</v>
       </c>
       <c r="F113" t="n">
-        <v>0.38</v>
+        <v>1.61</v>
       </c>
       <c r="G113" t="n">
-        <v>-1.73</v>
+        <v>1.12</v>
       </c>
       <c r="H113" t="n">
-        <v>-1.58</v>
+        <v>0.54</v>
       </c>
       <c r="I113" t="n">
-        <v>44.39</v>
+        <v>43.85</v>
       </c>
       <c r="J113" t="inlineStr"/>
       <c r="K113" t="inlineStr">
@@ -4841,31 +4841,31 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>-0.58</v>
+        <v>0</v>
       </c>
       <c r="C114" t="n">
-        <v>-2.1</v>
+        <v>1.79</v>
       </c>
       <c r="D114" t="n">
-        <v>-0.33</v>
+        <v>3.45</v>
       </c>
       <c r="E114" t="n">
-        <v>22.15</v>
+        <v>21.36</v>
       </c>
       <c r="F114" t="n">
-        <v>4.15</v>
+        <v>6.72</v>
       </c>
       <c r="G114" t="n">
-        <v>5.16</v>
+        <v>10.09</v>
       </c>
       <c r="H114" t="n">
-        <v>6.45</v>
+        <v>9.66</v>
       </c>
       <c r="I114" t="n">
-        <v>101.8</v>
+        <v>102.52</v>
       </c>
       <c r="J114" t="n">
-        <v>182.56</v>
+        <v>183.6</v>
       </c>
       <c r="K114" t="inlineStr">
         <is>
@@ -4880,31 +4880,31 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>-0.04</v>
+        <v>0</v>
       </c>
       <c r="C115" t="n">
-        <v>3.77</v>
+        <v>0.38</v>
       </c>
       <c r="D115" t="n">
-        <v>6.96</v>
+        <v>4.01</v>
       </c>
       <c r="E115" t="n">
-        <v>-11.62</v>
+        <v>-12.03</v>
       </c>
       <c r="F115" t="n">
-        <v>-0.42</v>
+        <v>-0.91</v>
       </c>
       <c r="G115" t="n">
-        <v>-2.88</v>
+        <v>-5.39</v>
       </c>
       <c r="H115" t="n">
-        <v>-0.42</v>
+        <v>-0.59</v>
       </c>
       <c r="I115" t="n">
-        <v>-12.79</v>
+        <v>-13.24</v>
       </c>
       <c r="J115" t="n">
-        <v>-3.19</v>
+        <v>-3.46</v>
       </c>
       <c r="K115" t="inlineStr">
         <is>
@@ -4919,31 +4919,31 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>-0.2</v>
+        <v>0</v>
       </c>
       <c r="C116" t="n">
-        <v>0.87</v>
+        <v>0.54</v>
       </c>
       <c r="D116" t="n">
         <v>0.87</v>
       </c>
       <c r="E116" t="n">
-        <v>7.07</v>
+        <v>6</v>
       </c>
       <c r="F116" t="n">
-        <v>1.01</v>
+        <v>2.24</v>
       </c>
       <c r="G116" t="n">
-        <v>0.08</v>
+        <v>0.05</v>
       </c>
       <c r="H116" t="n">
-        <v>-3.06</v>
+        <v>-2.13</v>
       </c>
       <c r="I116" t="n">
-        <v>28.26</v>
+        <v>26.72</v>
       </c>
       <c r="J116" t="n">
-        <v>101.77</v>
+        <v>100.51</v>
       </c>
       <c r="K116" t="inlineStr">
         <is>
@@ -4958,25 +4958,25 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>-0.61</v>
+        <v>0</v>
       </c>
       <c r="C117" t="n">
-        <v>3.22</v>
+        <v>2.57</v>
       </c>
       <c r="D117" t="n">
-        <v>-1.73</v>
+        <v>0.27</v>
       </c>
       <c r="E117" t="n">
-        <v>5.36</v>
+        <v>5.83</v>
       </c>
       <c r="F117" t="n">
-        <v>-3.78</v>
+        <v>-1.92</v>
       </c>
       <c r="G117" t="n">
-        <v>-4.35</v>
+        <v>-5.37</v>
       </c>
       <c r="H117" t="n">
-        <v>-42.47</v>
+        <v>-41.63</v>
       </c>
       <c r="I117" t="inlineStr"/>
       <c r="J117" t="inlineStr"/>
@@ -4993,25 +4993,25 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>-0.43</v>
+        <v>0</v>
       </c>
       <c r="C118" t="n">
-        <v>-0.53</v>
+        <v>0.2</v>
       </c>
       <c r="D118" t="n">
-        <v>-2.88</v>
+        <v>-2.27</v>
       </c>
       <c r="E118" t="n">
-        <v>0.26</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="F118" t="n">
-        <v>-3.72</v>
+        <v>-5.86</v>
       </c>
       <c r="G118" t="n">
-        <v>-6.91</v>
+        <v>-5.63</v>
       </c>
       <c r="H118" t="n">
-        <v>-2.7</v>
+        <v>-2.42</v>
       </c>
       <c r="I118" t="inlineStr"/>
       <c r="J118" t="inlineStr"/>
@@ -5028,31 +5028,31 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>-0.97</v>
+        <v>0</v>
       </c>
       <c r="C119" t="n">
-        <v>-0.51</v>
+        <v>-0.39</v>
       </c>
       <c r="D119" t="n">
-        <v>-0.78</v>
+        <v>0.54</v>
       </c>
       <c r="E119" t="n">
-        <v>5.78</v>
+        <v>5.81</v>
       </c>
       <c r="F119" t="n">
-        <v>1.92</v>
+        <v>1.62</v>
       </c>
       <c r="G119" t="n">
-        <v>-2.3</v>
+        <v>0.65</v>
       </c>
       <c r="H119" t="n">
-        <v>-17.27</v>
+        <v>-16.01</v>
       </c>
       <c r="I119" t="n">
-        <v>-19.43</v>
+        <v>-19.55</v>
       </c>
       <c r="J119" t="n">
-        <v>-18</v>
+        <v>-18.64</v>
       </c>
       <c r="K119" t="inlineStr">
         <is>
@@ -5070,28 +5070,28 @@
         <v>0</v>
       </c>
       <c r="C120" t="n">
-        <v>0.64</v>
+        <v>-0.19</v>
       </c>
       <c r="D120" t="n">
-        <v>-0.82</v>
+        <v>-1.18</v>
       </c>
       <c r="E120" t="n">
-        <v>3.48</v>
+        <v>1.55</v>
       </c>
       <c r="F120" t="n">
-        <v>-2.61</v>
+        <v>-3.07</v>
       </c>
       <c r="G120" t="n">
-        <v>-0.63</v>
+        <v>1.47</v>
       </c>
       <c r="H120" t="n">
-        <v>-8.859999999999999</v>
+        <v>-9.529999999999999</v>
       </c>
       <c r="I120" t="n">
-        <v>-20.22</v>
+        <v>-20.75</v>
       </c>
       <c r="J120" t="n">
-        <v>-22.73</v>
+        <v>-23.95</v>
       </c>
       <c r="K120" t="inlineStr">
         <is>
@@ -5106,31 +5106,31 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>-0.93</v>
+        <v>0</v>
       </c>
       <c r="C121" t="n">
-        <v>0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="D121" t="n">
-        <v>-0.28</v>
+        <v>0.88</v>
       </c>
       <c r="E121" t="n">
-        <v>8.08</v>
+        <v>8.140000000000001</v>
       </c>
       <c r="F121" t="n">
-        <v>3.63</v>
+        <v>3.51</v>
       </c>
       <c r="G121" t="n">
-        <v>-1.98</v>
+        <v>-0.06</v>
       </c>
       <c r="H121" t="n">
-        <v>-14.2</v>
+        <v>-12.62</v>
       </c>
       <c r="I121" t="n">
-        <v>-5.51</v>
+        <v>-5.74</v>
       </c>
       <c r="J121" t="n">
-        <v>-6.12</v>
+        <v>-5.34</v>
       </c>
       <c r="K121" t="inlineStr">
         <is>
@@ -5148,25 +5148,25 @@
         <v>0</v>
       </c>
       <c r="C122" t="n">
-        <v>-0.19</v>
+        <v>-0.5600000000000001</v>
       </c>
       <c r="D122" t="n">
-        <v>1.25</v>
+        <v>0.74</v>
       </c>
       <c r="E122" t="n">
-        <v>2.19</v>
+        <v>2.16</v>
       </c>
       <c r="F122" t="n">
-        <v>1.46</v>
+        <v>0.66</v>
       </c>
       <c r="G122" t="n">
-        <v>1.04</v>
+        <v>0.57</v>
       </c>
       <c r="H122" t="n">
-        <v>-0.41</v>
+        <v>-0.43</v>
       </c>
       <c r="I122" t="n">
-        <v>0.28</v>
+        <v>-0.26</v>
       </c>
       <c r="J122" t="inlineStr"/>
       <c r="K122" t="inlineStr">
@@ -5182,31 +5182,31 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>-0.46</v>
+        <v>0</v>
       </c>
       <c r="C123" t="n">
-        <v>-0.8</v>
+        <v>-0.37</v>
       </c>
       <c r="D123" t="n">
-        <v>0.06</v>
+        <v>0.67</v>
       </c>
       <c r="E123" t="n">
-        <v>4.74</v>
+        <v>4.16</v>
       </c>
       <c r="F123" t="n">
-        <v>3.67</v>
+        <v>3.4</v>
       </c>
       <c r="G123" t="n">
-        <v>-0.03</v>
+        <v>1.7</v>
       </c>
       <c r="H123" t="n">
-        <v>-9.050000000000001</v>
+        <v>-7.85</v>
       </c>
       <c r="I123" t="n">
-        <v>-8.859999999999999</v>
+        <v>-9.380000000000001</v>
       </c>
       <c r="J123" t="n">
-        <v>-16.57</v>
+        <v>-16.66</v>
       </c>
       <c r="K123" t="inlineStr">
         <is>
@@ -5224,25 +5224,25 @@
         <v>0</v>
       </c>
       <c r="C124" t="n">
-        <v>-0.22</v>
+        <v>-0.31</v>
       </c>
       <c r="D124" t="n">
-        <v>0.9</v>
+        <v>0.51</v>
       </c>
       <c r="E124" t="n">
-        <v>2.54</v>
+        <v>1.6</v>
       </c>
       <c r="F124" t="n">
-        <v>1.89</v>
+        <v>1.35</v>
       </c>
       <c r="G124" t="n">
-        <v>0.53</v>
+        <v>0.43</v>
       </c>
       <c r="H124" t="n">
-        <v>-2.23</v>
+        <v>-2.17</v>
       </c>
       <c r="I124" t="n">
-        <v>-4.61</v>
+        <v>-5.34</v>
       </c>
       <c r="J124" t="inlineStr"/>
       <c r="K124" t="inlineStr">

</xml_diff>